<commit_message>
Uploaded 04-May-2021 13:56:30 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="111">
   <si>
     <t>RuleSet</t>
   </si>
@@ -534,9 +534,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -551,6 +548,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -946,27 +946,27 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -1002,18 +1002,10 @@
       <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="L4" s="3"/>
     </row>
@@ -1073,13 +1065,13 @@
       <c r="C7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="20" t="s">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21">
+      <c r="G7" s="19"/>
+      <c r="H7" s="20">
         <v>0.5</v>
       </c>
     </row>
@@ -1091,13 +1083,13 @@
       <c r="C8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="20" t="s">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21">
+      <c r="G8" s="19"/>
+      <c r="H8" s="20">
         <v>0.6</v>
       </c>
     </row>
@@ -1109,13 +1101,13 @@
       <c r="C9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="20" t="s">
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21">
+      <c r="G9" s="19"/>
+      <c r="H9" s="20">
         <v>0.65</v>
       </c>
     </row>
@@ -1127,13 +1119,13 @@
       <c r="C10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="21">
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20">
         <v>0.7</v>
       </c>
     </row>
@@ -1145,13 +1137,13 @@
       <c r="C11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="20" t="s">
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21">
+      <c r="G11" s="19"/>
+      <c r="H11" s="20">
         <v>0.72</v>
       </c>
     </row>
@@ -1163,13 +1155,13 @@
       <c r="C12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="20" t="s">
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="21">
+      <c r="G12" s="19"/>
+      <c r="H12" s="20">
         <v>0.75</v>
       </c>
     </row>
@@ -1181,13 +1173,13 @@
       <c r="C13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="20" t="s">
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21">
+      <c r="G13" s="19"/>
+      <c r="H13" s="20">
         <v>0.86</v>
       </c>
     </row>
@@ -1199,13 +1191,13 @@
       <c r="C14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="20" t="s">
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21">
+      <c r="G14" s="19"/>
+      <c r="H14" s="20">
         <v>0.89</v>
       </c>
     </row>
@@ -1217,13 +1209,13 @@
       <c r="C15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="20" t="s">
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="21">
+      <c r="G15" s="19"/>
+      <c r="H15" s="20">
         <v>0.89900000000000002</v>
       </c>
     </row>
@@ -1235,13 +1227,13 @@
       <c r="C16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="20" t="s">
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21">
+      <c r="G16" s="19"/>
+      <c r="H16" s="20">
         <v>0.9</v>
       </c>
     </row>
@@ -1253,13 +1245,13 @@
       <c r="C17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="20" t="s">
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="21">
+      <c r="G17" s="19"/>
+      <c r="H17" s="20">
         <v>0.91</v>
       </c>
     </row>
@@ -1271,13 +1263,13 @@
       <c r="C18" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="20" t="s">
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="21">
+      <c r="G18" s="19"/>
+      <c r="H18" s="20">
         <v>0.99099999999999999</v>
       </c>
     </row>
@@ -1289,13 +1281,13 @@
       <c r="C19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="20" t="s">
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="21">
+      <c r="G19" s="19"/>
+      <c r="H19" s="20">
         <v>0.995</v>
       </c>
     </row>
@@ -1307,13 +1299,13 @@
       <c r="C20" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="20" t="s">
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="21">
+      <c r="G20" s="19"/>
+      <c r="H20" s="20">
         <v>0.996</v>
       </c>
     </row>
@@ -1325,13 +1317,13 @@
       <c r="C21" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="20" t="s">
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21">
+      <c r="G21" s="19"/>
+      <c r="H21" s="20">
         <v>0.997</v>
       </c>
     </row>
@@ -1343,13 +1335,13 @@
       <c r="C22" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="20" t="s">
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="21">
+      <c r="G22" s="19"/>
+      <c r="H22" s="20">
         <v>0.998</v>
       </c>
     </row>
@@ -1361,13 +1353,13 @@
       <c r="C23" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="20" t="s">
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21">
+      <c r="G23" s="19"/>
+      <c r="H23" s="20">
         <v>0.999</v>
       </c>
     </row>
@@ -1379,13 +1371,13 @@
       <c r="C24" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="20" t="s">
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21">
+      <c r="G24" s="19"/>
+      <c r="H24" s="20">
         <v>1</v>
       </c>
     </row>
@@ -1397,13 +1389,13 @@
       <c r="C25" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="20" t="s">
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="21">
+      <c r="G25" s="19"/>
+      <c r="H25" s="20">
         <v>0.4</v>
       </c>
     </row>
@@ -1415,13 +1407,13 @@
       <c r="C26" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="20" t="s">
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="21">
+      <c r="G26" s="19"/>
+      <c r="H26" s="20">
         <v>0.5</v>
       </c>
     </row>
@@ -1433,13 +1425,13 @@
       <c r="C27" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="20" t="s">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="21">
+      <c r="G27" s="19"/>
+      <c r="H27" s="20">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -1451,13 +1443,13 @@
       <c r="C28" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="20"/>
-      <c r="H28" s="21">
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20">
         <v>0.6</v>
       </c>
     </row>
@@ -1469,13 +1461,13 @@
       <c r="C29" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="20" t="s">
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="20"/>
-      <c r="H29" s="21">
+      <c r="G29" s="19"/>
+      <c r="H29" s="20">
         <v>0.62</v>
       </c>
     </row>
@@ -1487,13 +1479,13 @@
       <c r="C30" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="20" t="s">
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="21">
+      <c r="G30" s="19"/>
+      <c r="H30" s="20">
         <v>0.65</v>
       </c>
     </row>
@@ -1505,13 +1497,13 @@
       <c r="C31" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="20" t="s">
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="20"/>
-      <c r="H31" s="21">
+      <c r="G31" s="19"/>
+      <c r="H31" s="20">
         <v>0.7</v>
       </c>
     </row>
@@ -1523,13 +1515,13 @@
       <c r="C32" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="20" t="s">
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G32" s="20"/>
-      <c r="H32" s="21">
+      <c r="G32" s="19"/>
+      <c r="H32" s="20">
         <v>0.88</v>
       </c>
     </row>
@@ -1541,13 +1533,13 @@
       <c r="C33" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="20" t="s">
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G33" s="20"/>
-      <c r="H33" s="21">
+      <c r="G33" s="19"/>
+      <c r="H33" s="20">
         <v>0.9</v>
       </c>
     </row>
@@ -1559,13 +1551,13 @@
       <c r="C34" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="20" t="s">
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G34" s="20"/>
-      <c r="H34" s="21">
+      <c r="G34" s="19"/>
+      <c r="H34" s="20">
         <v>0.995</v>
       </c>
     </row>
@@ -1577,13 +1569,13 @@
       <c r="C35" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="20" t="s">
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="20"/>
-      <c r="H35" s="21">
+      <c r="G35" s="19"/>
+      <c r="H35" s="20">
         <v>0.99550000000000005</v>
       </c>
     </row>
@@ -1595,13 +1587,13 @@
       <c r="C36" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="20" t="s">
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G36" s="20"/>
-      <c r="H36" s="21">
+      <c r="G36" s="19"/>
+      <c r="H36" s="20">
         <v>0.996</v>
       </c>
     </row>
@@ -1613,13 +1605,13 @@
       <c r="C37" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="20" t="s">
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G37" s="20"/>
-      <c r="H37" s="21">
+      <c r="G37" s="19"/>
+      <c r="H37" s="20">
         <v>0.99650000000000005</v>
       </c>
     </row>
@@ -1631,13 +1623,13 @@
       <c r="C38" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="20" t="s">
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G38" s="20"/>
-      <c r="H38" s="21">
+      <c r="G38" s="19"/>
+      <c r="H38" s="20">
         <v>0.997</v>
       </c>
     </row>
@@ -1649,13 +1641,13 @@
       <c r="C39" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="20" t="s">
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G39" s="20"/>
-      <c r="H39" s="21">
+      <c r="G39" s="19"/>
+      <c r="H39" s="20">
         <v>0.99750000000000005</v>
       </c>
     </row>
@@ -1667,13 +1659,13 @@
       <c r="C40" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="20" t="s">
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G40" s="20"/>
-      <c r="H40" s="21">
+      <c r="G40" s="19"/>
+      <c r="H40" s="20">
         <v>0.998</v>
       </c>
     </row>
@@ -1685,13 +1677,13 @@
       <c r="C41" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="20" t="s">
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="20"/>
-      <c r="H41" s="21">
+      <c r="G41" s="19"/>
+      <c r="H41" s="20">
         <v>0.999</v>
       </c>
     </row>
@@ -1703,13 +1695,13 @@
       <c r="C42" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="20" t="s">
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="21">
+      <c r="G42" s="19"/>
+      <c r="H42" s="20">
         <v>1</v>
       </c>
     </row>
@@ -1721,13 +1713,13 @@
       <c r="C43" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="20" t="s">
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="20"/>
-      <c r="H43" s="21">
+      <c r="G43" s="19"/>
+      <c r="H43" s="20">
         <v>0.1</v>
       </c>
     </row>
@@ -1739,13 +1731,13 @@
       <c r="C44" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="20" t="s">
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G44" s="20"/>
-      <c r="H44" s="21">
+      <c r="G44" s="19"/>
+      <c r="H44" s="20">
         <v>0.25</v>
       </c>
     </row>
@@ -1757,13 +1749,13 @@
       <c r="C45" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="20" t="s">
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="20"/>
-      <c r="H45" s="21">
+      <c r="G45" s="19"/>
+      <c r="H45" s="20">
         <v>0.3</v>
       </c>
     </row>
@@ -1775,13 +1767,13 @@
       <c r="C46" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G46" s="20"/>
-      <c r="H46" s="21">
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" s="19"/>
+      <c r="H46" s="20">
         <v>0.4</v>
       </c>
     </row>
@@ -1793,13 +1785,13 @@
       <c r="C47" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="20" t="s">
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G47" s="20"/>
-      <c r="H47" s="21">
+      <c r="G47" s="19"/>
+      <c r="H47" s="20">
         <v>0.45</v>
       </c>
     </row>
@@ -1811,13 +1803,13 @@
       <c r="C48" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="20" t="s">
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G48" s="20"/>
-      <c r="H48" s="21">
+      <c r="G48" s="19"/>
+      <c r="H48" s="20">
         <v>0.5</v>
       </c>
     </row>
@@ -1829,13 +1821,13 @@
       <c r="C49" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="20" t="s">
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G49" s="20"/>
-      <c r="H49" s="21">
+      <c r="G49" s="19"/>
+      <c r="H49" s="20">
         <v>0.61</v>
       </c>
     </row>
@@ -1847,13 +1839,13 @@
       <c r="C50" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="20" t="s">
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G50" s="20"/>
-      <c r="H50" s="21">
+      <c r="G50" s="19"/>
+      <c r="H50" s="20">
         <v>0.65</v>
       </c>
     </row>
@@ -1865,13 +1857,13 @@
       <c r="C51" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="20" t="s">
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G51" s="20"/>
-      <c r="H51" s="21">
+      <c r="G51" s="19"/>
+      <c r="H51" s="20">
         <v>0.7</v>
       </c>
     </row>
@@ -1883,13 +1875,13 @@
       <c r="C52" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="20" t="s">
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G52" s="20"/>
-      <c r="H52" s="21">
+      <c r="G52" s="19"/>
+      <c r="H52" s="20">
         <v>0.8</v>
       </c>
     </row>
@@ -1901,13 +1893,13 @@
       <c r="C53" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="20" t="s">
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G53" s="20"/>
-      <c r="H53" s="21">
+      <c r="G53" s="19"/>
+      <c r="H53" s="20">
         <v>0.87</v>
       </c>
     </row>
@@ -1919,13 +1911,13 @@
       <c r="C54" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="20" t="s">
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G54" s="20"/>
-      <c r="H54" s="21">
+      <c r="G54" s="19"/>
+      <c r="H54" s="20">
         <v>0.88</v>
       </c>
     </row>
@@ -1937,13 +1929,13 @@
       <c r="C55" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="20" t="s">
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G55" s="20"/>
-      <c r="H55" s="21">
+      <c r="G55" s="19"/>
+      <c r="H55" s="20">
         <v>0.9</v>
       </c>
     </row>
@@ -1955,13 +1947,13 @@
       <c r="C56" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="22"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="20" t="s">
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G56" s="20"/>
-      <c r="H56" s="21">
+      <c r="G56" s="19"/>
+      <c r="H56" s="20">
         <v>0.996</v>
       </c>
     </row>
@@ -1973,13 +1965,13 @@
       <c r="C57" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="20" t="s">
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G57" s="20"/>
-      <c r="H57" s="21">
+      <c r="G57" s="19"/>
+      <c r="H57" s="20">
         <v>0.997</v>
       </c>
     </row>
@@ -1991,13 +1983,13 @@
       <c r="C58" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="20" t="s">
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G58" s="20"/>
-      <c r="H58" s="21">
+      <c r="G58" s="19"/>
+      <c r="H58" s="20">
         <v>0.998</v>
       </c>
     </row>
@@ -2009,13 +2001,13 @@
       <c r="C59" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="20" t="s">
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G59" s="20"/>
-      <c r="H59" s="21">
+      <c r="G59" s="19"/>
+      <c r="H59" s="20">
         <v>0.999</v>
       </c>
     </row>
@@ -2027,13 +2019,13 @@
       <c r="C60" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="20" t="s">
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G60" s="20"/>
-      <c r="H60" s="21">
+      <c r="G60" s="19"/>
+      <c r="H60" s="20">
         <v>1</v>
       </c>
     </row>
@@ -2045,13 +2037,13 @@
       <c r="C61" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="20" t="s">
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G61" s="20"/>
-      <c r="H61" s="21">
+      <c r="G61" s="19"/>
+      <c r="H61" s="20">
         <v>0.48</v>
       </c>
     </row>
@@ -2063,13 +2055,13 @@
       <c r="C62" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="22"/>
-      <c r="E62" s="22"/>
-      <c r="F62" s="20" t="s">
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G62" s="20"/>
-      <c r="H62" s="21">
+      <c r="G62" s="19"/>
+      <c r="H62" s="20">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -2081,13 +2073,13 @@
       <c r="C63" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D63" s="22"/>
-      <c r="E63" s="22"/>
-      <c r="F63" s="20" t="s">
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G63" s="20"/>
-      <c r="H63" s="21">
+      <c r="G63" s="19"/>
+      <c r="H63" s="20">
         <v>0.65</v>
       </c>
     </row>
@@ -2099,13 +2091,13 @@
       <c r="C64" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D64" s="22"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G64" s="20"/>
-      <c r="H64" s="21">
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G64" s="19"/>
+      <c r="H64" s="20">
         <v>0.77</v>
       </c>
     </row>
@@ -2117,13 +2109,13 @@
       <c r="C65" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D65" s="22"/>
-      <c r="E65" s="22"/>
-      <c r="F65" s="20" t="s">
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G65" s="20"/>
-      <c r="H65" s="21">
+      <c r="G65" s="19"/>
+      <c r="H65" s="20">
         <v>0.79</v>
       </c>
     </row>
@@ -2135,13 +2127,13 @@
       <c r="C66" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D66" s="22"/>
-      <c r="E66" s="22"/>
-      <c r="F66" s="20" t="s">
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G66" s="20"/>
-      <c r="H66" s="21">
+      <c r="G66" s="19"/>
+      <c r="H66" s="20">
         <v>0.8</v>
       </c>
     </row>
@@ -2153,13 +2145,13 @@
       <c r="C67" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D67" s="22"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="20" t="s">
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G67" s="20"/>
-      <c r="H67" s="21">
+      <c r="G67" s="19"/>
+      <c r="H67" s="20">
         <v>0.88</v>
       </c>
     </row>
@@ -2171,13 +2163,13 @@
       <c r="C68" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D68" s="22"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="20" t="s">
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G68" s="20"/>
-      <c r="H68" s="21">
+      <c r="G68" s="19"/>
+      <c r="H68" s="20">
         <v>0.99</v>
       </c>
     </row>
@@ -2189,13 +2181,13 @@
       <c r="C69" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D69" s="22"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="20" t="s">
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G69" s="20"/>
-      <c r="H69" s="21">
+      <c r="G69" s="19"/>
+      <c r="H69" s="20">
         <v>0.99099999999999999</v>
       </c>
     </row>
@@ -2207,13 +2199,13 @@
       <c r="C70" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D70" s="22"/>
-      <c r="E70" s="22"/>
-      <c r="F70" s="20" t="s">
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G70" s="20"/>
-      <c r="H70" s="21">
+      <c r="G70" s="19"/>
+      <c r="H70" s="20">
         <v>0.99199999999999999</v>
       </c>
     </row>
@@ -2225,13 +2217,13 @@
       <c r="C71" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D71" s="22"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="20" t="s">
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G71" s="20"/>
-      <c r="H71" s="21">
+      <c r="G71" s="19"/>
+      <c r="H71" s="20">
         <v>0.99299999999999999</v>
       </c>
     </row>
@@ -2243,13 +2235,13 @@
       <c r="C72" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="20" t="s">
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G72" s="20"/>
-      <c r="H72" s="21">
+      <c r="G72" s="19"/>
+      <c r="H72" s="20">
         <v>0.99399999999999999</v>
       </c>
     </row>
@@ -2261,13 +2253,13 @@
       <c r="C73" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D73" s="22"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="20" t="s">
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G73" s="20"/>
-      <c r="H73" s="21">
+      <c r="G73" s="19"/>
+      <c r="H73" s="20">
         <v>0.995</v>
       </c>
     </row>
@@ -2279,13 +2271,13 @@
       <c r="C74" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D74" s="22"/>
-      <c r="E74" s="22"/>
-      <c r="F74" s="20" t="s">
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G74" s="20"/>
-      <c r="H74" s="21">
+      <c r="G74" s="19"/>
+      <c r="H74" s="20">
         <v>0.996</v>
       </c>
     </row>
@@ -2297,13 +2289,13 @@
       <c r="C75" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D75" s="22"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="20" t="s">
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G75" s="20"/>
-      <c r="H75" s="21">
+      <c r="G75" s="19"/>
+      <c r="H75" s="20">
         <v>0.997</v>
       </c>
     </row>
@@ -2315,13 +2307,13 @@
       <c r="C76" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D76" s="22"/>
-      <c r="E76" s="22"/>
-      <c r="F76" s="20" t="s">
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G76" s="20"/>
-      <c r="H76" s="21">
+      <c r="G76" s="19"/>
+      <c r="H76" s="20">
         <v>0.998</v>
       </c>
     </row>
@@ -2333,13 +2325,13 @@
       <c r="C77" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D77" s="22"/>
-      <c r="E77" s="22"/>
-      <c r="F77" s="20" t="s">
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G77" s="20"/>
-      <c r="H77" s="21">
+      <c r="G77" s="19"/>
+      <c r="H77" s="20">
         <v>0.999</v>
       </c>
     </row>
@@ -2351,13 +2343,13 @@
       <c r="C78" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D78" s="22"/>
-      <c r="E78" s="22"/>
-      <c r="F78" s="20" t="s">
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G78" s="20"/>
-      <c r="H78" s="21">
+      <c r="G78" s="19"/>
+      <c r="H78" s="20">
         <v>1</v>
       </c>
     </row>
@@ -2369,13 +2361,13 @@
       <c r="C79" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D79" s="22"/>
-      <c r="E79" s="22"/>
-      <c r="F79" s="20" t="s">
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G79" s="20"/>
-      <c r="H79" s="21">
+      <c r="G79" s="19"/>
+      <c r="H79" s="20">
         <v>0.79</v>
       </c>
     </row>
@@ -2387,13 +2379,13 @@
       <c r="C80" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="20" t="s">
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G80" s="20"/>
-      <c r="H80" s="21">
+      <c r="G80" s="19"/>
+      <c r="H80" s="20">
         <v>0.82</v>
       </c>
     </row>
@@ -2405,13 +2397,13 @@
       <c r="C81" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D81" s="22"/>
-      <c r="E81" s="22"/>
-      <c r="F81" s="20" t="s">
+      <c r="D81" s="21"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G81" s="20"/>
-      <c r="H81" s="21">
+      <c r="G81" s="19"/>
+      <c r="H81" s="20">
         <v>0.85</v>
       </c>
     </row>
@@ -2423,13 +2415,13 @@
       <c r="C82" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D82" s="22"/>
-      <c r="E82" s="22"/>
-      <c r="F82" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G82" s="20"/>
-      <c r="H82" s="21">
+      <c r="D82" s="21"/>
+      <c r="E82" s="21"/>
+      <c r="F82" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G82" s="19"/>
+      <c r="H82" s="20">
         <v>0.9</v>
       </c>
     </row>
@@ -2441,13 +2433,13 @@
       <c r="C83" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D83" s="22"/>
-      <c r="E83" s="22"/>
-      <c r="F83" s="20" t="s">
+      <c r="D83" s="21"/>
+      <c r="E83" s="21"/>
+      <c r="F83" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G83" s="20"/>
-      <c r="H83" s="21">
+      <c r="G83" s="19"/>
+      <c r="H83" s="20">
         <v>0.98499999999999999</v>
       </c>
     </row>
@@ -2459,13 +2451,13 @@
       <c r="C84" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D84" s="22"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="20" t="s">
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G84" s="20"/>
-      <c r="H84" s="21">
+      <c r="G84" s="19"/>
+      <c r="H84" s="20">
         <v>0.98799999999999999</v>
       </c>
     </row>
@@ -2477,13 +2469,13 @@
       <c r="C85" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="20" t="s">
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G85" s="20"/>
-      <c r="H85" s="21">
+      <c r="G85" s="19"/>
+      <c r="H85" s="20">
         <v>0.98899999999999999</v>
       </c>
     </row>
@@ -2495,13 +2487,13 @@
       <c r="C86" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D86" s="22"/>
-      <c r="E86" s="22"/>
-      <c r="F86" s="20" t="s">
+      <c r="D86" s="21"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G86" s="20"/>
-      <c r="H86" s="21">
+      <c r="G86" s="19"/>
+      <c r="H86" s="20">
         <v>0.99</v>
       </c>
     </row>
@@ -2513,13 +2505,13 @@
       <c r="C87" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D87" s="22"/>
-      <c r="E87" s="22"/>
-      <c r="F87" s="20" t="s">
+      <c r="D87" s="21"/>
+      <c r="E87" s="21"/>
+      <c r="F87" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G87" s="20"/>
-      <c r="H87" s="21">
+      <c r="G87" s="19"/>
+      <c r="H87" s="20">
         <v>0.99099999999999999</v>
       </c>
     </row>
@@ -2531,13 +2523,13 @@
       <c r="C88" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D88" s="22"/>
-      <c r="E88" s="22"/>
-      <c r="F88" s="20" t="s">
+      <c r="D88" s="21"/>
+      <c r="E88" s="21"/>
+      <c r="F88" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G88" s="20"/>
-      <c r="H88" s="21">
+      <c r="G88" s="19"/>
+      <c r="H88" s="20">
         <v>0.99199999999999999</v>
       </c>
     </row>
@@ -2549,13 +2541,13 @@
       <c r="C89" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D89" s="22"/>
-      <c r="E89" s="22"/>
-      <c r="F89" s="20" t="s">
+      <c r="D89" s="21"/>
+      <c r="E89" s="21"/>
+      <c r="F89" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G89" s="20"/>
-      <c r="H89" s="21">
+      <c r="G89" s="19"/>
+      <c r="H89" s="20">
         <v>0.99299999999999999</v>
       </c>
     </row>
@@ -2567,13 +2559,13 @@
       <c r="C90" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D90" s="22"/>
-      <c r="E90" s="22"/>
-      <c r="F90" s="20" t="s">
+      <c r="D90" s="21"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G90" s="20"/>
-      <c r="H90" s="21">
+      <c r="G90" s="19"/>
+      <c r="H90" s="20">
         <v>0.99399999999999999</v>
       </c>
     </row>
@@ -2585,13 +2577,13 @@
       <c r="C91" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D91" s="22"/>
-      <c r="E91" s="22"/>
-      <c r="F91" s="20" t="s">
+      <c r="D91" s="21"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G91" s="20"/>
-      <c r="H91" s="21">
+      <c r="G91" s="19"/>
+      <c r="H91" s="20">
         <v>0.995</v>
       </c>
     </row>
@@ -2603,13 +2595,13 @@
       <c r="C92" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D92" s="22"/>
-      <c r="E92" s="22"/>
-      <c r="F92" s="20" t="s">
+      <c r="D92" s="21"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G92" s="20"/>
-      <c r="H92" s="21">
+      <c r="G92" s="19"/>
+      <c r="H92" s="20">
         <v>0.996</v>
       </c>
     </row>
@@ -2621,13 +2613,13 @@
       <c r="C93" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D93" s="22"/>
-      <c r="E93" s="22"/>
-      <c r="F93" s="20" t="s">
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G93" s="20"/>
-      <c r="H93" s="21">
+      <c r="G93" s="19"/>
+      <c r="H93" s="20">
         <v>0.997</v>
       </c>
     </row>
@@ -2639,13 +2631,13 @@
       <c r="C94" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D94" s="22"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="20" t="s">
+      <c r="D94" s="21"/>
+      <c r="E94" s="21"/>
+      <c r="F94" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G94" s="20"/>
-      <c r="H94" s="21">
+      <c r="G94" s="19"/>
+      <c r="H94" s="20">
         <v>0.998</v>
       </c>
     </row>
@@ -2657,13 +2649,13 @@
       <c r="C95" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D95" s="22"/>
-      <c r="E95" s="22"/>
-      <c r="F95" s="20" t="s">
+      <c r="D95" s="21"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G95" s="20"/>
-      <c r="H95" s="21">
+      <c r="G95" s="19"/>
+      <c r="H95" s="20">
         <v>0.999</v>
       </c>
     </row>
@@ -2675,13 +2667,13 @@
       <c r="C96" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D96" s="22"/>
-      <c r="E96" s="22"/>
-      <c r="F96" s="20" t="s">
+      <c r="D96" s="21"/>
+      <c r="E96" s="21"/>
+      <c r="F96" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G96" s="20"/>
-      <c r="H96" s="21">
+      <c r="G96" s="19"/>
+      <c r="H96" s="20">
         <v>1</v>
       </c>
     </row>
@@ -2693,13 +2685,13 @@
       <c r="C97" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D97" s="20" t="s">
+      <c r="D97" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E97" s="20"/>
-      <c r="F97" s="20"/>
-      <c r="G97" s="20"/>
-      <c r="H97" s="21">
+      <c r="E97" s="19"/>
+      <c r="F97" s="19"/>
+      <c r="G97" s="19"/>
+      <c r="H97" s="20">
         <v>0.2</v>
       </c>
     </row>
@@ -2711,13 +2703,13 @@
       <c r="C98" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D98" s="20" t="s">
+      <c r="D98" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E98" s="20"/>
-      <c r="F98" s="20"/>
-      <c r="G98" s="20"/>
-      <c r="H98" s="21">
+      <c r="E98" s="19"/>
+      <c r="F98" s="19"/>
+      <c r="G98" s="19"/>
+      <c r="H98" s="20">
         <v>0.3</v>
       </c>
     </row>
@@ -2729,13 +2721,13 @@
       <c r="C99" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D99" s="20" t="s">
+      <c r="D99" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E99" s="20"/>
-      <c r="F99" s="20"/>
-      <c r="G99" s="20"/>
-      <c r="H99" s="21">
+      <c r="E99" s="19"/>
+      <c r="F99" s="19"/>
+      <c r="G99" s="19"/>
+      <c r="H99" s="20">
         <v>0.4</v>
       </c>
     </row>
@@ -2747,13 +2739,13 @@
       <c r="C100" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D100" s="20" t="s">
+      <c r="D100" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E100" s="20"/>
-      <c r="F100" s="20"/>
-      <c r="G100" s="20"/>
-      <c r="H100" s="21">
+      <c r="E100" s="19"/>
+      <c r="F100" s="19"/>
+      <c r="G100" s="19"/>
+      <c r="H100" s="20">
         <v>0.5</v>
       </c>
     </row>
@@ -2765,13 +2757,13 @@
       <c r="C101" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D101" s="20" t="s">
+      <c r="D101" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E101" s="20"/>
-      <c r="F101" s="20"/>
-      <c r="G101" s="20"/>
-      <c r="H101" s="21">
+      <c r="E101" s="19"/>
+      <c r="F101" s="19"/>
+      <c r="G101" s="19"/>
+      <c r="H101" s="20">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -2783,13 +2775,13 @@
       <c r="C102" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D102" s="20" t="s">
+      <c r="D102" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E102" s="20"/>
-      <c r="F102" s="20"/>
-      <c r="G102" s="20"/>
-      <c r="H102" s="21">
+      <c r="E102" s="19"/>
+      <c r="F102" s="19"/>
+      <c r="G102" s="19"/>
+      <c r="H102" s="20">
         <v>0.6</v>
       </c>
     </row>
@@ -2801,13 +2793,13 @@
       <c r="C103" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D103" s="20" t="s">
+      <c r="D103" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E103" s="20"/>
-      <c r="F103" s="20"/>
-      <c r="G103" s="20"/>
-      <c r="H103" s="21">
+      <c r="E103" s="19"/>
+      <c r="F103" s="19"/>
+      <c r="G103" s="19"/>
+      <c r="H103" s="20">
         <v>0.65</v>
       </c>
     </row>
@@ -2819,13 +2811,13 @@
       <c r="C104" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D104" s="20" t="s">
+      <c r="D104" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E104" s="20"/>
-      <c r="F104" s="20"/>
-      <c r="G104" s="20"/>
-      <c r="H104" s="21">
+      <c r="E104" s="19"/>
+      <c r="F104" s="19"/>
+      <c r="G104" s="19"/>
+      <c r="H104" s="20">
         <v>0.72</v>
       </c>
     </row>
@@ -2837,13 +2829,13 @@
       <c r="C105" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D105" s="20" t="s">
+      <c r="D105" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="E105" s="20"/>
-      <c r="F105" s="20"/>
-      <c r="G105" s="20"/>
-      <c r="H105" s="21">
+      <c r="E105" s="19"/>
+      <c r="F105" s="19"/>
+      <c r="G105" s="19"/>
+      <c r="H105" s="20">
         <v>0.75</v>
       </c>
     </row>
@@ -2855,13 +2847,13 @@
       <c r="C106" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D106" s="20" t="s">
+      <c r="D106" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E106" s="20"/>
-      <c r="F106" s="20"/>
-      <c r="G106" s="20"/>
-      <c r="H106" s="21">
+      <c r="E106" s="19"/>
+      <c r="F106" s="19"/>
+      <c r="G106" s="19"/>
+      <c r="H106" s="20">
         <v>0.79</v>
       </c>
     </row>
@@ -2873,13 +2865,13 @@
       <c r="C107" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D107" s="20" t="s">
+      <c r="D107" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E107" s="20"/>
-      <c r="F107" s="20"/>
-      <c r="G107" s="20"/>
-      <c r="H107" s="21">
+      <c r="E107" s="19"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="19"/>
+      <c r="H107" s="20">
         <v>0.82</v>
       </c>
     </row>
@@ -2891,13 +2883,13 @@
       <c r="C108" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D108" s="20" t="s">
+      <c r="D108" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E108" s="20"/>
-      <c r="F108" s="20"/>
-      <c r="G108" s="20"/>
-      <c r="H108" s="21">
+      <c r="E108" s="19"/>
+      <c r="F108" s="19"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="20">
         <v>0.85</v>
       </c>
     </row>
@@ -2909,13 +2901,13 @@
       <c r="C109" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D109" s="20" t="s">
+      <c r="D109" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="E109" s="20"/>
-      <c r="F109" s="20"/>
-      <c r="G109" s="20"/>
-      <c r="H109" s="21">
+      <c r="E109" s="19"/>
+      <c r="F109" s="19"/>
+      <c r="G109" s="19"/>
+      <c r="H109" s="20">
         <v>0.88</v>
       </c>
     </row>
@@ -2927,13 +2919,13 @@
       <c r="C110" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D110" s="20" t="s">
+      <c r="D110" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E110" s="20"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="20"/>
-      <c r="H110" s="21">
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="19"/>
+      <c r="H110" s="20">
         <v>0.9</v>
       </c>
     </row>
@@ -2945,13 +2937,13 @@
       <c r="C111" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D111" s="20" t="s">
+      <c r="D111" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E111" s="20"/>
-      <c r="F111" s="20"/>
-      <c r="G111" s="20"/>
-      <c r="H111" s="21">
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="19"/>
+      <c r="H111" s="20">
         <v>0.92</v>
       </c>
     </row>
@@ -2963,13 +2955,13 @@
       <c r="C112" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D112" s="20" t="s">
+      <c r="D112" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E112" s="20"/>
-      <c r="F112" s="20"/>
-      <c r="G112" s="20"/>
-      <c r="H112" s="21">
+      <c r="E112" s="19"/>
+      <c r="F112" s="19"/>
+      <c r="G112" s="19"/>
+      <c r="H112" s="20">
         <v>0.94</v>
       </c>
     </row>
@@ -2981,13 +2973,13 @@
       <c r="C113" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D113" s="20" t="s">
+      <c r="D113" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E113" s="20"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="20"/>
-      <c r="H113" s="21">
+      <c r="E113" s="19"/>
+      <c r="F113" s="19"/>
+      <c r="G113" s="19"/>
+      <c r="H113" s="20">
         <v>0.96</v>
       </c>
     </row>
@@ -2999,13 +2991,13 @@
       <c r="C114" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D114" s="20" t="s">
+      <c r="D114" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E114" s="20"/>
-      <c r="F114" s="20"/>
-      <c r="G114" s="20"/>
-      <c r="H114" s="21">
+      <c r="E114" s="19"/>
+      <c r="F114" s="19"/>
+      <c r="G114" s="19"/>
+      <c r="H114" s="20">
         <v>0.99</v>
       </c>
     </row>
@@ -3017,13 +3009,13 @@
       <c r="C115" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D115" s="20" t="s">
+      <c r="D115" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E115" s="20"/>
-      <c r="F115" s="20"/>
-      <c r="G115" s="20"/>
-      <c r="H115" s="21">
+      <c r="E115" s="19"/>
+      <c r="F115" s="19"/>
+      <c r="G115" s="19"/>
+      <c r="H115" s="20">
         <v>1</v>
       </c>
     </row>
@@ -3036,12 +3028,12 @@
         <v>36</v>
       </c>
       <c r="D116" s="15"/>
-      <c r="E116" s="22"/>
-      <c r="F116" s="20" t="s">
+      <c r="E116" s="21"/>
+      <c r="F116" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G116" s="20"/>
-      <c r="H116" s="21">
+      <c r="G116" s="19"/>
+      <c r="H116" s="20">
         <v>0.5</v>
       </c>
     </row>
@@ -3054,12 +3046,12 @@
         <v>36</v>
       </c>
       <c r="D117" s="15"/>
-      <c r="E117" s="22"/>
-      <c r="F117" s="20" t="s">
+      <c r="E117" s="21"/>
+      <c r="F117" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G117" s="20"/>
-      <c r="H117" s="21">
+      <c r="G117" s="19"/>
+      <c r="H117" s="20">
         <v>1</v>
       </c>
     </row>
@@ -3072,12 +3064,12 @@
         <v>36</v>
       </c>
       <c r="D118" s="15"/>
-      <c r="E118" s="22"/>
-      <c r="F118" s="20" t="s">
+      <c r="E118" s="21"/>
+      <c r="F118" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G118" s="20"/>
-      <c r="H118" s="21">
+      <c r="G118" s="19"/>
+      <c r="H118" s="20">
         <v>1.3</v>
       </c>
     </row>
@@ -3090,12 +3082,12 @@
         <v>36</v>
       </c>
       <c r="D119" s="15"/>
-      <c r="E119" s="22"/>
-      <c r="F119" s="20" t="s">
+      <c r="E119" s="21"/>
+      <c r="F119" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G119" s="20"/>
-      <c r="H119" s="21">
+      <c r="G119" s="19"/>
+      <c r="H119" s="20">
         <v>2</v>
       </c>
     </row>
@@ -3108,12 +3100,12 @@
         <v>36</v>
       </c>
       <c r="D120" s="15"/>
-      <c r="E120" s="22"/>
-      <c r="F120" s="20" t="s">
+      <c r="E120" s="21"/>
+      <c r="F120" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G120" s="20"/>
-      <c r="H120" s="21">
+      <c r="G120" s="19"/>
+      <c r="H120" s="20">
         <v>2.1</v>
       </c>
     </row>
@@ -3126,12 +3118,12 @@
         <v>36</v>
       </c>
       <c r="D121" s="15"/>
-      <c r="E121" s="22"/>
-      <c r="F121" s="20" t="s">
+      <c r="E121" s="21"/>
+      <c r="F121" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G121" s="20"/>
-      <c r="H121" s="21">
+      <c r="G121" s="19"/>
+      <c r="H121" s="20">
         <v>3</v>
       </c>
     </row>
@@ -3144,12 +3136,12 @@
         <v>36</v>
       </c>
       <c r="D122" s="15"/>
-      <c r="E122" s="22"/>
-      <c r="F122" s="20" t="s">
+      <c r="E122" s="21"/>
+      <c r="F122" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G122" s="20"/>
-      <c r="H122" s="21">
+      <c r="G122" s="19"/>
+      <c r="H122" s="20">
         <v>3</v>
       </c>
     </row>
@@ -3162,12 +3154,12 @@
         <v>36</v>
       </c>
       <c r="D123" s="15"/>
-      <c r="E123" s="22"/>
-      <c r="F123" s="20" t="s">
+      <c r="E123" s="21"/>
+      <c r="F123" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="G123" s="20"/>
-      <c r="H123" s="21">
+      <c r="G123" s="19"/>
+      <c r="H123" s="20">
         <v>4</v>
       </c>
     </row>
@@ -3180,12 +3172,12 @@
         <v>36</v>
       </c>
       <c r="D124" s="15"/>
-      <c r="E124" s="22"/>
-      <c r="F124" s="20" t="s">
+      <c r="E124" s="21"/>
+      <c r="F124" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G124" s="20"/>
-      <c r="H124" s="21">
+      <c r="G124" s="19"/>
+      <c r="H124" s="20">
         <v>6</v>
       </c>
     </row>
@@ -3198,12 +3190,12 @@
         <v>36</v>
       </c>
       <c r="D125" s="15"/>
-      <c r="E125" s="22"/>
-      <c r="F125" s="20" t="s">
+      <c r="E125" s="21"/>
+      <c r="F125" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G125" s="20"/>
-      <c r="H125" s="21">
+      <c r="G125" s="19"/>
+      <c r="H125" s="20">
         <v>10</v>
       </c>
     </row>
@@ -3216,12 +3208,12 @@
         <v>36</v>
       </c>
       <c r="D126" s="15"/>
-      <c r="E126" s="22"/>
-      <c r="F126" s="20" t="s">
+      <c r="E126" s="21"/>
+      <c r="F126" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G126" s="20"/>
-      <c r="H126" s="21">
+      <c r="G126" s="19"/>
+      <c r="H126" s="20">
         <v>15</v>
       </c>
     </row>
@@ -3234,12 +3226,12 @@
         <v>36</v>
       </c>
       <c r="D127" s="15"/>
-      <c r="E127" s="22"/>
-      <c r="F127" s="20" t="s">
+      <c r="E127" s="21"/>
+      <c r="F127" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G127" s="20"/>
-      <c r="H127" s="21">
+      <c r="G127" s="19"/>
+      <c r="H127" s="20">
         <v>21</v>
       </c>
     </row>
@@ -3252,12 +3244,12 @@
         <v>64</v>
       </c>
       <c r="D128" s="15"/>
-      <c r="E128" s="22"/>
-      <c r="F128" s="20" t="s">
+      <c r="E128" s="21"/>
+      <c r="F128" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G128" s="20"/>
-      <c r="H128" s="21">
+      <c r="G128" s="19"/>
+      <c r="H128" s="20">
         <v>0.1</v>
       </c>
     </row>
@@ -3270,12 +3262,12 @@
         <v>64</v>
       </c>
       <c r="D129" s="15"/>
-      <c r="E129" s="22"/>
-      <c r="F129" s="20" t="s">
+      <c r="E129" s="21"/>
+      <c r="F129" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G129" s="20"/>
-      <c r="H129" s="21">
+      <c r="G129" s="19"/>
+      <c r="H129" s="20">
         <v>0.32</v>
       </c>
     </row>
@@ -3288,12 +3280,12 @@
         <v>64</v>
       </c>
       <c r="D130" s="15"/>
-      <c r="E130" s="22"/>
-      <c r="F130" s="20" t="s">
+      <c r="E130" s="21"/>
+      <c r="F130" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G130" s="20"/>
-      <c r="H130" s="21">
+      <c r="G130" s="19"/>
+      <c r="H130" s="20">
         <v>0.4</v>
       </c>
     </row>
@@ -3306,12 +3298,12 @@
         <v>64</v>
       </c>
       <c r="D131" s="15"/>
-      <c r="E131" s="22"/>
-      <c r="F131" s="20" t="s">
+      <c r="E131" s="21"/>
+      <c r="F131" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G131" s="20"/>
-      <c r="H131" s="21">
+      <c r="G131" s="19"/>
+      <c r="H131" s="20">
         <v>0.45</v>
       </c>
     </row>
@@ -3324,12 +3316,12 @@
         <v>64</v>
       </c>
       <c r="D132" s="15"/>
-      <c r="E132" s="22"/>
-      <c r="F132" s="20" t="s">
+      <c r="E132" s="21"/>
+      <c r="F132" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G132" s="20"/>
-      <c r="H132" s="21">
+      <c r="G132" s="19"/>
+      <c r="H132" s="20">
         <v>0.48</v>
       </c>
     </row>
@@ -3342,12 +3334,12 @@
         <v>64</v>
       </c>
       <c r="D133" s="15"/>
-      <c r="E133" s="22"/>
-      <c r="F133" s="20" t="s">
+      <c r="E133" s="21"/>
+      <c r="F133" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G133" s="20"/>
-      <c r="H133" s="21">
+      <c r="G133" s="19"/>
+      <c r="H133" s="20">
         <v>0.5</v>
       </c>
     </row>
@@ -3360,12 +3352,12 @@
         <v>64</v>
       </c>
       <c r="D134" s="15"/>
-      <c r="E134" s="22"/>
-      <c r="F134" s="20" t="s">
+      <c r="E134" s="21"/>
+      <c r="F134" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G134" s="20"/>
-      <c r="H134" s="21">
+      <c r="G134" s="19"/>
+      <c r="H134" s="20">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -3378,12 +3370,12 @@
         <v>64</v>
       </c>
       <c r="D135" s="15"/>
-      <c r="E135" s="22"/>
-      <c r="F135" s="20" t="s">
+      <c r="E135" s="21"/>
+      <c r="F135" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="G135" s="20"/>
-      <c r="H135" s="21">
+      <c r="G135" s="19"/>
+      <c r="H135" s="20">
         <v>0.6</v>
       </c>
     </row>
@@ -3396,12 +3388,12 @@
         <v>64</v>
       </c>
       <c r="D136" s="15"/>
-      <c r="E136" s="22"/>
-      <c r="F136" s="20" t="s">
+      <c r="E136" s="21"/>
+      <c r="F136" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G136" s="20"/>
-      <c r="H136" s="21">
+      <c r="G136" s="19"/>
+      <c r="H136" s="20">
         <v>0.75</v>
       </c>
     </row>
@@ -3414,12 +3406,12 @@
         <v>64</v>
       </c>
       <c r="D137" s="15"/>
-      <c r="E137" s="22"/>
-      <c r="F137" s="20" t="s">
+      <c r="E137" s="21"/>
+      <c r="F137" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G137" s="20"/>
-      <c r="H137" s="21">
+      <c r="G137" s="19"/>
+      <c r="H137" s="20">
         <v>0.8</v>
       </c>
     </row>
@@ -3432,12 +3424,12 @@
         <v>64</v>
       </c>
       <c r="D138" s="15"/>
-      <c r="E138" s="22"/>
-      <c r="F138" s="20" t="s">
+      <c r="E138" s="21"/>
+      <c r="F138" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G138" s="20"/>
-      <c r="H138" s="21">
+      <c r="G138" s="19"/>
+      <c r="H138" s="20">
         <v>0.99</v>
       </c>
     </row>
@@ -3450,12 +3442,12 @@
         <v>64</v>
       </c>
       <c r="D139" s="15"/>
-      <c r="E139" s="22"/>
-      <c r="F139" s="20" t="s">
+      <c r="E139" s="21"/>
+      <c r="F139" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G139" s="20"/>
-      <c r="H139" s="21">
+      <c r="G139" s="19"/>
+      <c r="H139" s="20">
         <v>1</v>
       </c>
     </row>
@@ -3468,12 +3460,12 @@
         <v>65</v>
       </c>
       <c r="D140" s="15"/>
-      <c r="E140" s="22"/>
-      <c r="F140" s="20" t="s">
+      <c r="E140" s="21"/>
+      <c r="F140" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G140" s="20"/>
-      <c r="H140" s="21">
+      <c r="G140" s="19"/>
+      <c r="H140" s="20">
         <v>0.5</v>
       </c>
     </row>
@@ -3486,12 +3478,12 @@
         <v>65</v>
       </c>
       <c r="D141" s="15"/>
-      <c r="E141" s="22"/>
-      <c r="F141" s="20" t="s">
+      <c r="E141" s="21"/>
+      <c r="F141" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G141" s="20"/>
-      <c r="H141" s="21">
+      <c r="G141" s="19"/>
+      <c r="H141" s="20">
         <v>1</v>
       </c>
     </row>
@@ -3504,12 +3496,12 @@
         <v>65</v>
       </c>
       <c r="D142" s="15"/>
-      <c r="E142" s="22"/>
-      <c r="F142" s="20" t="s">
+      <c r="E142" s="21"/>
+      <c r="F142" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G142" s="20"/>
-      <c r="H142" s="21">
+      <c r="G142" s="19"/>
+      <c r="H142" s="20">
         <v>1.3</v>
       </c>
     </row>
@@ -3522,12 +3514,12 @@
         <v>65</v>
       </c>
       <c r="D143" s="15"/>
-      <c r="E143" s="22"/>
-      <c r="F143" s="20" t="s">
+      <c r="E143" s="21"/>
+      <c r="F143" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G143" s="20"/>
-      <c r="H143" s="21">
+      <c r="G143" s="19"/>
+      <c r="H143" s="20">
         <v>2</v>
       </c>
     </row>
@@ -3540,12 +3532,12 @@
         <v>65</v>
       </c>
       <c r="D144" s="15"/>
-      <c r="E144" s="22"/>
-      <c r="F144" s="20" t="s">
+      <c r="E144" s="21"/>
+      <c r="F144" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G144" s="20"/>
-      <c r="H144" s="21">
+      <c r="G144" s="19"/>
+      <c r="H144" s="20">
         <v>2.1</v>
       </c>
     </row>
@@ -3558,12 +3550,12 @@
         <v>65</v>
       </c>
       <c r="D145" s="15"/>
-      <c r="E145" s="22"/>
-      <c r="F145" s="20" t="s">
+      <c r="E145" s="21"/>
+      <c r="F145" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G145" s="20"/>
-      <c r="H145" s="21">
+      <c r="G145" s="19"/>
+      <c r="H145" s="20">
         <v>3</v>
       </c>
     </row>
@@ -3576,12 +3568,12 @@
         <v>65</v>
       </c>
       <c r="D146" s="15"/>
-      <c r="E146" s="22"/>
-      <c r="F146" s="20" t="s">
+      <c r="E146" s="21"/>
+      <c r="F146" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G146" s="20"/>
-      <c r="H146" s="21">
+      <c r="G146" s="19"/>
+      <c r="H146" s="20">
         <v>3</v>
       </c>
     </row>
@@ -3594,12 +3586,12 @@
         <v>65</v>
       </c>
       <c r="D147" s="15"/>
-      <c r="E147" s="22"/>
-      <c r="F147" s="20" t="s">
+      <c r="E147" s="21"/>
+      <c r="F147" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="G147" s="20"/>
-      <c r="H147" s="21">
+      <c r="G147" s="19"/>
+      <c r="H147" s="20">
         <v>4</v>
       </c>
     </row>
@@ -3612,12 +3604,12 @@
         <v>65</v>
       </c>
       <c r="D148" s="15"/>
-      <c r="E148" s="22"/>
-      <c r="F148" s="20" t="s">
+      <c r="E148" s="21"/>
+      <c r="F148" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G148" s="20"/>
-      <c r="H148" s="21">
+      <c r="G148" s="19"/>
+      <c r="H148" s="20">
         <v>6</v>
       </c>
     </row>
@@ -3630,12 +3622,12 @@
         <v>65</v>
       </c>
       <c r="D149" s="15"/>
-      <c r="E149" s="22"/>
-      <c r="F149" s="20" t="s">
+      <c r="E149" s="21"/>
+      <c r="F149" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G149" s="20"/>
-      <c r="H149" s="21">
+      <c r="G149" s="19"/>
+      <c r="H149" s="20">
         <v>10</v>
       </c>
     </row>
@@ -3648,12 +3640,12 @@
         <v>65</v>
       </c>
       <c r="D150" s="15"/>
-      <c r="E150" s="22"/>
-      <c r="F150" s="20" t="s">
+      <c r="E150" s="21"/>
+      <c r="F150" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G150" s="20"/>
-      <c r="H150" s="21">
+      <c r="G150" s="19"/>
+      <c r="H150" s="20">
         <v>15</v>
       </c>
     </row>
@@ -3666,12 +3658,12 @@
         <v>65</v>
       </c>
       <c r="D151" s="15"/>
-      <c r="E151" s="22"/>
-      <c r="F151" s="20" t="s">
+      <c r="E151" s="21"/>
+      <c r="F151" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G151" s="20"/>
-      <c r="H151" s="21">
+      <c r="G151" s="19"/>
+      <c r="H151" s="20">
         <v>21</v>
       </c>
     </row>
@@ -3684,12 +3676,12 @@
         <v>66</v>
       </c>
       <c r="D152" s="15"/>
-      <c r="E152" s="22"/>
-      <c r="F152" s="20" t="s">
+      <c r="E152" s="21"/>
+      <c r="F152" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G152" s="20"/>
-      <c r="H152" s="21">
+      <c r="G152" s="19"/>
+      <c r="H152" s="20">
         <v>0.4</v>
       </c>
     </row>
@@ -3702,12 +3694,12 @@
         <v>66</v>
       </c>
       <c r="D153" s="15"/>
-      <c r="E153" s="22"/>
-      <c r="F153" s="20" t="s">
+      <c r="E153" s="21"/>
+      <c r="F153" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G153" s="20"/>
-      <c r="H153" s="21">
+      <c r="G153" s="19"/>
+      <c r="H153" s="20">
         <v>0.8</v>
       </c>
     </row>
@@ -3720,12 +3712,12 @@
         <v>66</v>
       </c>
       <c r="D154" s="15"/>
-      <c r="E154" s="22"/>
-      <c r="F154" s="20" t="s">
+      <c r="E154" s="21"/>
+      <c r="F154" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G154" s="20"/>
-      <c r="H154" s="21">
+      <c r="G154" s="19"/>
+      <c r="H154" s="20">
         <v>0.82</v>
       </c>
     </row>
@@ -3738,12 +3730,12 @@
         <v>66</v>
       </c>
       <c r="D155" s="15"/>
-      <c r="E155" s="22"/>
-      <c r="F155" s="20" t="s">
+      <c r="E155" s="21"/>
+      <c r="F155" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G155" s="20"/>
-      <c r="H155" s="21">
+      <c r="G155" s="19"/>
+      <c r="H155" s="20">
         <v>0.85</v>
       </c>
     </row>
@@ -3756,12 +3748,12 @@
         <v>66</v>
       </c>
       <c r="D156" s="15"/>
-      <c r="E156" s="22"/>
-      <c r="F156" s="20" t="s">
+      <c r="E156" s="21"/>
+      <c r="F156" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G156" s="20"/>
-      <c r="H156" s="21">
+      <c r="G156" s="19"/>
+      <c r="H156" s="20">
         <v>0.87</v>
       </c>
     </row>
@@ -3774,12 +3766,12 @@
         <v>66</v>
       </c>
       <c r="D157" s="15"/>
-      <c r="E157" s="22"/>
-      <c r="F157" s="20" t="s">
+      <c r="E157" s="21"/>
+      <c r="F157" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G157" s="20"/>
-      <c r="H157" s="21">
+      <c r="G157" s="19"/>
+      <c r="H157" s="20">
         <v>0.88</v>
       </c>
     </row>
@@ -3792,12 +3784,12 @@
         <v>66</v>
       </c>
       <c r="D158" s="15"/>
-      <c r="E158" s="22"/>
-      <c r="F158" s="20" t="s">
+      <c r="E158" s="21"/>
+      <c r="F158" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G158" s="20"/>
-      <c r="H158" s="21">
+      <c r="G158" s="19"/>
+      <c r="H158" s="20">
         <v>0.9</v>
       </c>
     </row>
@@ -3810,12 +3802,12 @@
         <v>66</v>
       </c>
       <c r="D159" s="15"/>
-      <c r="E159" s="22"/>
-      <c r="F159" s="20" t="s">
+      <c r="E159" s="21"/>
+      <c r="F159" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="G159" s="20"/>
-      <c r="H159" s="21">
+      <c r="G159" s="19"/>
+      <c r="H159" s="20">
         <v>0.91</v>
       </c>
     </row>
@@ -3828,12 +3820,12 @@
         <v>66</v>
       </c>
       <c r="D160" s="15"/>
-      <c r="E160" s="22"/>
-      <c r="F160" s="20" t="s">
+      <c r="E160" s="21"/>
+      <c r="F160" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G160" s="20"/>
-      <c r="H160" s="21">
+      <c r="G160" s="19"/>
+      <c r="H160" s="20">
         <v>0.93</v>
       </c>
     </row>
@@ -3846,12 +3838,12 @@
         <v>66</v>
       </c>
       <c r="D161" s="15"/>
-      <c r="E161" s="22"/>
-      <c r="F161" s="20" t="s">
+      <c r="E161" s="21"/>
+      <c r="F161" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G161" s="20"/>
-      <c r="H161" s="21">
+      <c r="G161" s="19"/>
+      <c r="H161" s="20">
         <v>0.95</v>
       </c>
     </row>
@@ -3864,12 +3856,12 @@
         <v>66</v>
       </c>
       <c r="D162" s="15"/>
-      <c r="E162" s="22"/>
-      <c r="F162" s="20" t="s">
+      <c r="E162" s="21"/>
+      <c r="F162" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G162" s="20"/>
-      <c r="H162" s="21">
+      <c r="G162" s="19"/>
+      <c r="H162" s="20">
         <v>0.99</v>
       </c>
     </row>
@@ -3882,12 +3874,12 @@
         <v>66</v>
       </c>
       <c r="D163" s="15"/>
-      <c r="E163" s="22"/>
-      <c r="F163" s="20" t="s">
+      <c r="E163" s="21"/>
+      <c r="F163" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G163" s="20"/>
-      <c r="H163" s="21">
+      <c r="G163" s="19"/>
+      <c r="H163" s="20">
         <v>1</v>
       </c>
     </row>
@@ -3899,13 +3891,13 @@
       <c r="C164" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D164" s="20"/>
-      <c r="E164" s="20"/>
-      <c r="F164" s="20" t="s">
+      <c r="D164" s="19"/>
+      <c r="E164" s="19"/>
+      <c r="F164" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="G164" s="20"/>
-      <c r="H164" s="21">
+      <c r="G164" s="19"/>
+      <c r="H164" s="20">
         <v>0.4</v>
       </c>
     </row>
@@ -3917,13 +3909,13 @@
       <c r="C165" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D165" s="20"/>
-      <c r="E165" s="20"/>
-      <c r="F165" s="20" t="s">
+      <c r="D165" s="19"/>
+      <c r="E165" s="19"/>
+      <c r="F165" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G165" s="20"/>
-      <c r="H165" s="21">
+      <c r="G165" s="19"/>
+      <c r="H165" s="20">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -3935,13 +3927,13 @@
       <c r="C166" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D166" s="20"/>
-      <c r="E166" s="20"/>
-      <c r="F166" s="20" t="s">
+      <c r="D166" s="19"/>
+      <c r="E166" s="19"/>
+      <c r="F166" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G166" s="20"/>
-      <c r="H166" s="21">
+      <c r="G166" s="19"/>
+      <c r="H166" s="20">
         <v>0.63</v>
       </c>
     </row>
@@ -3953,13 +3945,13 @@
       <c r="C167" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D167" s="20"/>
-      <c r="E167" s="20"/>
-      <c r="F167" s="20" t="s">
+      <c r="D167" s="19"/>
+      <c r="E167" s="19"/>
+      <c r="F167" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="G167" s="20"/>
-      <c r="H167" s="21">
+      <c r="G167" s="19"/>
+      <c r="H167" s="20">
         <v>0.74</v>
       </c>
     </row>
@@ -3971,13 +3963,13 @@
       <c r="C168" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D168" s="20"/>
-      <c r="E168" s="20"/>
-      <c r="F168" s="20" t="s">
+      <c r="D168" s="19"/>
+      <c r="E168" s="19"/>
+      <c r="F168" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G168" s="20"/>
-      <c r="H168" s="21">
+      <c r="G168" s="19"/>
+      <c r="H168" s="20">
         <v>0.85</v>
       </c>
     </row>
@@ -3989,13 +3981,13 @@
       <c r="C169" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D169" s="20"/>
-      <c r="E169" s="20"/>
-      <c r="F169" s="20" t="s">
+      <c r="D169" s="19"/>
+      <c r="E169" s="19"/>
+      <c r="F169" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G169" s="20"/>
-      <c r="H169" s="21">
+      <c r="G169" s="19"/>
+      <c r="H169" s="20">
         <v>0.98</v>
       </c>
     </row>
@@ -4007,13 +3999,13 @@
       <c r="C170" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D170" s="20"/>
-      <c r="E170" s="20"/>
-      <c r="F170" s="20" t="s">
+      <c r="D170" s="19"/>
+      <c r="E170" s="19"/>
+      <c r="F170" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="G170" s="20"/>
-      <c r="H170" s="21">
+      <c r="G170" s="19"/>
+      <c r="H170" s="20">
         <v>1</v>
       </c>
     </row>
@@ -4026,14 +4018,14 @@
         <v>75</v>
       </c>
       <c r="D171" s="15"/>
-      <c r="E171" s="22" t="s">
+      <c r="E171" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="F171" s="20" t="s">
+      <c r="F171" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="G171" s="20"/>
-      <c r="H171" s="21">
+      <c r="G171" s="19"/>
+      <c r="H171" s="20">
         <v>1</v>
       </c>
     </row>
@@ -4046,14 +4038,14 @@
         <v>75</v>
       </c>
       <c r="D172" s="15"/>
-      <c r="E172" s="22" t="s">
+      <c r="E172" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="F172" s="20" t="s">
+      <c r="F172" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="G172" s="20"/>
-      <c r="H172" s="21">
+      <c r="G172" s="19"/>
+      <c r="H172" s="20">
         <v>2</v>
       </c>
     </row>
@@ -4066,14 +4058,14 @@
         <v>75</v>
       </c>
       <c r="D173" s="15"/>
-      <c r="E173" s="22" t="s">
+      <c r="E173" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="F173" s="20" t="s">
+      <c r="F173" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="G173" s="20"/>
-      <c r="H173" s="21">
+      <c r="G173" s="19"/>
+      <c r="H173" s="20">
         <v>3</v>
       </c>
     </row>
@@ -4086,14 +4078,14 @@
         <v>75</v>
       </c>
       <c r="D174" s="15"/>
-      <c r="E174" s="22" t="s">
+      <c r="E174" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="F174" s="20" t="s">
+      <c r="F174" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="G174" s="20"/>
-      <c r="H174" s="21">
+      <c r="G174" s="19"/>
+      <c r="H174" s="20">
         <v>4</v>
       </c>
     </row>
@@ -4106,14 +4098,14 @@
         <v>75</v>
       </c>
       <c r="D175" s="15"/>
-      <c r="E175" s="22" t="s">
+      <c r="E175" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="F175" s="20" t="s">
+      <c r="F175" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="G175" s="20"/>
-      <c r="H175" s="21">
+      <c r="G175" s="19"/>
+      <c r="H175" s="20">
         <v>5</v>
       </c>
     </row>
@@ -4126,14 +4118,14 @@
         <v>75</v>
       </c>
       <c r="D176" s="15"/>
-      <c r="E176" s="22" t="s">
+      <c r="E176" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="F176" s="20" t="s">
+      <c r="F176" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="G176" s="20"/>
-      <c r="H176" s="21">
+      <c r="G176" s="19"/>
+      <c r="H176" s="20">
         <v>6</v>
       </c>
     </row>
@@ -4146,14 +4138,14 @@
         <v>75</v>
       </c>
       <c r="D177" s="15"/>
-      <c r="E177" s="22" t="s">
+      <c r="E177" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="F177" s="20" t="s">
+      <c r="F177" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="G177" s="20"/>
-      <c r="H177" s="21">
+      <c r="G177" s="19"/>
+      <c r="H177" s="20">
         <v>7</v>
       </c>
     </row>
@@ -4169,11 +4161,11 @@
       <c r="E178" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F178" s="20" t="s">
+      <c r="F178" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="G178" s="20"/>
-      <c r="H178" s="21">
+      <c r="G178" s="19"/>
+      <c r="H178" s="20">
         <v>0.4</v>
       </c>
     </row>
@@ -4189,11 +4181,11 @@
       <c r="E179" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F179" s="20" t="s">
+      <c r="F179" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="G179" s="20"/>
-      <c r="H179" s="21">
+      <c r="G179" s="19"/>
+      <c r="H179" s="20">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -4209,11 +4201,11 @@
       <c r="E180" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F180" s="20" t="s">
+      <c r="F180" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="G180" s="20"/>
-      <c r="H180" s="21">
+      <c r="G180" s="19"/>
+      <c r="H180" s="20">
         <v>0.63</v>
       </c>
     </row>
@@ -4229,11 +4221,11 @@
       <c r="E181" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F181" s="20" t="s">
+      <c r="F181" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="G181" s="20"/>
-      <c r="H181" s="21">
+      <c r="G181" s="19"/>
+      <c r="H181" s="20">
         <v>0.74</v>
       </c>
     </row>
@@ -4249,11 +4241,11 @@
       <c r="E182" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F182" s="20" t="s">
+      <c r="F182" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="G182" s="20"/>
-      <c r="H182" s="21">
+      <c r="G182" s="19"/>
+      <c r="H182" s="20">
         <v>0.85</v>
       </c>
     </row>
@@ -4269,11 +4261,11 @@
       <c r="E183" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F183" s="20" t="s">
+      <c r="F183" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="G183" s="20"/>
-      <c r="H183" s="21">
+      <c r="G183" s="19"/>
+      <c r="H183" s="20">
         <v>0.98</v>
       </c>
     </row>
@@ -4289,11 +4281,11 @@
       <c r="E184" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F184" s="20" t="s">
+      <c r="F184" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="G184" s="20"/>
-      <c r="H184" s="21">
+      <c r="G184" s="19"/>
+      <c r="H184" s="20">
         <v>1</v>
       </c>
     </row>
@@ -4305,13 +4297,13 @@
       <c r="C185" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D185" s="23"/>
+      <c r="D185" s="22"/>
       <c r="E185" s="15"/>
-      <c r="F185" s="23" t="s">
+      <c r="F185" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="G185" s="23"/>
-      <c r="H185" s="24">
+      <c r="G185" s="22"/>
+      <c r="H185" s="23">
         <v>1</v>
       </c>
     </row>
@@ -4323,13 +4315,13 @@
       <c r="C186" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D186" s="23"/>
+      <c r="D186" s="22"/>
       <c r="E186" s="15"/>
-      <c r="F186" s="23" t="s">
+      <c r="F186" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="G186" s="23"/>
-      <c r="H186" s="24">
+      <c r="G186" s="22"/>
+      <c r="H186" s="23">
         <v>2</v>
       </c>
     </row>
@@ -4341,13 +4333,13 @@
       <c r="C187" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D187" s="23"/>
+      <c r="D187" s="22"/>
       <c r="E187" s="15"/>
-      <c r="F187" s="23" t="s">
+      <c r="F187" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="G187" s="23"/>
-      <c r="H187" s="24">
+      <c r="G187" s="22"/>
+      <c r="H187" s="23">
         <v>2.5</v>
       </c>
     </row>
@@ -4363,11 +4355,11 @@
       <c r="E188" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="F188" s="23" t="s">
+      <c r="F188" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="G188" s="23"/>
-      <c r="H188" s="24">
+      <c r="G188" s="22"/>
+      <c r="H188" s="23">
         <v>1</v>
       </c>
     </row>
@@ -4383,11 +4375,11 @@
       <c r="E189" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="F189" s="23" t="s">
+      <c r="F189" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="G189" s="23"/>
-      <c r="H189" s="24">
+      <c r="G189" s="22"/>
+      <c r="H189" s="23">
         <v>1.5</v>
       </c>
     </row>
@@ -4403,11 +4395,11 @@
       <c r="E190" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="F190" s="23" t="s">
+      <c r="F190" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="G190" s="23"/>
-      <c r="H190" s="24">
+      <c r="G190" s="22"/>
+      <c r="H190" s="23">
         <v>2</v>
       </c>
     </row>
@@ -4420,10 +4412,10 @@
       <c r="D191" s="15"/>
       <c r="E191" s="15"/>
       <c r="F191" s="14"/>
-      <c r="G191" s="20" t="s">
+      <c r="G191" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="H191" s="21">
+      <c r="H191" s="20">
         <v>1</v>
       </c>
     </row>
@@ -4436,10 +4428,10 @@
       <c r="D192" s="15"/>
       <c r="E192" s="15"/>
       <c r="F192" s="14"/>
-      <c r="G192" s="20" t="s">
+      <c r="G192" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="H192" s="21">
+      <c r="H192" s="20">
         <v>0.99039999999999995</v>
       </c>
     </row>
@@ -4452,10 +4444,10 @@
       <c r="D193" s="15"/>
       <c r="E193" s="15"/>
       <c r="F193" s="14"/>
-      <c r="G193" s="20" t="s">
+      <c r="G193" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="H193" s="21">
+      <c r="H193" s="20">
         <v>0.97119999999999995</v>
       </c>
     </row>
@@ -4468,10 +4460,10 @@
       <c r="D194" s="15"/>
       <c r="E194" s="15"/>
       <c r="F194" s="14"/>
-      <c r="G194" s="20" t="s">
+      <c r="G194" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="H194" s="21">
+      <c r="H194" s="20">
         <v>0.95830000000000004</v>
       </c>
     </row>
@@ -4484,10 +4476,10 @@
       <c r="D195" s="15"/>
       <c r="E195" s="15"/>
       <c r="F195" s="14"/>
-      <c r="G195" s="20" t="s">
+      <c r="G195" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="H195" s="21">
+      <c r="H195" s="20">
         <v>0.88</v>
       </c>
     </row>
@@ -4500,10 +4492,10 @@
       <c r="D196" s="15"/>
       <c r="E196" s="15"/>
       <c r="F196" s="14"/>
-      <c r="G196" s="20" t="s">
+      <c r="G196" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="H196" s="21">
+      <c r="H196" s="20">
         <v>0.74</v>
       </c>
     </row>
@@ -4516,10 +4508,10 @@
       <c r="D197" s="15"/>
       <c r="E197" s="15"/>
       <c r="F197" s="14"/>
-      <c r="G197" s="20" t="s">
+      <c r="G197" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="H197" s="21">
+      <c r="H197" s="20">
         <v>0.5</v>
       </c>
     </row>
@@ -4532,10 +4524,10 @@
       <c r="D198" s="15"/>
       <c r="E198" s="15"/>
       <c r="F198" s="14"/>
-      <c r="G198" s="20" t="s">
+      <c r="G198" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H198" s="21">
+      <c r="H198" s="20">
         <v>0.4</v>
       </c>
     </row>
@@ -4548,10 +4540,10 @@
       <c r="D199" s="15"/>
       <c r="E199" s="15"/>
       <c r="F199" s="14"/>
-      <c r="G199" s="20" t="s">
+      <c r="G199" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="H199" s="21">
+      <c r="H199" s="20">
         <v>0.3</v>
       </c>
     </row>
@@ -4564,10 +4556,10 @@
       <c r="D200" s="15"/>
       <c r="E200" s="15"/>
       <c r="F200" s="14"/>
-      <c r="G200" s="20" t="s">
+      <c r="G200" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="H200" s="21">
+      <c r="H200" s="20">
         <v>0.2</v>
       </c>
     </row>
@@ -4580,10 +4572,10 @@
       <c r="D201" s="15"/>
       <c r="E201" s="15"/>
       <c r="F201" s="14"/>
-      <c r="G201" s="20" t="s">
+      <c r="G201" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="H201" s="21">
+      <c r="H201" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -4596,10 +4588,10 @@
       <c r="D202" s="15"/>
       <c r="E202" s="15"/>
       <c r="F202" s="14"/>
-      <c r="G202" s="20" t="s">
+      <c r="G202" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="H202" s="21">
+      <c r="H202" s="20">
         <v>0.16669999999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded 04-May-2021 14:02:37 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="112">
   <si>
     <t>RuleSet</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>coverageFrom</t>
+  </si>
+  <si>
+    <t>$benefit</t>
   </si>
 </sst>
 </file>
@@ -923,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1002,10 +1005,18 @@
       <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="D4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="H4" s="8"/>
       <c r="L4" s="3"/>
     </row>

</xml_diff>

<commit_message>
Uploaded 04-May-2021 14:54:50 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="111">
   <si>
     <t>RuleSet</t>
   </si>
@@ -364,9 +364,6 @@
   </si>
   <si>
     <t>coverageFrom</t>
-  </si>
-  <si>
-    <t>$benefit</t>
   </si>
 </sst>
 </file>
@@ -926,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1006,16 +1003,14 @@
         <v>6</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>111</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="H4" s="8"/>
       <c r="L4" s="3"/>

</xml_diff>

<commit_message>
Uploaded 06-May-2021 14:01:33 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -1089,6 +1089,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1100,12 +1106,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1478,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F184" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190:B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1501,27 +1501,27 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -1554,13 +1554,13 @@
     <row r="4" spans="1:12" ht="25.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="27" t="s">
         <v>264</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="8"/>
       <c r="L4" s="3"/>
     </row>
@@ -5328,155 +5328,177 @@
     </row>
     <row r="191" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="14"/>
-      <c r="B191" s="15"/>
+      <c r="B191" s="15">
+        <v>17</v>
+      </c>
       <c r="C191" s="15"/>
       <c r="D191" s="15"/>
       <c r="E191" s="15"/>
       <c r="F191" s="14"/>
-      <c r="G191" s="28" t="s">
+      <c r="G191" s="24" t="s">
         <v>267</v>
       </c>
-      <c r="H191" s="29">
+      <c r="H191" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="14"/>
-      <c r="B192" s="15"/>
+      <c r="B192" s="15">
+        <v>17</v>
+      </c>
       <c r="C192" s="15"/>
       <c r="D192" s="15"/>
       <c r="E192" s="15"/>
       <c r="F192" s="14"/>
-      <c r="G192" s="28" t="s">
+      <c r="G192" s="24" t="s">
         <v>268</v>
       </c>
-      <c r="H192" s="29">
+      <c r="H192" s="25">
         <v>0.99039999999999995</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="14"/>
-      <c r="B193" s="15"/>
+      <c r="B193" s="15">
+        <v>17</v>
+      </c>
       <c r="C193" s="15"/>
       <c r="D193" s="15"/>
       <c r="E193" s="15"/>
       <c r="F193" s="14"/>
-      <c r="G193" s="28" t="s">
+      <c r="G193" s="24" t="s">
         <v>269</v>
       </c>
-      <c r="H193" s="29">
+      <c r="H193" s="25">
         <v>0.97119999999999995</v>
       </c>
     </row>
     <row r="194" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="14"/>
-      <c r="B194" s="15"/>
+      <c r="B194" s="15">
+        <v>17</v>
+      </c>
       <c r="C194" s="15"/>
       <c r="D194" s="15"/>
       <c r="E194" s="15"/>
       <c r="F194" s="14"/>
-      <c r="G194" s="28" t="s">
+      <c r="G194" s="24" t="s">
         <v>270</v>
       </c>
-      <c r="H194" s="29">
+      <c r="H194" s="25">
         <v>0.95830000000000004</v>
       </c>
     </row>
     <row r="195" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="14"/>
-      <c r="B195" s="15"/>
+      <c r="B195" s="15">
+        <v>17</v>
+      </c>
       <c r="C195" s="15"/>
       <c r="D195" s="15"/>
       <c r="E195" s="15"/>
       <c r="F195" s="14"/>
-      <c r="G195" s="28" t="s">
+      <c r="G195" s="24" t="s">
         <v>271</v>
       </c>
-      <c r="H195" s="29">
+      <c r="H195" s="25">
         <v>0.88</v>
       </c>
     </row>
     <row r="196" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="14"/>
-      <c r="B196" s="15"/>
+      <c r="B196" s="15">
+        <v>17</v>
+      </c>
       <c r="C196" s="15"/>
       <c r="D196" s="15"/>
       <c r="E196" s="15"/>
       <c r="F196" s="14"/>
-      <c r="G196" s="28" t="s">
+      <c r="G196" s="24" t="s">
         <v>272</v>
       </c>
-      <c r="H196" s="29">
+      <c r="H196" s="25">
         <v>0.74</v>
       </c>
     </row>
     <row r="197" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A197" s="14"/>
-      <c r="B197" s="15"/>
+      <c r="B197" s="15">
+        <v>17</v>
+      </c>
       <c r="C197" s="15"/>
       <c r="D197" s="15"/>
       <c r="E197" s="15"/>
       <c r="F197" s="14"/>
-      <c r="G197" s="28" t="s">
+      <c r="G197" s="24" t="s">
         <v>273</v>
       </c>
-      <c r="H197" s="29">
+      <c r="H197" s="25">
         <v>0.5</v>
       </c>
     </row>
     <row r="198" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A198" s="14"/>
-      <c r="B198" s="15"/>
+      <c r="B198" s="15">
+        <v>17</v>
+      </c>
       <c r="C198" s="15"/>
       <c r="D198" s="15"/>
       <c r="E198" s="15"/>
       <c r="F198" s="14"/>
-      <c r="G198" s="28" t="s">
+      <c r="G198" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="H198" s="29">
+      <c r="H198" s="25">
         <v>0.4</v>
       </c>
     </row>
     <row r="199" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" s="14"/>
-      <c r="B199" s="15"/>
+      <c r="B199" s="15">
+        <v>17</v>
+      </c>
       <c r="C199" s="15"/>
       <c r="D199" s="15"/>
       <c r="E199" s="15"/>
       <c r="F199" s="14"/>
-      <c r="G199" s="28" t="s">
+      <c r="G199" s="24" t="s">
         <v>275</v>
       </c>
-      <c r="H199" s="29">
+      <c r="H199" s="25">
         <v>0.3</v>
       </c>
     </row>
     <row r="200" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A200" s="14"/>
-      <c r="B200" s="15"/>
+      <c r="B200" s="15">
+        <v>17</v>
+      </c>
       <c r="C200" s="15"/>
       <c r="D200" s="15"/>
       <c r="E200" s="15"/>
       <c r="F200" s="14"/>
-      <c r="G200" s="28" t="s">
+      <c r="G200" s="24" t="s">
         <v>276</v>
       </c>
-      <c r="H200" s="29">
+      <c r="H200" s="25">
         <v>0.2</v>
       </c>
     </row>
     <row r="201" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A201" s="14"/>
-      <c r="B201" s="15"/>
+      <c r="B201" s="15">
+        <v>17</v>
+      </c>
       <c r="C201" s="15"/>
       <c r="D201" s="15"/>
       <c r="E201" s="15"/>
       <c r="F201" s="14"/>
-      <c r="G201" s="28" t="s">
+      <c r="G201" s="24" t="s">
         <v>277</v>
       </c>
-      <c r="H201" s="29">
+      <c r="H201" s="25">
         <v>0.18</v>
       </c>
     </row>
@@ -5487,10 +5509,10 @@
       <c r="D202" s="15"/>
       <c r="E202" s="15"/>
       <c r="F202" s="14"/>
-      <c r="G202" s="28" t="s">
+      <c r="G202" s="24" t="s">
         <v>278</v>
       </c>
-      <c r="H202" s="29">
+      <c r="H202" s="25">
         <v>0.16669999999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded 06-May-2021 14:06:54 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -1478,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B190" sqref="B190:B201"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190:B202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5504,7 +5504,9 @@
     </row>
     <row r="202" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A202" s="14"/>
-      <c r="B202" s="15"/>
+      <c r="B202" s="15">
+        <v>17</v>
+      </c>
       <c r="C202" s="15"/>
       <c r="D202" s="15"/>
       <c r="E202" s="15"/>

</xml_diff>

<commit_message>
Uploaded 06-May-2021 15:40:30 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="292">
   <si>
     <t>RuleSet</t>
   </si>
@@ -867,6 +867,42 @@
   </si>
   <si>
     <t>coverageFrom</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupName185</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupName186</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupName187</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupName188</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupName189</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupName190</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupName191</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupName192</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupName193</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupName194</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupName195</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupName196</t>
   </si>
 </sst>
 </file>
@@ -1478,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B190" sqref="B190:B202"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A190" sqref="A190:A202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5327,7 +5363,9 @@
       </c>
     </row>
     <row r="191" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A191" s="14"/>
+      <c r="A191" s="14" t="s">
+        <v>280</v>
+      </c>
       <c r="B191" s="15">
         <v>17</v>
       </c>
@@ -5343,7 +5381,9 @@
       </c>
     </row>
     <row r="192" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A192" s="14"/>
+      <c r="A192" s="14" t="s">
+        <v>281</v>
+      </c>
       <c r="B192" s="15">
         <v>17</v>
       </c>
@@ -5359,7 +5399,9 @@
       </c>
     </row>
     <row r="193" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A193" s="14"/>
+      <c r="A193" s="14" t="s">
+        <v>282</v>
+      </c>
       <c r="B193" s="15">
         <v>17</v>
       </c>
@@ -5375,7 +5417,9 @@
       </c>
     </row>
     <row r="194" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A194" s="14"/>
+      <c r="A194" s="14" t="s">
+        <v>283</v>
+      </c>
       <c r="B194" s="15">
         <v>17</v>
       </c>
@@ -5391,7 +5435,9 @@
       </c>
     </row>
     <row r="195" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A195" s="14"/>
+      <c r="A195" s="14" t="s">
+        <v>284</v>
+      </c>
       <c r="B195" s="15">
         <v>17</v>
       </c>
@@ -5407,7 +5453,9 @@
       </c>
     </row>
     <row r="196" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A196" s="14"/>
+      <c r="A196" s="14" t="s">
+        <v>285</v>
+      </c>
       <c r="B196" s="15">
         <v>17</v>
       </c>
@@ -5423,7 +5471,9 @@
       </c>
     </row>
     <row r="197" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A197" s="14"/>
+      <c r="A197" s="14" t="s">
+        <v>286</v>
+      </c>
       <c r="B197" s="15">
         <v>17</v>
       </c>
@@ -5439,7 +5489,9 @@
       </c>
     </row>
     <row r="198" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A198" s="14"/>
+      <c r="A198" s="14" t="s">
+        <v>287</v>
+      </c>
       <c r="B198" s="15">
         <v>17</v>
       </c>
@@ -5455,7 +5507,9 @@
       </c>
     </row>
     <row r="199" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A199" s="14"/>
+      <c r="A199" s="14" t="s">
+        <v>288</v>
+      </c>
       <c r="B199" s="15">
         <v>17</v>
       </c>
@@ -5471,7 +5525,9 @@
       </c>
     </row>
     <row r="200" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A200" s="14"/>
+      <c r="A200" s="14" t="s">
+        <v>289</v>
+      </c>
       <c r="B200" s="15">
         <v>17</v>
       </c>
@@ -5487,7 +5543,9 @@
       </c>
     </row>
     <row r="201" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A201" s="14"/>
+      <c r="A201" s="14" t="s">
+        <v>290</v>
+      </c>
       <c r="B201" s="15">
         <v>17</v>
       </c>
@@ -5503,7 +5561,9 @@
       </c>
     </row>
     <row r="202" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A202" s="14"/>
+      <c r="A202" s="14" t="s">
+        <v>291</v>
+      </c>
       <c r="B202" s="15">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Uploaded 07-May-2021 09:08:39 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -148,12 +148,6 @@
     <t>ADMISSIONS AND ACCOMMODATION_F</t>
   </si>
   <si>
-    <t>ICU AND ICU-RELATED CARE</t>
-  </si>
-  <si>
-    <t>ICU AND ICU-RELATED CARE_F</t>
-  </si>
-  <si>
     <t>GYM</t>
   </si>
   <si>
@@ -236,6 +230,76 @@
   </si>
   <si>
     <t>benefitName</t>
+  </si>
+  <si>
+    <t>RENAL CARE (DIALYSIS)</t>
+  </si>
+  <si>
+    <t>getBenefit_group().getName().equals("$param")</t>
+  </si>
+  <si>
+    <t>getBenefit_group().getCoveredDays()==$param</t>
+  </si>
+  <si>
+    <t>getName().equals("$param")</t>
+  </si>
+  <si>
+    <t>getValue().equals("$param")</t>
+  </si>
+  <si>
+    <t>$benefit: Benefit</t>
+  </si>
+  <si>
+    <t>$benefit.setCalculationResult($benefit.getCalculationResult()*$param);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getBenefit_group().getCoverageFrom().equals("$param")
+</t>
+  </si>
+  <si>
+    <t>1st Quarter</t>
+  </si>
+  <si>
+    <t>1 Week</t>
+  </si>
+  <si>
+    <t>2 Weeks</t>
+  </si>
+  <si>
+    <t>1 Month</t>
+  </si>
+  <si>
+    <t>2nd Quarter</t>
+  </si>
+  <si>
+    <t>3rd Quarter</t>
+  </si>
+  <si>
+    <t>4th Quarter</t>
+  </si>
+  <si>
+    <t>5th Quarter</t>
+  </si>
+  <si>
+    <t>6th Quarter</t>
+  </si>
+  <si>
+    <t>7th Quarter</t>
+  </si>
+  <si>
+    <t>8th Quarter</t>
+  </si>
+  <si>
+    <t>Lifetime Benefit</t>
+  </si>
+  <si>
+    <t>coverageFrom</t>
+  </si>
+  <si>
+    <t>INTENSIVE CARE</t>
+  </si>
+  <si>
+    <t>INTENSIVE CARE_F</t>
   </si>
   <si>
     <r>
@@ -249,660 +313,596 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>AssumptionUsedByGroupName</t>
+      <t>AssumptionUsedDecision</t>
     </r>
   </si>
   <si>
-    <t>AssumptionUsedByGroupName1</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName2</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName3</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName4</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName5</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName6</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName7</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName8</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName9</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName10</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName11</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName12</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName13</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName14</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName15</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName16</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName17</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName18</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName19</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName20</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName21</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName22</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName23</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName24</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName25</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName26</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName27</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName28</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName29</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName30</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName31</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName32</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName33</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName34</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName35</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName36</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName37</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName38</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName39</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName40</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName41</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName42</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName43</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName44</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName45</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName46</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName47</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName48</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName49</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName50</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName51</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName52</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName53</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName54</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName55</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName56</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName57</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName58</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName59</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName60</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName61</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName62</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName63</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName64</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName65</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName66</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName67</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName68</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName69</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName70</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName71</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName72</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName73</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName74</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName75</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName76</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName77</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName78</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName79</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName80</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName81</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName82</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName83</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName84</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName85</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName86</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName87</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName88</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName89</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName90</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName91</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName92</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName93</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName94</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName95</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName96</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName97</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName98</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName99</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName100</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName101</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName102</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName103</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName104</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName105</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName106</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName107</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName108</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName109</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName110</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName111</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName112</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName113</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName114</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName115</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName116</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName117</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName118</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName119</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName120</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName121</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName122</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName123</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName124</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName125</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName126</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName127</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName128</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName129</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName130</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName131</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName132</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName133</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName134</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName135</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName136</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName137</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName138</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName139</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName140</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName141</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName142</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName143</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName144</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName145</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName146</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName147</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName148</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName149</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName150</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName151</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName152</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName153</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName154</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName155</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName156</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName157</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName158</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName159</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName160</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName161</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName162</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName163</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName164</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName165</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName166</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName167</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName168</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName169</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName170</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName171</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName172</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName173</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName174</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName175</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName176</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName177</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName178</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName179</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName180</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName181</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName182</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName183</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName184</t>
-  </si>
-  <si>
-    <t>RENAL CARE (DIALYSIS)</t>
-  </si>
-  <si>
-    <t>getBenefit_group().getName().equals("$param")</t>
-  </si>
-  <si>
-    <t>getBenefit_group().getCoveredDays()==$param</t>
-  </si>
-  <si>
-    <t>getName().equals("$param")</t>
-  </si>
-  <si>
-    <t>getValue().equals("$param")</t>
-  </si>
-  <si>
-    <t>$benefit: Benefit</t>
-  </si>
-  <si>
-    <t>$benefit.setCalculationResult($benefit.getCalculationResult()*$param);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">getBenefit_group().getCoverageFrom().equals("$param")
-</t>
-  </si>
-  <si>
-    <t>1st Quarter</t>
-  </si>
-  <si>
-    <t>1 Week</t>
-  </si>
-  <si>
-    <t>2 Weeks</t>
-  </si>
-  <si>
-    <t>1 Month</t>
-  </si>
-  <si>
-    <t>2nd Quarter</t>
-  </si>
-  <si>
-    <t>3rd Quarter</t>
-  </si>
-  <si>
-    <t>4th Quarter</t>
-  </si>
-  <si>
-    <t>5th Quarter</t>
-  </si>
-  <si>
-    <t>6th Quarter</t>
-  </si>
-  <si>
-    <t>7th Quarter</t>
-  </si>
-  <si>
-    <t>8th Quarter</t>
-  </si>
-  <si>
-    <t>Lifetime Benefit</t>
-  </si>
-  <si>
-    <t>coverageFrom</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName185</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName186</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName187</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName188</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName189</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName190</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName191</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName192</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName193</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName194</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName195</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupName196</t>
+    <t>AssumptionUsedByGroupDecision1</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision2</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision3</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision4</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision5</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision6</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision7</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision8</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision9</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision10</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision11</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision12</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision13</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision14</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision15</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision16</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision17</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision18</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision19</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision20</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision21</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision22</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision23</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision24</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision25</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision26</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision27</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision28</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision29</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision30</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision31</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision32</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision33</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision34</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision35</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision36</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision37</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision38</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision39</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision40</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision41</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision42</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision43</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision44</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision45</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision46</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision47</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision48</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision49</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision50</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision51</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision52</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision53</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision54</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision55</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision56</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision57</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision58</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision59</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision60</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision61</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision62</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision63</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision64</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision65</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision66</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision67</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision68</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision69</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision70</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision71</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision72</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision73</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision74</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision75</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision76</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision77</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision78</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision79</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision80</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision81</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision82</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision83</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision84</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision85</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision86</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision87</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision88</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision89</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision90</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision91</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision92</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision93</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision94</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision95</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision96</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision97</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision98</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision99</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision100</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision101</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision102</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision103</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision104</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision105</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision106</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision107</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision108</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision109</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision110</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision111</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision112</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision113</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision114</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision115</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision116</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision117</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision118</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision119</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision120</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision121</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision122</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision123</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision124</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision125</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision126</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision127</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision128</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision129</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision130</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision131</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision132</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision133</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision134</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision135</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision136</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision137</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision138</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision139</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision140</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision141</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision142</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision143</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision144</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision145</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision146</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision147</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision148</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision149</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision150</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision151</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision152</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision153</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision154</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision155</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision156</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision157</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision158</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision159</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision160</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision161</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision162</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision163</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision164</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision165</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision166</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision167</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision168</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision169</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision170</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision171</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision172</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision173</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision174</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision175</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision176</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision177</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision178</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision179</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision180</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision181</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision182</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision183</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision184</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision185</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision186</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision187</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision188</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision189</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision190</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision191</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision192</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision193</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision194</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision195</t>
+  </si>
+  <si>
+    <t>AssumptionUsedByGroupDecision196</t>
   </si>
 </sst>
 </file>
@@ -1514,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A190" sqref="A190:A202"/>
+    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1591,7 +1591,7 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="27" t="s">
-        <v>264</v>
+        <v>77</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
@@ -1604,22 +1604,22 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>260</v>
+        <v>73</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>261</v>
+        <v>74</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>262</v>
+        <v>75</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>263</v>
+        <v>76</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>266</v>
+        <v>79</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>265</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -1633,16 +1633,16 @@
         <v>6</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>279</v>
+        <v>92</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>8</v>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="B7" s="15">
         <v>17</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="B8" s="15">
         <v>17</v>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B9" s="15">
         <v>17</v>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="B10" s="15">
         <v>17</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="B11" s="15">
         <v>17</v>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="B12" s="15">
         <v>17</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="B13" s="15">
         <v>17</v>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="B14" s="15">
         <v>17</v>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="B15" s="15">
         <v>17</v>
@@ -1830,7 +1830,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B16" s="15">
         <v>17</v>
@@ -1850,7 +1850,7 @@
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="B17" s="15">
         <v>17</v>
@@ -1870,7 +1870,7 @@
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="B18" s="15">
         <v>17</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="B19" s="15">
         <v>17</v>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="B20" s="15">
         <v>17</v>
@@ -1930,7 +1930,7 @@
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="B21" s="15">
         <v>17</v>
@@ -1950,7 +1950,7 @@
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="B22" s="15">
         <v>17</v>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="B23" s="15">
         <v>17</v>
@@ -1990,7 +1990,7 @@
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="B24" s="15">
         <v>17</v>
@@ -2010,7 +2010,7 @@
     </row>
     <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="B25" s="15">
         <v>17</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="B26" s="15">
         <v>17</v>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="B27" s="15">
         <v>17</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="B28" s="15">
         <v>17</v>
@@ -2090,7 +2090,7 @@
     </row>
     <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="B29" s="15">
         <v>17</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="B30" s="15">
         <v>17</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="B31" s="15">
         <v>17</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="B32" s="15">
         <v>17</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="B33" s="15">
         <v>17</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="B34" s="15">
         <v>17</v>
@@ -2210,7 +2210,7 @@
     </row>
     <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="B35" s="15">
         <v>17</v>
@@ -2230,7 +2230,7 @@
     </row>
     <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="B36" s="15">
         <v>17</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="B37" s="15">
         <v>17</v>
@@ -2270,7 +2270,7 @@
     </row>
     <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="B38" s="15">
         <v>17</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="B39" s="15">
         <v>17</v>
@@ -2310,7 +2310,7 @@
     </row>
     <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="B40" s="15">
         <v>17</v>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="B41" s="15">
         <v>17</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="B42" s="15">
         <v>17</v>
@@ -2370,7 +2370,7 @@
     </row>
     <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="B43" s="15">
         <v>17</v>
@@ -2390,7 +2390,7 @@
     </row>
     <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="B44" s="15">
         <v>17</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="B45" s="15">
         <v>17</v>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="B46" s="15">
         <v>17</v>
@@ -2450,7 +2450,7 @@
     </row>
     <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="B47" s="15">
         <v>17</v>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="B48" s="15">
         <v>17</v>
@@ -2490,7 +2490,7 @@
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="B49" s="15">
         <v>17</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="B50" s="15">
         <v>17</v>
@@ -2530,7 +2530,7 @@
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="B51" s="15">
         <v>17</v>
@@ -2550,7 +2550,7 @@
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="B52" s="15">
         <v>17</v>
@@ -2570,7 +2570,7 @@
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="B53" s="15">
         <v>17</v>
@@ -2590,7 +2590,7 @@
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="B54" s="15">
         <v>17</v>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="B55" s="15">
         <v>17</v>
@@ -2630,7 +2630,7 @@
     </row>
     <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="B56" s="15">
         <v>17</v>
@@ -2650,7 +2650,7 @@
     </row>
     <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="B57" s="15">
         <v>17</v>
@@ -2670,7 +2670,7 @@
     </row>
     <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="B58" s="15">
         <v>17</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="B59" s="15">
         <v>17</v>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="B60" s="15">
         <v>17</v>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="B61" s="15">
         <v>17</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="B62" s="15">
         <v>17</v>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="B63" s="15">
         <v>17</v>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="B64" s="15">
         <v>17</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="B65" s="15">
         <v>17</v>
@@ -2830,7 +2830,7 @@
     </row>
     <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="B66" s="15">
         <v>17</v>
@@ -2850,7 +2850,7 @@
     </row>
     <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="B67" s="15">
         <v>17</v>
@@ -2870,7 +2870,7 @@
     </row>
     <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B68" s="15">
         <v>17</v>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="B69" s="15">
         <v>17</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="B70" s="15">
         <v>17</v>
@@ -2930,7 +2930,7 @@
     </row>
     <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="B71" s="15">
         <v>17</v>
@@ -2950,7 +2950,7 @@
     </row>
     <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="B72" s="15">
         <v>17</v>
@@ -2970,7 +2970,7 @@
     </row>
     <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B73" s="15">
         <v>17</v>
@@ -2990,7 +2990,7 @@
     </row>
     <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="B74" s="15">
         <v>17</v>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="75" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="B75" s="15">
         <v>17</v>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="76" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="B76" s="15">
         <v>17</v>
@@ -3050,7 +3050,7 @@
     </row>
     <row r="77" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="B77" s="15">
         <v>17</v>
@@ -3070,7 +3070,7 @@
     </row>
     <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="B78" s="15">
         <v>17</v>
@@ -3090,13 +3090,13 @@
     </row>
     <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B79" s="15">
         <v>17</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="21"/>
@@ -3110,13 +3110,13 @@
     </row>
     <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="B80" s="15">
         <v>17</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="21"/>
@@ -3130,13 +3130,13 @@
     </row>
     <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="B81" s="15">
         <v>17</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="21"/>
@@ -3150,13 +3150,13 @@
     </row>
     <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="B82" s="15">
         <v>17</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="21"/>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="83" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="B83" s="15">
         <v>17</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="21"/>
@@ -3190,13 +3190,13 @@
     </row>
     <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="B84" s="15">
         <v>17</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="21"/>
@@ -3210,13 +3210,13 @@
     </row>
     <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="B85" s="15">
         <v>17</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21"/>
@@ -3230,13 +3230,13 @@
     </row>
     <row r="86" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="B86" s="15">
         <v>17</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="21"/>
@@ -3250,13 +3250,13 @@
     </row>
     <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="B87" s="15">
         <v>17</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D87" s="21"/>
       <c r="E87" s="21"/>
@@ -3270,13 +3270,13 @@
     </row>
     <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="B88" s="15">
         <v>17</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D88" s="21"/>
       <c r="E88" s="21"/>
@@ -3290,13 +3290,13 @@
     </row>
     <row r="89" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="B89" s="15">
         <v>17</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D89" s="21"/>
       <c r="E89" s="21"/>
@@ -3310,13 +3310,13 @@
     </row>
     <row r="90" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="B90" s="15">
         <v>17</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D90" s="21"/>
       <c r="E90" s="21"/>
@@ -3330,13 +3330,13 @@
     </row>
     <row r="91" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="B91" s="15">
         <v>17</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D91" s="21"/>
       <c r="E91" s="21"/>
@@ -3350,13 +3350,13 @@
     </row>
     <row r="92" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="B92" s="15">
         <v>17</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D92" s="21"/>
       <c r="E92" s="21"/>
@@ -3370,13 +3370,13 @@
     </row>
     <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="B93" s="15">
         <v>17</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D93" s="21"/>
       <c r="E93" s="21"/>
@@ -3390,13 +3390,13 @@
     </row>
     <row r="94" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="B94" s="15">
         <v>17</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D94" s="21"/>
       <c r="E94" s="21"/>
@@ -3410,13 +3410,13 @@
     </row>
     <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="B95" s="15">
         <v>17</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D95" s="21"/>
       <c r="E95" s="21"/>
@@ -3430,13 +3430,13 @@
     </row>
     <row r="96" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="B96" s="15">
         <v>17</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="D96" s="21"/>
       <c r="E96" s="21"/>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="B97" s="15">
         <v>17</v>
@@ -3470,7 +3470,7 @@
     </row>
     <row r="98" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="B98" s="15">
         <v>17</v>
@@ -3490,7 +3490,7 @@
     </row>
     <row r="99" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="B99" s="15">
         <v>17</v>
@@ -3510,7 +3510,7 @@
     </row>
     <row r="100" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="B100" s="15">
         <v>17</v>
@@ -3530,7 +3530,7 @@
     </row>
     <row r="101" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="B101" s="15">
         <v>17</v>
@@ -3550,7 +3550,7 @@
     </row>
     <row r="102" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="B102" s="15">
         <v>17</v>
@@ -3570,7 +3570,7 @@
     </row>
     <row r="103" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="B103" s="15">
         <v>17</v>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="104" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="B104" s="15">
         <v>17</v>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="105" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
       <c r="B105" s="15">
         <v>17</v>
@@ -3630,7 +3630,7 @@
     </row>
     <row r="106" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="B106" s="15">
         <v>17</v>
@@ -3650,7 +3650,7 @@
     </row>
     <row r="107" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="B107" s="15">
         <v>17</v>
@@ -3670,7 +3670,7 @@
     </row>
     <row r="108" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="B108" s="15">
         <v>17</v>
@@ -3690,7 +3690,7 @@
     </row>
     <row r="109" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="B109" s="15">
         <v>17</v>
@@ -3710,7 +3710,7 @@
     </row>
     <row r="110" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="B110" s="15">
         <v>17</v>
@@ -3730,7 +3730,7 @@
     </row>
     <row r="111" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="B111" s="15">
         <v>17</v>
@@ -3750,7 +3750,7 @@
     </row>
     <row r="112" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="B112" s="15">
         <v>17</v>
@@ -3770,7 +3770,7 @@
     </row>
     <row r="113" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="B113" s="15">
         <v>17</v>
@@ -3790,7 +3790,7 @@
     </row>
     <row r="114" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="B114" s="15">
         <v>17</v>
@@ -3810,7 +3810,7 @@
     </row>
     <row r="115" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="B115" s="15">
         <v>17</v>
@@ -3830,7 +3830,7 @@
     </row>
     <row r="116" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
       <c r="B116" s="15">
         <v>17</v>
@@ -3850,7 +3850,7 @@
     </row>
     <row r="117" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="B117" s="15">
         <v>17</v>
@@ -3870,7 +3870,7 @@
     </row>
     <row r="118" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
-        <v>186</v>
+        <v>207</v>
       </c>
       <c r="B118" s="15">
         <v>17</v>
@@ -3890,7 +3890,7 @@
     </row>
     <row r="119" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
       <c r="B119" s="15">
         <v>17</v>
@@ -3910,7 +3910,7 @@
     </row>
     <row r="120" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="B120" s="15">
         <v>17</v>
@@ -3930,7 +3930,7 @@
     </row>
     <row r="121" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="B121" s="15">
         <v>17</v>
@@ -3950,7 +3950,7 @@
     </row>
     <row r="122" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>190</v>
+        <v>211</v>
       </c>
       <c r="B122" s="15">
         <v>17</v>
@@ -3970,7 +3970,7 @@
     </row>
     <row r="123" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
       <c r="B123" s="15">
         <v>17</v>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="124" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="B124" s="15">
         <v>17</v>
@@ -4010,7 +4010,7 @@
     </row>
     <row r="125" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
-        <v>193</v>
+        <v>214</v>
       </c>
       <c r="B125" s="15">
         <v>17</v>
@@ -4030,7 +4030,7 @@
     </row>
     <row r="126" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="B126" s="15">
         <v>17</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="127" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
-        <v>195</v>
+        <v>216</v>
       </c>
       <c r="B127" s="15">
         <v>17</v>
@@ -4070,7 +4070,7 @@
     </row>
     <row r="128" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="B128" s="15">
         <v>17</v>
@@ -4090,7 +4090,7 @@
     </row>
     <row r="129" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="B129" s="15">
         <v>17</v>
@@ -4110,7 +4110,7 @@
     </row>
     <row r="130" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
       <c r="B130" s="15">
         <v>17</v>
@@ -4130,7 +4130,7 @@
     </row>
     <row r="131" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
-        <v>199</v>
+        <v>220</v>
       </c>
       <c r="B131" s="15">
         <v>17</v>
@@ -4150,7 +4150,7 @@
     </row>
     <row r="132" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="B132" s="15">
         <v>17</v>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="133" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
-        <v>201</v>
+        <v>222</v>
       </c>
       <c r="B133" s="15">
         <v>17</v>
@@ -4190,7 +4190,7 @@
     </row>
     <row r="134" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="B134" s="15">
         <v>17</v>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="135" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
-        <v>203</v>
+        <v>224</v>
       </c>
       <c r="B135" s="15">
         <v>17</v>
@@ -4230,7 +4230,7 @@
     </row>
     <row r="136" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
-        <v>204</v>
+        <v>225</v>
       </c>
       <c r="B136" s="15">
         <v>17</v>
@@ -4250,7 +4250,7 @@
     </row>
     <row r="137" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="B137" s="15">
         <v>17</v>
@@ -4270,7 +4270,7 @@
     </row>
     <row r="138" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="B138" s="15">
         <v>17</v>
@@ -4290,7 +4290,7 @@
     </row>
     <row r="139" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
-        <v>207</v>
+        <v>228</v>
       </c>
       <c r="B139" s="15">
         <v>17</v>
@@ -4310,13 +4310,13 @@
     </row>
     <row r="140" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
-        <v>208</v>
+        <v>229</v>
       </c>
       <c r="B140" s="15">
         <v>17</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D140" s="15"/>
       <c r="E140" s="21"/>
@@ -4330,13 +4330,13 @@
     </row>
     <row r="141" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>209</v>
+        <v>230</v>
       </c>
       <c r="B141" s="15">
         <v>17</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D141" s="15"/>
       <c r="E141" s="21"/>
@@ -4350,13 +4350,13 @@
     </row>
     <row r="142" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="B142" s="15">
         <v>17</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D142" s="15"/>
       <c r="E142" s="21"/>
@@ -4370,13 +4370,13 @@
     </row>
     <row r="143" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="B143" s="15">
         <v>17</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D143" s="15"/>
       <c r="E143" s="21"/>
@@ -4390,13 +4390,13 @@
     </row>
     <row r="144" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="B144" s="15">
         <v>17</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D144" s="15"/>
       <c r="E144" s="21"/>
@@ -4410,13 +4410,13 @@
     </row>
     <row r="145" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="B145" s="15">
         <v>17</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D145" s="15"/>
       <c r="E145" s="21"/>
@@ -4430,13 +4430,13 @@
     </row>
     <row r="146" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
       <c r="B146" s="15">
         <v>17</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D146" s="15"/>
       <c r="E146" s="21"/>
@@ -4450,13 +4450,13 @@
     </row>
     <row r="147" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="B147" s="15">
         <v>17</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D147" s="15"/>
       <c r="E147" s="21"/>
@@ -4470,13 +4470,13 @@
     </row>
     <row r="148" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
-        <v>216</v>
+        <v>237</v>
       </c>
       <c r="B148" s="15">
         <v>17</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D148" s="15"/>
       <c r="E148" s="21"/>
@@ -4490,13 +4490,13 @@
     </row>
     <row r="149" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
-        <v>217</v>
+        <v>238</v>
       </c>
       <c r="B149" s="15">
         <v>17</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D149" s="15"/>
       <c r="E149" s="21"/>
@@ -4510,13 +4510,13 @@
     </row>
     <row r="150" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="B150" s="15">
         <v>17</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D150" s="15"/>
       <c r="E150" s="21"/>
@@ -4530,13 +4530,13 @@
     </row>
     <row r="151" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
-        <v>219</v>
+        <v>240</v>
       </c>
       <c r="B151" s="15">
         <v>17</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D151" s="15"/>
       <c r="E151" s="21"/>
@@ -4550,13 +4550,13 @@
     </row>
     <row r="152" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
       <c r="B152" s="15">
         <v>17</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D152" s="15"/>
       <c r="E152" s="21"/>
@@ -4570,13 +4570,13 @@
     </row>
     <row r="153" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="B153" s="15">
         <v>17</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D153" s="15"/>
       <c r="E153" s="21"/>
@@ -4590,13 +4590,13 @@
     </row>
     <row r="154" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
       <c r="B154" s="15">
         <v>17</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D154" s="15"/>
       <c r="E154" s="21"/>
@@ -4610,13 +4610,13 @@
     </row>
     <row r="155" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
-        <v>223</v>
+        <v>244</v>
       </c>
       <c r="B155" s="15">
         <v>17</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D155" s="15"/>
       <c r="E155" s="21"/>
@@ -4630,13 +4630,13 @@
     </row>
     <row r="156" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
-        <v>224</v>
+        <v>245</v>
       </c>
       <c r="B156" s="15">
         <v>17</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D156" s="15"/>
       <c r="E156" s="21"/>
@@ -4650,13 +4650,13 @@
     </row>
     <row r="157" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
-        <v>225</v>
+        <v>246</v>
       </c>
       <c r="B157" s="15">
         <v>17</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D157" s="15"/>
       <c r="E157" s="21"/>
@@ -4670,13 +4670,13 @@
     </row>
     <row r="158" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
       <c r="B158" s="15">
         <v>17</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D158" s="15"/>
       <c r="E158" s="21"/>
@@ -4690,13 +4690,13 @@
     </row>
     <row r="159" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
-        <v>227</v>
+        <v>248</v>
       </c>
       <c r="B159" s="15">
         <v>17</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D159" s="15"/>
       <c r="E159" s="21"/>
@@ -4710,13 +4710,13 @@
     </row>
     <row r="160" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
       <c r="B160" s="15">
         <v>17</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D160" s="15"/>
       <c r="E160" s="21"/>
@@ -4730,13 +4730,13 @@
     </row>
     <row r="161" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
-        <v>229</v>
+        <v>250</v>
       </c>
       <c r="B161" s="15">
         <v>17</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D161" s="15"/>
       <c r="E161" s="21"/>
@@ -4750,13 +4750,13 @@
     </row>
     <row r="162" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
-        <v>230</v>
+        <v>251</v>
       </c>
       <c r="B162" s="15">
         <v>17</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D162" s="15"/>
       <c r="E162" s="21"/>
@@ -4770,13 +4770,13 @@
     </row>
     <row r="163" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="14" t="s">
-        <v>231</v>
+        <v>252</v>
       </c>
       <c r="B163" s="15">
         <v>17</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D163" s="15"/>
       <c r="E163" s="21"/>
@@ -4790,18 +4790,18 @@
     </row>
     <row r="164" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
-        <v>232</v>
+        <v>253</v>
       </c>
       <c r="B164" s="15">
         <v>17</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D164" s="19"/>
       <c r="E164" s="19"/>
       <c r="F164" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G164" s="19"/>
       <c r="H164" s="20">
@@ -4810,18 +4810,18 @@
     </row>
     <row r="165" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
-        <v>233</v>
+        <v>254</v>
       </c>
       <c r="B165" s="15">
         <v>17</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D165" s="19"/>
       <c r="E165" s="19"/>
       <c r="F165" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G165" s="19"/>
       <c r="H165" s="20">
@@ -4830,18 +4830,18 @@
     </row>
     <row r="166" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="14" t="s">
-        <v>234</v>
+        <v>255</v>
       </c>
       <c r="B166" s="15">
         <v>17</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D166" s="19"/>
       <c r="E166" s="19"/>
       <c r="F166" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G166" s="19"/>
       <c r="H166" s="20">
@@ -4850,18 +4850,18 @@
     </row>
     <row r="167" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="B167" s="15">
         <v>17</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D167" s="19"/>
       <c r="E167" s="19"/>
       <c r="F167" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G167" s="19"/>
       <c r="H167" s="20">
@@ -4870,18 +4870,18 @@
     </row>
     <row r="168" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="B168" s="15">
         <v>17</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D168" s="19"/>
       <c r="E168" s="19"/>
       <c r="F168" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G168" s="19"/>
       <c r="H168" s="20">
@@ -4890,18 +4890,18 @@
     </row>
     <row r="169" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
       <c r="B169" s="15">
         <v>17</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D169" s="19"/>
       <c r="E169" s="19"/>
       <c r="F169" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G169" s="19"/>
       <c r="H169" s="20">
@@ -4910,18 +4910,18 @@
     </row>
     <row r="170" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
-        <v>238</v>
+        <v>259</v>
       </c>
       <c r="B170" s="15">
         <v>17</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D170" s="19"/>
       <c r="E170" s="19"/>
       <c r="F170" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G170" s="19"/>
       <c r="H170" s="20">
@@ -4930,20 +4930,20 @@
     </row>
     <row r="171" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
-        <v>239</v>
+        <v>260</v>
       </c>
       <c r="B171" s="15">
         <v>17</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D171" s="15"/>
       <c r="E171" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F171" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G171" s="19"/>
       <c r="H171" s="20">
@@ -4952,20 +4952,20 @@
     </row>
     <row r="172" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="14" t="s">
-        <v>240</v>
+        <v>261</v>
       </c>
       <c r="B172" s="15">
         <v>17</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D172" s="15"/>
       <c r="E172" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F172" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G172" s="19"/>
       <c r="H172" s="20">
@@ -4974,20 +4974,20 @@
     </row>
     <row r="173" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="14" t="s">
-        <v>241</v>
+        <v>262</v>
       </c>
       <c r="B173" s="15">
         <v>17</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D173" s="15"/>
       <c r="E173" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F173" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G173" s="19"/>
       <c r="H173" s="20">
@@ -4996,20 +4996,20 @@
     </row>
     <row r="174" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="B174" s="15">
         <v>17</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D174" s="15"/>
       <c r="E174" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F174" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G174" s="19"/>
       <c r="H174" s="20">
@@ -5018,20 +5018,20 @@
     </row>
     <row r="175" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
-        <v>243</v>
+        <v>264</v>
       </c>
       <c r="B175" s="15">
         <v>17</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D175" s="15"/>
       <c r="E175" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F175" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G175" s="19"/>
       <c r="H175" s="20">
@@ -5040,20 +5040,20 @@
     </row>
     <row r="176" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
-        <v>244</v>
+        <v>265</v>
       </c>
       <c r="B176" s="15">
         <v>17</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D176" s="15"/>
       <c r="E176" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F176" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G176" s="19"/>
       <c r="H176" s="20">
@@ -5062,20 +5062,20 @@
     </row>
     <row r="177" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
-        <v>245</v>
+        <v>266</v>
       </c>
       <c r="B177" s="15">
         <v>17</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D177" s="15"/>
       <c r="E177" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F177" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G177" s="19"/>
       <c r="H177" s="20">
@@ -5084,20 +5084,20 @@
     </row>
     <row r="178" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="B178" s="15">
         <v>17</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F178" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G178" s="19"/>
       <c r="H178" s="20">
@@ -5106,20 +5106,20 @@
     </row>
     <row r="179" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
-        <v>247</v>
+        <v>268</v>
       </c>
       <c r="B179" s="15">
         <v>17</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F179" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G179" s="19"/>
       <c r="H179" s="20">
@@ -5128,20 +5128,20 @@
     </row>
     <row r="180" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="14" t="s">
-        <v>248</v>
+        <v>269</v>
       </c>
       <c r="B180" s="15">
         <v>17</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D180" s="15"/>
       <c r="E180" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F180" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G180" s="19"/>
       <c r="H180" s="20">
@@ -5150,20 +5150,20 @@
     </row>
     <row r="181" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="14" t="s">
-        <v>249</v>
+        <v>270</v>
       </c>
       <c r="B181" s="15">
         <v>17</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D181" s="15"/>
       <c r="E181" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F181" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G181" s="19"/>
       <c r="H181" s="20">
@@ -5172,20 +5172,20 @@
     </row>
     <row r="182" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="14" t="s">
-        <v>250</v>
+        <v>271</v>
       </c>
       <c r="B182" s="15">
         <v>17</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D182" s="15"/>
       <c r="E182" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F182" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G182" s="19"/>
       <c r="H182" s="20">
@@ -5194,20 +5194,20 @@
     </row>
     <row r="183" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
-        <v>251</v>
+        <v>272</v>
       </c>
       <c r="B183" s="15">
         <v>17</v>
       </c>
       <c r="C183" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D183" s="15"/>
       <c r="E183" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F183" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G183" s="19"/>
       <c r="H183" s="20">
@@ -5216,20 +5216,20 @@
     </row>
     <row r="184" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="14" t="s">
-        <v>252</v>
+        <v>273</v>
       </c>
       <c r="B184" s="15">
         <v>17</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D184" s="15"/>
       <c r="E184" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F184" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G184" s="19"/>
       <c r="H184" s="20">
@@ -5238,18 +5238,18 @@
     </row>
     <row r="185" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="14" t="s">
-        <v>253</v>
+        <v>274</v>
       </c>
       <c r="B185" s="15">
         <v>17</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D185" s="22"/>
       <c r="E185" s="15"/>
       <c r="F185" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G185" s="22"/>
       <c r="H185" s="23">
@@ -5258,18 +5258,18 @@
     </row>
     <row r="186" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
-        <v>254</v>
+        <v>275</v>
       </c>
       <c r="B186" s="15">
         <v>17</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D186" s="22"/>
       <c r="E186" s="15"/>
       <c r="F186" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G186" s="22"/>
       <c r="H186" s="23">
@@ -5278,18 +5278,18 @@
     </row>
     <row r="187" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
-        <v>255</v>
+        <v>276</v>
       </c>
       <c r="B187" s="15">
         <v>17</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D187" s="22"/>
       <c r="E187" s="15"/>
       <c r="F187" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G187" s="22"/>
       <c r="H187" s="23">
@@ -5298,7 +5298,7 @@
     </row>
     <row r="188" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
-        <v>256</v>
+        <v>277</v>
       </c>
       <c r="B188" s="15">
         <v>17</v>
@@ -5308,10 +5308,10 @@
       </c>
       <c r="D188" s="15"/>
       <c r="E188" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F188" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G188" s="22"/>
       <c r="H188" s="23">
@@ -5320,7 +5320,7 @@
     </row>
     <row r="189" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
-        <v>257</v>
+        <v>278</v>
       </c>
       <c r="B189" s="15">
         <v>17</v>
@@ -5330,10 +5330,10 @@
       </c>
       <c r="D189" s="15"/>
       <c r="E189" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F189" s="22" t="s">
         <v>68</v>
-      </c>
-      <c r="F189" s="22" t="s">
-        <v>70</v>
       </c>
       <c r="G189" s="22"/>
       <c r="H189" s="23">
@@ -5342,7 +5342,7 @@
     </row>
     <row r="190" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
-        <v>258</v>
+        <v>279</v>
       </c>
       <c r="B190" s="15">
         <v>17</v>
@@ -5352,10 +5352,10 @@
       </c>
       <c r="D190" s="15"/>
       <c r="E190" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F190" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G190" s="22"/>
       <c r="H190" s="23">
@@ -5374,7 +5374,7 @@
       <c r="E191" s="15"/>
       <c r="F191" s="14"/>
       <c r="G191" s="24" t="s">
-        <v>267</v>
+        <v>80</v>
       </c>
       <c r="H191" s="25">
         <v>1</v>
@@ -5392,7 +5392,7 @@
       <c r="E192" s="15"/>
       <c r="F192" s="14"/>
       <c r="G192" s="24" t="s">
-        <v>268</v>
+        <v>81</v>
       </c>
       <c r="H192" s="25">
         <v>0.99039999999999995</v>
@@ -5410,7 +5410,7 @@
       <c r="E193" s="15"/>
       <c r="F193" s="14"/>
       <c r="G193" s="24" t="s">
-        <v>269</v>
+        <v>82</v>
       </c>
       <c r="H193" s="25">
         <v>0.97119999999999995</v>
@@ -5428,7 +5428,7 @@
       <c r="E194" s="15"/>
       <c r="F194" s="14"/>
       <c r="G194" s="24" t="s">
-        <v>270</v>
+        <v>83</v>
       </c>
       <c r="H194" s="25">
         <v>0.95830000000000004</v>
@@ -5446,7 +5446,7 @@
       <c r="E195" s="15"/>
       <c r="F195" s="14"/>
       <c r="G195" s="24" t="s">
-        <v>271</v>
+        <v>84</v>
       </c>
       <c r="H195" s="25">
         <v>0.88</v>
@@ -5464,7 +5464,7 @@
       <c r="E196" s="15"/>
       <c r="F196" s="14"/>
       <c r="G196" s="24" t="s">
-        <v>272</v>
+        <v>85</v>
       </c>
       <c r="H196" s="25">
         <v>0.74</v>
@@ -5482,7 +5482,7 @@
       <c r="E197" s="15"/>
       <c r="F197" s="14"/>
       <c r="G197" s="24" t="s">
-        <v>273</v>
+        <v>86</v>
       </c>
       <c r="H197" s="25">
         <v>0.5</v>
@@ -5500,7 +5500,7 @@
       <c r="E198" s="15"/>
       <c r="F198" s="14"/>
       <c r="G198" s="24" t="s">
-        <v>274</v>
+        <v>87</v>
       </c>
       <c r="H198" s="25">
         <v>0.4</v>
@@ -5518,7 +5518,7 @@
       <c r="E199" s="15"/>
       <c r="F199" s="14"/>
       <c r="G199" s="24" t="s">
-        <v>275</v>
+        <v>88</v>
       </c>
       <c r="H199" s="25">
         <v>0.3</v>
@@ -5536,7 +5536,7 @@
       <c r="E200" s="15"/>
       <c r="F200" s="14"/>
       <c r="G200" s="24" t="s">
-        <v>276</v>
+        <v>89</v>
       </c>
       <c r="H200" s="25">
         <v>0.2</v>
@@ -5554,7 +5554,7 @@
       <c r="E201" s="15"/>
       <c r="F201" s="14"/>
       <c r="G201" s="24" t="s">
-        <v>277</v>
+        <v>90</v>
       </c>
       <c r="H201" s="25">
         <v>0.18</v>
@@ -5572,7 +5572,7 @@
       <c r="E202" s="15"/>
       <c r="F202" s="14"/>
       <c r="G202" s="24" t="s">
-        <v>278</v>
+        <v>91</v>
       </c>
       <c r="H202" s="25">
         <v>0.16669999999999999</v>

</xml_diff>

<commit_message>
Uploaded 07-May-2021 09:12:31 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -317,592 +317,592 @@
     </r>
   </si>
   <si>
-    <t>AssumptionUsedByGroupDecision1</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision2</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision3</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision4</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision5</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision6</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision7</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision8</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision9</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision10</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision11</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision12</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision13</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision14</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision15</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision16</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision17</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision18</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision19</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision20</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision21</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision22</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision23</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision24</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision25</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision26</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision27</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision28</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision29</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision30</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision31</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision32</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision33</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision34</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision35</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision36</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision37</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision38</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision39</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision40</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision41</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision42</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision43</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision44</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision45</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision46</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision47</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision48</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision49</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision50</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision51</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision52</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision53</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision54</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision55</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision56</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision57</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision58</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision59</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision60</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision61</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision62</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision63</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision64</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision65</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision66</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision67</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision68</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision69</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision70</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision71</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision72</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision73</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision74</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision75</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision76</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision77</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision78</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision79</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision80</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision81</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision82</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision83</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision84</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision85</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision86</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision87</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision88</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision89</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision90</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision91</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision92</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision93</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision94</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision95</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision96</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision97</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision98</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision99</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision100</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision101</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision102</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision103</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision104</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision105</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision106</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision107</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision108</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision109</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision110</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision111</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision112</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision113</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision114</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision115</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision116</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision117</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision118</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision119</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision120</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision121</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision122</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision123</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision124</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision125</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision126</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision127</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision128</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision129</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision130</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision131</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision132</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision133</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision134</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision135</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision136</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision137</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision138</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision139</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision140</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision141</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision142</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision143</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision144</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision145</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision146</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision147</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision148</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision149</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision150</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision151</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision152</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision153</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision154</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision155</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision156</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision157</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision158</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision159</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision160</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision161</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision162</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision163</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision164</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision165</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision166</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision167</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision168</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision169</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision170</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision171</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision172</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision173</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision174</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision175</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision176</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision177</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision178</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision179</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision180</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision181</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision182</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision183</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision184</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision185</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision186</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision187</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision188</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision189</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision190</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision191</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision192</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision193</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision194</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision195</t>
-  </si>
-  <si>
-    <t>AssumptionUsedByGroupDecision196</t>
+    <t>AssumptionUsedDecision1</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision2</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision3</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision4</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision5</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision6</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision7</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision8</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision9</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision10</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision11</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision12</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision13</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision14</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision15</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision16</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision17</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision18</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision19</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision20</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision21</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision22</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision23</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision24</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision25</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision26</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision27</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision28</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision29</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision30</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision31</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision32</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision33</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision34</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision35</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision36</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision37</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision38</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision39</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision40</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision41</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision42</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision43</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision44</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision45</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision46</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision47</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision48</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision49</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision50</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision51</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision52</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision53</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision54</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision55</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision56</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision57</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision58</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision59</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision60</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision61</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision62</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision63</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision64</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision65</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision66</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision67</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision68</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision69</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision70</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision71</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision72</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision73</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision74</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision75</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision76</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision77</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision78</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision79</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision80</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision81</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision82</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision83</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision84</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision85</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision86</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision87</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision88</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision89</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision90</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision91</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision92</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision93</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision94</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision95</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision96</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision97</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision98</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision99</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision100</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision101</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision102</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision103</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision104</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision105</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision106</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision107</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision108</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision109</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision110</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision111</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision112</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision113</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision114</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision115</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision116</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision117</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision118</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision119</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision120</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision121</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision122</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision123</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision124</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision125</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision126</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision127</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision128</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision129</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision130</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision131</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision132</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision133</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision134</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision135</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision136</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision137</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision138</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision139</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision140</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision141</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision142</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision143</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision144</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision145</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision146</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision147</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision148</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision149</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision150</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision151</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision152</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision153</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision154</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision155</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision156</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision157</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision158</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision159</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision160</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision161</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision162</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision163</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision164</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision165</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision166</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision167</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision168</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision169</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision170</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision171</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision172</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision173</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision174</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision175</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision176</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision177</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision178</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision179</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision180</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision181</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision182</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision183</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision184</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision185</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision186</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision187</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision188</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision189</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision190</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision191</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision192</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision193</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision194</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision195</t>
+  </si>
+  <si>
+    <t>AssumptionUsedDecision196</t>
   </si>
 </sst>
 </file>
@@ -1514,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A202"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A204" sqref="A204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Uploaded 07-May-2021 14:51:32 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="292">
   <si>
     <t>RuleSet</t>
   </si>
@@ -1131,9 +1131,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1142,6 +1139,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1514,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A204" sqref="A204"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1537,27 +1537,27 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -1590,13 +1590,21 @@
     <row r="4" spans="1:12" ht="25.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
+      <c r="D4" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>77</v>
+      </c>
       <c r="H4" s="8"/>
       <c r="L4" s="3"/>
     </row>
@@ -14739,10 +14747,9 @@
       <c r="H1118" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="C4:G4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploaded 07-May-2021 15:35:51 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="294">
   <si>
     <t>RuleSet</t>
   </si>
@@ -1524,7 +1524,7 @@
   <dimension ref="A1:M1118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1579,7 +1579,9 @@
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Uploaded 07-May-2021 15:44:50 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="295">
   <si>
     <t>RuleSet</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>RENAL CARE (DIALYSIS)</t>
+  </si>
+  <si>
+    <t>getBenefit_group().getName().equals("$param")</t>
   </si>
   <si>
     <t>$benefit: Benefit</t>
@@ -895,9 +898,6 @@
     <t>benefit</t>
   </si>
   <si>
-    <t>$benefit.getBenefit_group().getName().equals("$param")</t>
-  </si>
-  <si>
     <t>$benefit.getBenefit_group().getCoveredDays()==$param</t>
   </si>
   <si>
@@ -909,6 +909,9 @@
   <si>
     <t xml:space="preserve">$benefit.getBenefit_group().getCoverageFrom().equals("$param")
 </t>
+  </si>
+  <si>
+    <t>$benefit</t>
   </si>
 </sst>
 </file>
@@ -1523,15 +1526,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.42578125" style="17"/>
     <col min="2" max="2" width="12.140625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="17"/>
+    <col min="3" max="3" width="14.42578125" style="17" customWidth="1"/>
     <col min="4" max="5" width="41" style="17" customWidth="1"/>
     <col min="6" max="6" width="36.140625" style="17" customWidth="1"/>
     <col min="7" max="8" width="25.140625" style="17" customWidth="1"/>
@@ -1560,7 +1563,7 @@
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -1606,9 +1609,11 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="26"/>
+        <v>74</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>294</v>
+      </c>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
@@ -1620,10 +1625,10 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>289</v>
+        <v>73</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>290</v>
@@ -1638,7 +1643,7 @@
         <v>293</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -1649,7 +1654,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>6</v>
@@ -1664,7 +1669,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>8</v>
@@ -1672,13 +1677,13 @@
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B7" s="15">
         <v>17</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>9</v>
@@ -1695,13 +1700,13 @@
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B8" s="15">
         <v>17</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>9</v>
@@ -1718,13 +1723,13 @@
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B9" s="15">
         <v>17</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>9</v>
@@ -1741,13 +1746,13 @@
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B10" s="15">
         <v>17</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>9</v>
@@ -1764,13 +1769,13 @@
     </row>
     <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B11" s="15">
         <v>17</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>9</v>
@@ -1787,13 +1792,13 @@
     </row>
     <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B12" s="15">
         <v>17</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>9</v>
@@ -1810,13 +1815,13 @@
     </row>
     <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B13" s="15">
         <v>17</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>9</v>
@@ -1833,13 +1838,13 @@
     </row>
     <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B14" s="15">
         <v>17</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>9</v>
@@ -1856,13 +1861,13 @@
     </row>
     <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B15" s="15">
         <v>17</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>9</v>
@@ -1879,13 +1884,13 @@
     </row>
     <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B16" s="15">
         <v>17</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>9</v>
@@ -1902,13 +1907,13 @@
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B17" s="15">
         <v>17</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>9</v>
@@ -1925,13 +1930,13 @@
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B18" s="15">
         <v>17</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>9</v>
@@ -1948,13 +1953,13 @@
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19" s="15">
         <v>17</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>9</v>
@@ -1971,13 +1976,13 @@
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B20" s="15">
         <v>17</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>9</v>
@@ -1994,13 +1999,13 @@
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B21" s="15">
         <v>17</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>9</v>
@@ -2017,13 +2022,13 @@
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B22" s="15">
         <v>17</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>9</v>
@@ -2040,13 +2045,13 @@
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B23" s="15">
         <v>17</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>9</v>
@@ -2063,13 +2068,13 @@
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B24" s="15">
         <v>17</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>9</v>
@@ -2086,13 +2091,13 @@
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B25" s="15">
         <v>17</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>28</v>
@@ -2109,13 +2114,13 @@
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B26" s="15">
         <v>17</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>28</v>
@@ -2132,13 +2137,13 @@
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B27" s="15">
         <v>17</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>28</v>
@@ -2155,13 +2160,13 @@
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B28" s="15">
         <v>17</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>28</v>
@@ -2178,13 +2183,13 @@
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B29" s="15">
         <v>17</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>28</v>
@@ -2201,13 +2206,13 @@
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B30" s="15">
         <v>17</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>28</v>
@@ -2224,13 +2229,13 @@
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B31" s="15">
         <v>17</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>28</v>
@@ -2247,13 +2252,13 @@
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B32" s="15">
         <v>17</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>28</v>
@@ -2270,13 +2275,13 @@
     </row>
     <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B33" s="15">
         <v>17</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>28</v>
@@ -2293,13 +2298,13 @@
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B34" s="15">
         <v>17</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>28</v>
@@ -2316,13 +2321,13 @@
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B35" s="15">
         <v>17</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>28</v>
@@ -2339,13 +2344,13 @@
     </row>
     <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B36" s="15">
         <v>17</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>28</v>
@@ -2362,13 +2367,13 @@
     </row>
     <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B37" s="15">
         <v>17</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>28</v>
@@ -2385,13 +2390,13 @@
     </row>
     <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B38" s="15">
         <v>17</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>28</v>
@@ -2408,13 +2413,13 @@
     </row>
     <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B39" s="15">
         <v>17</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>28</v>
@@ -2431,13 +2436,13 @@
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B40" s="15">
         <v>17</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>28</v>
@@ -2454,13 +2459,13 @@
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B41" s="15">
         <v>17</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>28</v>
@@ -2477,13 +2482,13 @@
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B42" s="15">
         <v>17</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>28</v>
@@ -2500,13 +2505,13 @@
     </row>
     <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B43" s="15">
         <v>17</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>29</v>
@@ -2523,13 +2528,13 @@
     </row>
     <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B44" s="15">
         <v>17</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>29</v>
@@ -2546,13 +2551,13 @@
     </row>
     <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B45" s="15">
         <v>17</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>29</v>
@@ -2569,13 +2574,13 @@
     </row>
     <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B46" s="15">
         <v>17</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>29</v>
@@ -2592,13 +2597,13 @@
     </row>
     <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B47" s="15">
         <v>17</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D47" s="15" t="s">
         <v>29</v>
@@ -2615,13 +2620,13 @@
     </row>
     <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B48" s="15">
         <v>17</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>29</v>
@@ -2638,13 +2643,13 @@
     </row>
     <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B49" s="15">
         <v>17</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>29</v>
@@ -2661,13 +2666,13 @@
     </row>
     <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B50" s="15">
         <v>17</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>29</v>
@@ -2684,13 +2689,13 @@
     </row>
     <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B51" s="15">
         <v>17</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>29</v>
@@ -2707,13 +2712,13 @@
     </row>
     <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B52" s="15">
         <v>17</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D52" s="15" t="s">
         <v>29</v>
@@ -2730,13 +2735,13 @@
     </row>
     <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B53" s="15">
         <v>17</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>29</v>
@@ -2753,13 +2758,13 @@
     </row>
     <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B54" s="15">
         <v>17</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>29</v>
@@ -2776,13 +2781,13 @@
     </row>
     <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B55" s="15">
         <v>17</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>29</v>
@@ -2799,13 +2804,13 @@
     </row>
     <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B56" s="15">
         <v>17</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>29</v>
@@ -2822,13 +2827,13 @@
     </row>
     <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B57" s="15">
         <v>17</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>29</v>
@@ -2845,13 +2850,13 @@
     </row>
     <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B58" s="15">
         <v>17</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D58" s="15" t="s">
         <v>29</v>
@@ -2868,13 +2873,13 @@
     </row>
     <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B59" s="15">
         <v>17</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D59" s="15" t="s">
         <v>29</v>
@@ -2891,13 +2896,13 @@
     </row>
     <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B60" s="15">
         <v>17</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D60" s="15" t="s">
         <v>29</v>
@@ -2914,13 +2919,13 @@
     </row>
     <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B61" s="15">
         <v>17</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D61" s="15" t="s">
         <v>30</v>
@@ -2937,13 +2942,13 @@
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B62" s="15">
         <v>17</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D62" s="15" t="s">
         <v>30</v>
@@ -2960,13 +2965,13 @@
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B63" s="15">
         <v>17</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D63" s="15" t="s">
         <v>30</v>
@@ -2983,13 +2988,13 @@
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B64" s="15">
         <v>17</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>30</v>
@@ -3006,13 +3011,13 @@
     </row>
     <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B65" s="15">
         <v>17</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D65" s="15" t="s">
         <v>30</v>
@@ -3029,13 +3034,13 @@
     </row>
     <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B66" s="15">
         <v>17</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D66" s="15" t="s">
         <v>30</v>
@@ -3052,13 +3057,13 @@
     </row>
     <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B67" s="15">
         <v>17</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D67" s="15" t="s">
         <v>30</v>
@@ -3075,13 +3080,13 @@
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B68" s="15">
         <v>17</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D68" s="15" t="s">
         <v>30</v>
@@ -3098,13 +3103,13 @@
     </row>
     <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B69" s="15">
         <v>17</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D69" s="15" t="s">
         <v>30</v>
@@ -3121,13 +3126,13 @@
     </row>
     <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B70" s="15">
         <v>17</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D70" s="15" t="s">
         <v>30</v>
@@ -3144,13 +3149,13 @@
     </row>
     <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B71" s="15">
         <v>17</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D71" s="15" t="s">
         <v>30</v>
@@ -3167,13 +3172,13 @@
     </row>
     <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B72" s="15">
         <v>17</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D72" s="15" t="s">
         <v>30</v>
@@ -3190,13 +3195,13 @@
     </row>
     <row r="73" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B73" s="15">
         <v>17</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D73" s="15" t="s">
         <v>30</v>
@@ -3213,13 +3218,13 @@
     </row>
     <row r="74" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B74" s="15">
         <v>17</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D74" s="15" t="s">
         <v>30</v>
@@ -3236,13 +3241,13 @@
     </row>
     <row r="75" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B75" s="15">
         <v>17</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D75" s="15" t="s">
         <v>30</v>
@@ -3259,13 +3264,13 @@
     </row>
     <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B76" s="15">
         <v>17</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D76" s="15" t="s">
         <v>30</v>
@@ -3282,13 +3287,13 @@
     </row>
     <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B77" s="15">
         <v>17</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D77" s="15" t="s">
         <v>30</v>
@@ -3305,13 +3310,13 @@
     </row>
     <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B78" s="15">
         <v>17</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D78" s="15" t="s">
         <v>30</v>
@@ -3328,13 +3333,13 @@
     </row>
     <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B79" s="15">
         <v>17</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D79" s="15" t="s">
         <v>72</v>
@@ -3351,13 +3356,13 @@
     </row>
     <row r="80" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B80" s="15">
         <v>17</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D80" s="15" t="s">
         <v>72</v>
@@ -3374,13 +3379,13 @@
     </row>
     <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B81" s="15">
         <v>17</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D81" s="15" t="s">
         <v>72</v>
@@ -3397,13 +3402,13 @@
     </row>
     <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B82" s="15">
         <v>17</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D82" s="15" t="s">
         <v>72</v>
@@ -3420,13 +3425,13 @@
     </row>
     <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B83" s="15">
         <v>17</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D83" s="15" t="s">
         <v>72</v>
@@ -3443,13 +3448,13 @@
     </row>
     <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B84" s="15">
         <v>17</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D84" s="15" t="s">
         <v>72</v>
@@ -3466,13 +3471,13 @@
     </row>
     <row r="85" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B85" s="15">
         <v>17</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D85" s="15" t="s">
         <v>72</v>
@@ -3489,13 +3494,13 @@
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B86" s="15">
         <v>17</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D86" s="15" t="s">
         <v>72</v>
@@ -3512,13 +3517,13 @@
     </row>
     <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B87" s="15">
         <v>17</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D87" s="15" t="s">
         <v>72</v>
@@ -3535,13 +3540,13 @@
     </row>
     <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B88" s="15">
         <v>17</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D88" s="15" t="s">
         <v>72</v>
@@ -3558,13 +3563,13 @@
     </row>
     <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B89" s="15">
         <v>17</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D89" s="15" t="s">
         <v>72</v>
@@ -3581,13 +3586,13 @@
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B90" s="15">
         <v>17</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D90" s="15" t="s">
         <v>72</v>
@@ -3604,13 +3609,13 @@
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B91" s="15">
         <v>17</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D91" s="15" t="s">
         <v>72</v>
@@ -3627,13 +3632,13 @@
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B92" s="15">
         <v>17</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>72</v>
@@ -3650,13 +3655,13 @@
     </row>
     <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B93" s="15">
         <v>17</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D93" s="15" t="s">
         <v>72</v>
@@ -3673,13 +3678,13 @@
     </row>
     <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B94" s="15">
         <v>17</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D94" s="15" t="s">
         <v>72</v>
@@ -3696,13 +3701,13 @@
     </row>
     <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B95" s="15">
         <v>17</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D95" s="15" t="s">
         <v>72</v>
@@ -3719,13 +3724,13 @@
     </row>
     <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B96" s="15">
         <v>17</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D96" s="15" t="s">
         <v>72</v>
@@ -3742,13 +3747,13 @@
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B97" s="15">
         <v>17</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D97" s="15" t="s">
         <v>31</v>
@@ -3765,13 +3770,13 @@
     </row>
     <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B98" s="15">
         <v>17</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D98" s="15" t="s">
         <v>31</v>
@@ -3788,13 +3793,13 @@
     </row>
     <row r="99" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B99" s="15">
         <v>17</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D99" s="15" t="s">
         <v>31</v>
@@ -3811,13 +3816,13 @@
     </row>
     <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B100" s="15">
         <v>17</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D100" s="15" t="s">
         <v>31</v>
@@ -3834,13 +3839,13 @@
     </row>
     <row r="101" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B101" s="15">
         <v>17</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D101" s="15" t="s">
         <v>31</v>
@@ -3857,13 +3862,13 @@
     </row>
     <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B102" s="15">
         <v>17</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D102" s="15" t="s">
         <v>31</v>
@@ -3880,13 +3885,13 @@
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B103" s="15">
         <v>17</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D103" s="15" t="s">
         <v>31</v>
@@ -3903,13 +3908,13 @@
     </row>
     <row r="104" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B104" s="15">
         <v>17</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D104" s="15" t="s">
         <v>31</v>
@@ -3926,13 +3931,13 @@
     </row>
     <row r="105" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B105" s="15">
         <v>17</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D105" s="15" t="s">
         <v>31</v>
@@ -3949,13 +3954,13 @@
     </row>
     <row r="106" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B106" s="15">
         <v>17</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D106" s="15" t="s">
         <v>31</v>
@@ -3972,13 +3977,13 @@
     </row>
     <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B107" s="15">
         <v>17</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D107" s="15" t="s">
         <v>31</v>
@@ -3995,13 +4000,13 @@
     </row>
     <row r="108" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B108" s="15">
         <v>17</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D108" s="15" t="s">
         <v>31</v>
@@ -4018,13 +4023,13 @@
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B109" s="15">
         <v>17</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D109" s="15" t="s">
         <v>31</v>
@@ -4041,13 +4046,13 @@
     </row>
     <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B110" s="15">
         <v>17</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D110" s="15" t="s">
         <v>31</v>
@@ -4064,13 +4069,13 @@
     </row>
     <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B111" s="15">
         <v>17</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D111" s="15" t="s">
         <v>31</v>
@@ -4087,13 +4092,13 @@
     </row>
     <row r="112" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B112" s="15">
         <v>17</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D112" s="15" t="s">
         <v>31</v>
@@ -4110,13 +4115,13 @@
     </row>
     <row r="113" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B113" s="15">
         <v>17</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D113" s="15" t="s">
         <v>31</v>
@@ -4133,13 +4138,13 @@
     </row>
     <row r="114" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B114" s="15">
         <v>17</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D114" s="15" t="s">
         <v>31</v>
@@ -4156,13 +4161,13 @@
     </row>
     <row r="115" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B115" s="15">
         <v>17</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D115" s="15" t="s">
         <v>31</v>
@@ -4179,13 +4184,13 @@
     </row>
     <row r="116" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B116" s="15">
         <v>17</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D116" s="15" t="s">
         <v>31</v>
@@ -4202,13 +4207,13 @@
     </row>
     <row r="117" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B117" s="15">
         <v>17</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D117" s="15" t="s">
         <v>31</v>
@@ -4225,13 +4230,13 @@
     </row>
     <row r="118" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B118" s="15">
         <v>17</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D118" s="15" t="s">
         <v>31</v>
@@ -4248,13 +4253,13 @@
     </row>
     <row r="119" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B119" s="15">
         <v>17</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D119" s="15" t="s">
         <v>31</v>
@@ -4271,13 +4276,13 @@
     </row>
     <row r="120" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B120" s="15">
         <v>17</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D120" s="15" t="s">
         <v>31</v>
@@ -4294,13 +4299,13 @@
     </row>
     <row r="121" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B121" s="15">
         <v>17</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D121" s="15" t="s">
         <v>31</v>
@@ -4317,13 +4322,13 @@
     </row>
     <row r="122" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B122" s="15">
         <v>17</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D122" s="15" t="s">
         <v>31</v>
@@ -4340,13 +4345,13 @@
     </row>
     <row r="123" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B123" s="15">
         <v>17</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D123" s="15" t="s">
         <v>31</v>
@@ -4363,13 +4368,13 @@
     </row>
     <row r="124" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B124" s="15">
         <v>17</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D124" s="15" t="s">
         <v>31</v>
@@ -4386,13 +4391,13 @@
     </row>
     <row r="125" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B125" s="15">
         <v>17</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D125" s="15" t="s">
         <v>31</v>
@@ -4409,13 +4414,13 @@
     </row>
     <row r="126" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B126" s="15">
         <v>17</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D126" s="15" t="s">
         <v>31</v>
@@ -4432,13 +4437,13 @@
     </row>
     <row r="127" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B127" s="15">
         <v>17</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D127" s="15" t="s">
         <v>31</v>
@@ -4455,13 +4460,13 @@
     </row>
     <row r="128" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B128" s="15">
         <v>17</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D128" s="15" t="s">
         <v>43</v>
@@ -4478,13 +4483,13 @@
     </row>
     <row r="129" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B129" s="15">
         <v>17</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D129" s="15" t="s">
         <v>43</v>
@@ -4501,13 +4506,13 @@
     </row>
     <row r="130" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B130" s="15">
         <v>17</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D130" s="15" t="s">
         <v>43</v>
@@ -4524,13 +4529,13 @@
     </row>
     <row r="131" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B131" s="15">
         <v>17</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D131" s="15" t="s">
         <v>43</v>
@@ -4547,13 +4552,13 @@
     </row>
     <row r="132" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B132" s="15">
         <v>17</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D132" s="15" t="s">
         <v>43</v>
@@ -4570,13 +4575,13 @@
     </row>
     <row r="133" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B133" s="15">
         <v>17</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D133" s="15" t="s">
         <v>43</v>
@@ -4593,13 +4598,13 @@
     </row>
     <row r="134" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B134" s="15">
         <v>17</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D134" s="15" t="s">
         <v>43</v>
@@ -4616,13 +4621,13 @@
     </row>
     <row r="135" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B135" s="15">
         <v>17</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D135" s="15" t="s">
         <v>43</v>
@@ -4639,13 +4644,13 @@
     </row>
     <row r="136" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B136" s="15">
         <v>17</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D136" s="15" t="s">
         <v>43</v>
@@ -4662,13 +4667,13 @@
     </row>
     <row r="137" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B137" s="15">
         <v>17</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D137" s="15" t="s">
         <v>43</v>
@@ -4685,13 +4690,13 @@
     </row>
     <row r="138" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B138" s="15">
         <v>17</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D138" s="15" t="s">
         <v>43</v>
@@ -4708,13 +4713,13 @@
     </row>
     <row r="139" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B139" s="15">
         <v>17</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D139" s="15" t="s">
         <v>43</v>
@@ -4731,16 +4736,16 @@
     </row>
     <row r="140" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B140" s="15">
         <v>17</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D140" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E140" s="15"/>
       <c r="F140" s="21"/>
@@ -4754,16 +4759,16 @@
     </row>
     <row r="141" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B141" s="15">
         <v>17</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D141" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E141" s="15"/>
       <c r="F141" s="21"/>
@@ -4777,16 +4782,16 @@
     </row>
     <row r="142" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B142" s="15">
         <v>17</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D142" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E142" s="15"/>
       <c r="F142" s="21"/>
@@ -4800,16 +4805,16 @@
     </row>
     <row r="143" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B143" s="15">
         <v>17</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D143" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E143" s="15"/>
       <c r="F143" s="21"/>
@@ -4823,16 +4828,16 @@
     </row>
     <row r="144" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B144" s="15">
         <v>17</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D144" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E144" s="15"/>
       <c r="F144" s="21"/>
@@ -4846,16 +4851,16 @@
     </row>
     <row r="145" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B145" s="15">
         <v>17</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D145" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E145" s="15"/>
       <c r="F145" s="21"/>
@@ -4869,16 +4874,16 @@
     </row>
     <row r="146" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B146" s="15">
         <v>17</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D146" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E146" s="15"/>
       <c r="F146" s="21"/>
@@ -4892,16 +4897,16 @@
     </row>
     <row r="147" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B147" s="15">
         <v>17</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D147" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E147" s="15"/>
       <c r="F147" s="21"/>
@@ -4915,16 +4920,16 @@
     </row>
     <row r="148" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B148" s="15">
         <v>17</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D148" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E148" s="15"/>
       <c r="F148" s="21"/>
@@ -4938,16 +4943,16 @@
     </row>
     <row r="149" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B149" s="15">
         <v>17</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D149" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E149" s="15"/>
       <c r="F149" s="21"/>
@@ -4961,16 +4966,16 @@
     </row>
     <row r="150" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B150" s="15">
         <v>17</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D150" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E150" s="15"/>
       <c r="F150" s="21"/>
@@ -4984,16 +4989,16 @@
     </row>
     <row r="151" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B151" s="15">
         <v>17</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D151" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E151" s="15"/>
       <c r="F151" s="21"/>
@@ -5007,16 +5012,16 @@
     </row>
     <row r="152" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B152" s="15">
         <v>17</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D152" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E152" s="15"/>
       <c r="F152" s="21"/>
@@ -5030,16 +5035,16 @@
     </row>
     <row r="153" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B153" s="15">
         <v>17</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D153" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E153" s="15"/>
       <c r="F153" s="21"/>
@@ -5053,16 +5058,16 @@
     </row>
     <row r="154" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B154" s="15">
         <v>17</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D154" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E154" s="15"/>
       <c r="F154" s="21"/>
@@ -5076,16 +5081,16 @@
     </row>
     <row r="155" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B155" s="15">
         <v>17</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D155" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E155" s="15"/>
       <c r="F155" s="21"/>
@@ -5099,16 +5104,16 @@
     </row>
     <row r="156" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B156" s="15">
         <v>17</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D156" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E156" s="15"/>
       <c r="F156" s="21"/>
@@ -5122,16 +5127,16 @@
     </row>
     <row r="157" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B157" s="15">
         <v>17</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D157" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E157" s="15"/>
       <c r="F157" s="21"/>
@@ -5145,16 +5150,16 @@
     </row>
     <row r="158" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B158" s="15">
         <v>17</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D158" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E158" s="15"/>
       <c r="F158" s="21"/>
@@ -5168,16 +5173,16 @@
     </row>
     <row r="159" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B159" s="15">
         <v>17</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D159" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E159" s="15"/>
       <c r="F159" s="21"/>
@@ -5191,16 +5196,16 @@
     </row>
     <row r="160" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B160" s="15">
         <v>17</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D160" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E160" s="15"/>
       <c r="F160" s="21"/>
@@ -5214,16 +5219,16 @@
     </row>
     <row r="161" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B161" s="15">
         <v>17</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D161" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E161" s="15"/>
       <c r="F161" s="21"/>
@@ -5237,16 +5242,16 @@
     </row>
     <row r="162" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B162" s="15">
         <v>17</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D162" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E162" s="15"/>
       <c r="F162" s="21"/>
@@ -5260,16 +5265,16 @@
     </row>
     <row r="163" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="14" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B163" s="15">
         <v>17</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D163" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E163" s="15"/>
       <c r="F163" s="21"/>
@@ -5283,13 +5288,13 @@
     </row>
     <row r="164" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B164" s="15">
         <v>17</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D164" s="15" t="s">
         <v>44</v>
@@ -5306,13 +5311,13 @@
     </row>
     <row r="165" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B165" s="15">
         <v>17</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D165" s="15" t="s">
         <v>44</v>
@@ -5329,13 +5334,13 @@
     </row>
     <row r="166" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="14" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B166" s="15">
         <v>17</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D166" s="15" t="s">
         <v>44</v>
@@ -5352,13 +5357,13 @@
     </row>
     <row r="167" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B167" s="15">
         <v>17</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D167" s="15" t="s">
         <v>44</v>
@@ -5375,13 +5380,13 @@
     </row>
     <row r="168" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B168" s="15">
         <v>17</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D168" s="15" t="s">
         <v>44</v>
@@ -5398,13 +5403,13 @@
     </row>
     <row r="169" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B169" s="15">
         <v>17</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D169" s="15" t="s">
         <v>44</v>
@@ -5421,13 +5426,13 @@
     </row>
     <row r="170" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B170" s="15">
         <v>17</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D170" s="15" t="s">
         <v>44</v>
@@ -5444,13 +5449,13 @@
     </row>
     <row r="171" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B171" s="15">
         <v>17</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D171" s="15" t="s">
         <v>52</v>
@@ -5469,13 +5474,13 @@
     </row>
     <row r="172" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="14" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B172" s="15">
         <v>17</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D172" s="15" t="s">
         <v>52</v>
@@ -5494,13 +5499,13 @@
     </row>
     <row r="173" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B173" s="15">
         <v>17</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D173" s="15" t="s">
         <v>52</v>
@@ -5519,13 +5524,13 @@
     </row>
     <row r="174" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B174" s="15">
         <v>17</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D174" s="15" t="s">
         <v>52</v>
@@ -5544,13 +5549,13 @@
     </row>
     <row r="175" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B175" s="15">
         <v>17</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D175" s="15" t="s">
         <v>52</v>
@@ -5569,13 +5574,13 @@
     </row>
     <row r="176" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B176" s="15">
         <v>17</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D176" s="15" t="s">
         <v>52</v>
@@ -5594,13 +5599,13 @@
     </row>
     <row r="177" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B177" s="15">
         <v>17</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D177" s="15" t="s">
         <v>52</v>
@@ -5619,13 +5624,13 @@
     </row>
     <row r="178" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B178" s="15">
         <v>17</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D178" s="15" t="s">
         <v>52</v>
@@ -5644,13 +5649,13 @@
     </row>
     <row r="179" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B179" s="15">
         <v>17</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D179" s="15" t="s">
         <v>52</v>
@@ -5669,13 +5674,13 @@
     </row>
     <row r="180" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="14" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B180" s="15">
         <v>17</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D180" s="15" t="s">
         <v>52</v>
@@ -5694,13 +5699,13 @@
     </row>
     <row r="181" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="14" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B181" s="15">
         <v>17</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D181" s="15" t="s">
         <v>52</v>
@@ -5719,13 +5724,13 @@
     </row>
     <row r="182" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="14" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B182" s="15">
         <v>17</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D182" s="15" t="s">
         <v>52</v>
@@ -5744,13 +5749,13 @@
     </row>
     <row r="183" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B183" s="15">
         <v>17</v>
       </c>
       <c r="C183" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D183" s="15" t="s">
         <v>52</v>
@@ -5769,13 +5774,13 @@
     </row>
     <row r="184" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="14" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B184" s="15">
         <v>17</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D184" s="15" t="s">
         <v>52</v>
@@ -5794,13 +5799,13 @@
     </row>
     <row r="185" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="14" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B185" s="15">
         <v>17</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D185" s="15" t="s">
         <v>62</v>
@@ -5817,13 +5822,13 @@
     </row>
     <row r="186" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B186" s="15">
         <v>17</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D186" s="15" t="s">
         <v>62</v>
@@ -5840,13 +5845,13 @@
     </row>
     <row r="187" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B187" s="15">
         <v>17</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D187" s="15" t="s">
         <v>62</v>
@@ -5863,13 +5868,13 @@
     </row>
     <row r="188" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B188" s="15">
         <v>17</v>
       </c>
       <c r="C188" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D188" s="15" t="s">
         <v>31</v>
@@ -5888,13 +5893,13 @@
     </row>
     <row r="189" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B189" s="15">
         <v>17</v>
       </c>
       <c r="C189" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D189" s="15" t="s">
         <v>31</v>
@@ -5913,13 +5918,13 @@
     </row>
     <row r="190" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B190" s="15">
         <v>17</v>
       </c>
       <c r="C190" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D190" s="15" t="s">
         <v>31</v>
@@ -5938,20 +5943,20 @@
     </row>
     <row r="191" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="14" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B191" s="15">
         <v>17</v>
       </c>
       <c r="C191" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D191" s="15"/>
       <c r="E191" s="15"/>
       <c r="F191" s="15"/>
       <c r="G191" s="14"/>
       <c r="H191" s="24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I191" s="25">
         <v>1</v>
@@ -5959,20 +5964,20 @@
     </row>
     <row r="192" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="14" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B192" s="15">
         <v>17</v>
       </c>
       <c r="C192" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D192" s="15"/>
       <c r="E192" s="15"/>
       <c r="F192" s="15"/>
       <c r="G192" s="14"/>
       <c r="H192" s="24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I192" s="25">
         <v>0.99039999999999995</v>
@@ -5980,20 +5985,20 @@
     </row>
     <row r="193" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="14" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B193" s="15">
         <v>17</v>
       </c>
       <c r="C193" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D193" s="15"/>
       <c r="E193" s="15"/>
       <c r="F193" s="15"/>
       <c r="G193" s="14"/>
       <c r="H193" s="24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I193" s="25">
         <v>0.97119999999999995</v>
@@ -6001,20 +6006,20 @@
     </row>
     <row r="194" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="14" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B194" s="15">
         <v>17</v>
       </c>
       <c r="C194" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D194" s="15"/>
       <c r="E194" s="15"/>
       <c r="F194" s="15"/>
       <c r="G194" s="14"/>
       <c r="H194" s="24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I194" s="25">
         <v>0.95830000000000004</v>
@@ -6022,20 +6027,20 @@
     </row>
     <row r="195" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="14" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B195" s="15">
         <v>17</v>
       </c>
       <c r="C195" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D195" s="15"/>
       <c r="E195" s="15"/>
       <c r="F195" s="15"/>
       <c r="G195" s="14"/>
       <c r="H195" s="24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I195" s="25">
         <v>0.88</v>
@@ -6043,20 +6048,20 @@
     </row>
     <row r="196" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="14" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B196" s="15">
         <v>17</v>
       </c>
       <c r="C196" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D196" s="15"/>
       <c r="E196" s="15"/>
       <c r="F196" s="15"/>
       <c r="G196" s="14"/>
       <c r="H196" s="24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I196" s="25">
         <v>0.74</v>
@@ -6064,20 +6069,20 @@
     </row>
     <row r="197" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A197" s="14" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B197" s="15">
         <v>17</v>
       </c>
       <c r="C197" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D197" s="15"/>
       <c r="E197" s="15"/>
       <c r="F197" s="15"/>
       <c r="G197" s="14"/>
       <c r="H197" s="24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I197" s="25">
         <v>0.5</v>
@@ -6085,20 +6090,20 @@
     </row>
     <row r="198" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A198" s="14" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B198" s="15">
         <v>17</v>
       </c>
       <c r="C198" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D198" s="15"/>
       <c r="E198" s="15"/>
       <c r="F198" s="15"/>
       <c r="G198" s="14"/>
       <c r="H198" s="24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I198" s="25">
         <v>0.4</v>
@@ -6106,20 +6111,20 @@
     </row>
     <row r="199" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" s="14" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B199" s="15">
         <v>17</v>
       </c>
       <c r="C199" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D199" s="15"/>
       <c r="E199" s="15"/>
       <c r="F199" s="15"/>
       <c r="G199" s="14"/>
       <c r="H199" s="24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I199" s="25">
         <v>0.3</v>
@@ -6127,20 +6132,20 @@
     </row>
     <row r="200" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A200" s="14" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B200" s="15">
         <v>17</v>
       </c>
       <c r="C200" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D200" s="15"/>
       <c r="E200" s="15"/>
       <c r="F200" s="15"/>
       <c r="G200" s="14"/>
       <c r="H200" s="24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I200" s="25">
         <v>0.2</v>
@@ -6148,20 +6153,20 @@
     </row>
     <row r="201" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A201" s="14" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B201" s="15">
         <v>17</v>
       </c>
       <c r="C201" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D201" s="15"/>
       <c r="E201" s="15"/>
       <c r="F201" s="15"/>
       <c r="G201" s="14"/>
       <c r="H201" s="24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I201" s="25">
         <v>0.18</v>
@@ -6169,20 +6174,20 @@
     </row>
     <row r="202" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A202" s="14" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B202" s="15">
         <v>17</v>
       </c>
       <c r="C202" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D202" s="15"/>
       <c r="E202" s="15"/>
       <c r="F202" s="15"/>
       <c r="G202" s="14"/>
       <c r="H202" s="24" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I202" s="25">
         <v>0.16669999999999999</v>

</xml_diff>

<commit_message>
Uploaded 07-May-2021 15:46:24 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="295">
   <si>
     <t>RuleSet</t>
   </si>
@@ -236,6 +236,15 @@
   </si>
   <si>
     <t>getBenefit_group().getName().equals("$param")</t>
+  </si>
+  <si>
+    <t>getBenefit_group().getCoveredDays()==$param</t>
+  </si>
+  <si>
+    <t>getName().equals("$param")</t>
+  </si>
+  <si>
+    <t>getValue().equals("$param")</t>
   </si>
   <si>
     <t>$benefit: Benefit</t>
@@ -896,15 +905,6 @@
   </si>
   <si>
     <t>benefit</t>
-  </si>
-  <si>
-    <t>$benefit.getBenefit_group().getCoveredDays()==$param</t>
-  </si>
-  <si>
-    <t>$benefit.getName().equals("$param")</t>
-  </si>
-  <si>
-    <t>$benefit.getValue().equals("$param")</t>
   </si>
   <si>
     <t xml:space="preserve">$benefit.getBenefit_group().getCoverageFrom().equals("$param")
@@ -1526,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -1609,15 +1609,23 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="30" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
+      <c r="E4" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>294</v>
+      </c>
       <c r="I4" s="8"/>
       <c r="M4" s="3"/>
     </row>
@@ -1625,25 +1633,25 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>290</v>
+        <v>74</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>291</v>
+        <v>75</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>292</v>
+        <v>76</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>293</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -1654,7 +1662,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>6</v>
@@ -1669,7 +1677,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>8</v>
@@ -1677,13 +1685,13 @@
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B7" s="15">
         <v>17</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>9</v>
@@ -1700,13 +1708,13 @@
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B8" s="15">
         <v>17</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>9</v>
@@ -1723,13 +1731,13 @@
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B9" s="15">
         <v>17</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>9</v>
@@ -1746,13 +1754,13 @@
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B10" s="15">
         <v>17</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>9</v>
@@ -1769,13 +1777,13 @@
     </row>
     <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B11" s="15">
         <v>17</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>9</v>
@@ -1792,13 +1800,13 @@
     </row>
     <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B12" s="15">
         <v>17</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>9</v>
@@ -1815,13 +1823,13 @@
     </row>
     <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B13" s="15">
         <v>17</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>9</v>
@@ -1838,13 +1846,13 @@
     </row>
     <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B14" s="15">
         <v>17</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>9</v>
@@ -1861,13 +1869,13 @@
     </row>
     <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B15" s="15">
         <v>17</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>9</v>
@@ -1884,13 +1892,13 @@
     </row>
     <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B16" s="15">
         <v>17</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>9</v>
@@ -1907,13 +1915,13 @@
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B17" s="15">
         <v>17</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>9</v>
@@ -1930,13 +1938,13 @@
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B18" s="15">
         <v>17</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>9</v>
@@ -1953,13 +1961,13 @@
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B19" s="15">
         <v>17</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>9</v>
@@ -1976,13 +1984,13 @@
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B20" s="15">
         <v>17</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>9</v>
@@ -1999,13 +2007,13 @@
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B21" s="15">
         <v>17</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>9</v>
@@ -2022,13 +2030,13 @@
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B22" s="15">
         <v>17</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>9</v>
@@ -2045,13 +2053,13 @@
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B23" s="15">
         <v>17</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>9</v>
@@ -2068,13 +2076,13 @@
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B24" s="15">
         <v>17</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>9</v>
@@ -2091,13 +2099,13 @@
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B25" s="15">
         <v>17</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>28</v>
@@ -2114,13 +2122,13 @@
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B26" s="15">
         <v>17</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>28</v>
@@ -2137,13 +2145,13 @@
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B27" s="15">
         <v>17</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>28</v>
@@ -2160,13 +2168,13 @@
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B28" s="15">
         <v>17</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>28</v>
@@ -2183,13 +2191,13 @@
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B29" s="15">
         <v>17</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>28</v>
@@ -2206,13 +2214,13 @@
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B30" s="15">
         <v>17</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>28</v>
@@ -2229,13 +2237,13 @@
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B31" s="15">
         <v>17</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>28</v>
@@ -2252,13 +2260,13 @@
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B32" s="15">
         <v>17</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>28</v>
@@ -2275,13 +2283,13 @@
     </row>
     <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B33" s="15">
         <v>17</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>28</v>
@@ -2298,13 +2306,13 @@
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B34" s="15">
         <v>17</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>28</v>
@@ -2321,13 +2329,13 @@
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B35" s="15">
         <v>17</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>28</v>
@@ -2344,13 +2352,13 @@
     </row>
     <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B36" s="15">
         <v>17</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>28</v>
@@ -2367,13 +2375,13 @@
     </row>
     <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B37" s="15">
         <v>17</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>28</v>
@@ -2390,13 +2398,13 @@
     </row>
     <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B38" s="15">
         <v>17</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>28</v>
@@ -2413,13 +2421,13 @@
     </row>
     <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B39" s="15">
         <v>17</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>28</v>
@@ -2436,13 +2444,13 @@
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B40" s="15">
         <v>17</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>28</v>
@@ -2459,13 +2467,13 @@
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B41" s="15">
         <v>17</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>28</v>
@@ -2482,13 +2490,13 @@
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B42" s="15">
         <v>17</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>28</v>
@@ -2505,13 +2513,13 @@
     </row>
     <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B43" s="15">
         <v>17</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>29</v>
@@ -2528,13 +2536,13 @@
     </row>
     <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B44" s="15">
         <v>17</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>29</v>
@@ -2551,13 +2559,13 @@
     </row>
     <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B45" s="15">
         <v>17</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>29</v>
@@ -2574,13 +2582,13 @@
     </row>
     <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B46" s="15">
         <v>17</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>29</v>
@@ -2597,13 +2605,13 @@
     </row>
     <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B47" s="15">
         <v>17</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D47" s="15" t="s">
         <v>29</v>
@@ -2620,13 +2628,13 @@
     </row>
     <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B48" s="15">
         <v>17</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>29</v>
@@ -2643,13 +2651,13 @@
     </row>
     <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B49" s="15">
         <v>17</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>29</v>
@@ -2666,13 +2674,13 @@
     </row>
     <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B50" s="15">
         <v>17</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>29</v>
@@ -2689,13 +2697,13 @@
     </row>
     <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B51" s="15">
         <v>17</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>29</v>
@@ -2712,13 +2720,13 @@
     </row>
     <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B52" s="15">
         <v>17</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D52" s="15" t="s">
         <v>29</v>
@@ -2735,13 +2743,13 @@
     </row>
     <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B53" s="15">
         <v>17</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>29</v>
@@ -2758,13 +2766,13 @@
     </row>
     <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B54" s="15">
         <v>17</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>29</v>
@@ -2781,13 +2789,13 @@
     </row>
     <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B55" s="15">
         <v>17</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>29</v>
@@ -2804,13 +2812,13 @@
     </row>
     <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B56" s="15">
         <v>17</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>29</v>
@@ -2827,13 +2835,13 @@
     </row>
     <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B57" s="15">
         <v>17</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>29</v>
@@ -2850,13 +2858,13 @@
     </row>
     <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B58" s="15">
         <v>17</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D58" s="15" t="s">
         <v>29</v>
@@ -2873,13 +2881,13 @@
     </row>
     <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B59" s="15">
         <v>17</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D59" s="15" t="s">
         <v>29</v>
@@ -2896,13 +2904,13 @@
     </row>
     <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B60" s="15">
         <v>17</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D60" s="15" t="s">
         <v>29</v>
@@ -2919,13 +2927,13 @@
     </row>
     <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B61" s="15">
         <v>17</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D61" s="15" t="s">
         <v>30</v>
@@ -2942,13 +2950,13 @@
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B62" s="15">
         <v>17</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D62" s="15" t="s">
         <v>30</v>
@@ -2965,13 +2973,13 @@
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B63" s="15">
         <v>17</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D63" s="15" t="s">
         <v>30</v>
@@ -2988,13 +2996,13 @@
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B64" s="15">
         <v>17</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>30</v>
@@ -3011,13 +3019,13 @@
     </row>
     <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B65" s="15">
         <v>17</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D65" s="15" t="s">
         <v>30</v>
@@ -3034,13 +3042,13 @@
     </row>
     <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B66" s="15">
         <v>17</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D66" s="15" t="s">
         <v>30</v>
@@ -3057,13 +3065,13 @@
     </row>
     <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B67" s="15">
         <v>17</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D67" s="15" t="s">
         <v>30</v>
@@ -3080,13 +3088,13 @@
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B68" s="15">
         <v>17</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D68" s="15" t="s">
         <v>30</v>
@@ -3103,13 +3111,13 @@
     </row>
     <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B69" s="15">
         <v>17</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D69" s="15" t="s">
         <v>30</v>
@@ -3126,13 +3134,13 @@
     </row>
     <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B70" s="15">
         <v>17</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D70" s="15" t="s">
         <v>30</v>
@@ -3149,13 +3157,13 @@
     </row>
     <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B71" s="15">
         <v>17</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D71" s="15" t="s">
         <v>30</v>
@@ -3172,13 +3180,13 @@
     </row>
     <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B72" s="15">
         <v>17</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D72" s="15" t="s">
         <v>30</v>
@@ -3195,13 +3203,13 @@
     </row>
     <row r="73" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B73" s="15">
         <v>17</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D73" s="15" t="s">
         <v>30</v>
@@ -3218,13 +3226,13 @@
     </row>
     <row r="74" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B74" s="15">
         <v>17</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D74" s="15" t="s">
         <v>30</v>
@@ -3241,13 +3249,13 @@
     </row>
     <row r="75" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B75" s="15">
         <v>17</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D75" s="15" t="s">
         <v>30</v>
@@ -3264,13 +3272,13 @@
     </row>
     <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B76" s="15">
         <v>17</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D76" s="15" t="s">
         <v>30</v>
@@ -3287,13 +3295,13 @@
     </row>
     <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B77" s="15">
         <v>17</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D77" s="15" t="s">
         <v>30</v>
@@ -3310,13 +3318,13 @@
     </row>
     <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B78" s="15">
         <v>17</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D78" s="15" t="s">
         <v>30</v>
@@ -3333,13 +3341,13 @@
     </row>
     <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B79" s="15">
         <v>17</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D79" s="15" t="s">
         <v>72</v>
@@ -3356,13 +3364,13 @@
     </row>
     <row r="80" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B80" s="15">
         <v>17</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D80" s="15" t="s">
         <v>72</v>
@@ -3379,13 +3387,13 @@
     </row>
     <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B81" s="15">
         <v>17</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D81" s="15" t="s">
         <v>72</v>
@@ -3402,13 +3410,13 @@
     </row>
     <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B82" s="15">
         <v>17</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D82" s="15" t="s">
         <v>72</v>
@@ -3425,13 +3433,13 @@
     </row>
     <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B83" s="15">
         <v>17</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D83" s="15" t="s">
         <v>72</v>
@@ -3448,13 +3456,13 @@
     </row>
     <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B84" s="15">
         <v>17</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D84" s="15" t="s">
         <v>72</v>
@@ -3471,13 +3479,13 @@
     </row>
     <row r="85" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B85" s="15">
         <v>17</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D85" s="15" t="s">
         <v>72</v>
@@ -3494,13 +3502,13 @@
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B86" s="15">
         <v>17</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D86" s="15" t="s">
         <v>72</v>
@@ -3517,13 +3525,13 @@
     </row>
     <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B87" s="15">
         <v>17</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D87" s="15" t="s">
         <v>72</v>
@@ -3540,13 +3548,13 @@
     </row>
     <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B88" s="15">
         <v>17</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D88" s="15" t="s">
         <v>72</v>
@@ -3563,13 +3571,13 @@
     </row>
     <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B89" s="15">
         <v>17</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D89" s="15" t="s">
         <v>72</v>
@@ -3586,13 +3594,13 @@
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B90" s="15">
         <v>17</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D90" s="15" t="s">
         <v>72</v>
@@ -3609,13 +3617,13 @@
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B91" s="15">
         <v>17</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D91" s="15" t="s">
         <v>72</v>
@@ -3632,13 +3640,13 @@
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B92" s="15">
         <v>17</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>72</v>
@@ -3655,13 +3663,13 @@
     </row>
     <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B93" s="15">
         <v>17</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D93" s="15" t="s">
         <v>72</v>
@@ -3678,13 +3686,13 @@
     </row>
     <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B94" s="15">
         <v>17</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D94" s="15" t="s">
         <v>72</v>
@@ -3701,13 +3709,13 @@
     </row>
     <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B95" s="15">
         <v>17</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D95" s="15" t="s">
         <v>72</v>
@@ -3724,13 +3732,13 @@
     </row>
     <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B96" s="15">
         <v>17</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D96" s="15" t="s">
         <v>72</v>
@@ -3747,13 +3755,13 @@
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B97" s="15">
         <v>17</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D97" s="15" t="s">
         <v>31</v>
@@ -3770,13 +3778,13 @@
     </row>
     <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B98" s="15">
         <v>17</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D98" s="15" t="s">
         <v>31</v>
@@ -3793,13 +3801,13 @@
     </row>
     <row r="99" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B99" s="15">
         <v>17</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D99" s="15" t="s">
         <v>31</v>
@@ -3816,13 +3824,13 @@
     </row>
     <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B100" s="15">
         <v>17</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D100" s="15" t="s">
         <v>31</v>
@@ -3839,13 +3847,13 @@
     </row>
     <row r="101" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B101" s="15">
         <v>17</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D101" s="15" t="s">
         <v>31</v>
@@ -3862,13 +3870,13 @@
     </row>
     <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B102" s="15">
         <v>17</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D102" s="15" t="s">
         <v>31</v>
@@ -3885,13 +3893,13 @@
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B103" s="15">
         <v>17</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D103" s="15" t="s">
         <v>31</v>
@@ -3908,13 +3916,13 @@
     </row>
     <row r="104" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B104" s="15">
         <v>17</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D104" s="15" t="s">
         <v>31</v>
@@ -3931,13 +3939,13 @@
     </row>
     <row r="105" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B105" s="15">
         <v>17</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D105" s="15" t="s">
         <v>31</v>
@@ -3954,13 +3962,13 @@
     </row>
     <row r="106" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B106" s="15">
         <v>17</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D106" s="15" t="s">
         <v>31</v>
@@ -3977,13 +3985,13 @@
     </row>
     <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B107" s="15">
         <v>17</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D107" s="15" t="s">
         <v>31</v>
@@ -4000,13 +4008,13 @@
     </row>
     <row r="108" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B108" s="15">
         <v>17</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D108" s="15" t="s">
         <v>31</v>
@@ -4023,13 +4031,13 @@
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B109" s="15">
         <v>17</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D109" s="15" t="s">
         <v>31</v>
@@ -4046,13 +4054,13 @@
     </row>
     <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B110" s="15">
         <v>17</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D110" s="15" t="s">
         <v>31</v>
@@ -4069,13 +4077,13 @@
     </row>
     <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B111" s="15">
         <v>17</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D111" s="15" t="s">
         <v>31</v>
@@ -4092,13 +4100,13 @@
     </row>
     <row r="112" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B112" s="15">
         <v>17</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D112" s="15" t="s">
         <v>31</v>
@@ -4115,13 +4123,13 @@
     </row>
     <row r="113" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B113" s="15">
         <v>17</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D113" s="15" t="s">
         <v>31</v>
@@ -4138,13 +4146,13 @@
     </row>
     <row r="114" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B114" s="15">
         <v>17</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D114" s="15" t="s">
         <v>31</v>
@@ -4161,13 +4169,13 @@
     </row>
     <row r="115" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B115" s="15">
         <v>17</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D115" s="15" t="s">
         <v>31</v>
@@ -4184,13 +4192,13 @@
     </row>
     <row r="116" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B116" s="15">
         <v>17</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D116" s="15" t="s">
         <v>31</v>
@@ -4207,13 +4215,13 @@
     </row>
     <row r="117" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B117" s="15">
         <v>17</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D117" s="15" t="s">
         <v>31</v>
@@ -4230,13 +4238,13 @@
     </row>
     <row r="118" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B118" s="15">
         <v>17</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D118" s="15" t="s">
         <v>31</v>
@@ -4253,13 +4261,13 @@
     </row>
     <row r="119" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B119" s="15">
         <v>17</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D119" s="15" t="s">
         <v>31</v>
@@ -4276,13 +4284,13 @@
     </row>
     <row r="120" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B120" s="15">
         <v>17</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D120" s="15" t="s">
         <v>31</v>
@@ -4299,13 +4307,13 @@
     </row>
     <row r="121" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B121" s="15">
         <v>17</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D121" s="15" t="s">
         <v>31</v>
@@ -4322,13 +4330,13 @@
     </row>
     <row r="122" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B122" s="15">
         <v>17</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D122" s="15" t="s">
         <v>31</v>
@@ -4345,13 +4353,13 @@
     </row>
     <row r="123" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B123" s="15">
         <v>17</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D123" s="15" t="s">
         <v>31</v>
@@ -4368,13 +4376,13 @@
     </row>
     <row r="124" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B124" s="15">
         <v>17</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D124" s="15" t="s">
         <v>31</v>
@@ -4391,13 +4399,13 @@
     </row>
     <row r="125" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B125" s="15">
         <v>17</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D125" s="15" t="s">
         <v>31</v>
@@ -4414,13 +4422,13 @@
     </row>
     <row r="126" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B126" s="15">
         <v>17</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D126" s="15" t="s">
         <v>31</v>
@@ -4437,13 +4445,13 @@
     </row>
     <row r="127" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B127" s="15">
         <v>17</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D127" s="15" t="s">
         <v>31</v>
@@ -4460,13 +4468,13 @@
     </row>
     <row r="128" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B128" s="15">
         <v>17</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D128" s="15" t="s">
         <v>43</v>
@@ -4483,13 +4491,13 @@
     </row>
     <row r="129" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B129" s="15">
         <v>17</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D129" s="15" t="s">
         <v>43</v>
@@ -4506,13 +4514,13 @@
     </row>
     <row r="130" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B130" s="15">
         <v>17</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D130" s="15" t="s">
         <v>43</v>
@@ -4529,13 +4537,13 @@
     </row>
     <row r="131" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B131" s="15">
         <v>17</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D131" s="15" t="s">
         <v>43</v>
@@ -4552,13 +4560,13 @@
     </row>
     <row r="132" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B132" s="15">
         <v>17</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D132" s="15" t="s">
         <v>43</v>
@@ -4575,13 +4583,13 @@
     </row>
     <row r="133" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B133" s="15">
         <v>17</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D133" s="15" t="s">
         <v>43</v>
@@ -4598,13 +4606,13 @@
     </row>
     <row r="134" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B134" s="15">
         <v>17</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D134" s="15" t="s">
         <v>43</v>
@@ -4621,13 +4629,13 @@
     </row>
     <row r="135" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B135" s="15">
         <v>17</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D135" s="15" t="s">
         <v>43</v>
@@ -4644,13 +4652,13 @@
     </row>
     <row r="136" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B136" s="15">
         <v>17</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D136" s="15" t="s">
         <v>43</v>
@@ -4667,13 +4675,13 @@
     </row>
     <row r="137" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B137" s="15">
         <v>17</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D137" s="15" t="s">
         <v>43</v>
@@ -4690,13 +4698,13 @@
     </row>
     <row r="138" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B138" s="15">
         <v>17</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D138" s="15" t="s">
         <v>43</v>
@@ -4713,13 +4721,13 @@
     </row>
     <row r="139" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B139" s="15">
         <v>17</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D139" s="15" t="s">
         <v>43</v>
@@ -4736,16 +4744,16 @@
     </row>
     <row r="140" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B140" s="15">
         <v>17</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D140" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E140" s="15"/>
       <c r="F140" s="21"/>
@@ -4759,16 +4767,16 @@
     </row>
     <row r="141" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B141" s="15">
         <v>17</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D141" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E141" s="15"/>
       <c r="F141" s="21"/>
@@ -4782,16 +4790,16 @@
     </row>
     <row r="142" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B142" s="15">
         <v>17</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D142" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E142" s="15"/>
       <c r="F142" s="21"/>
@@ -4805,16 +4813,16 @@
     </row>
     <row r="143" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B143" s="15">
         <v>17</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D143" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E143" s="15"/>
       <c r="F143" s="21"/>
@@ -4828,16 +4836,16 @@
     </row>
     <row r="144" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B144" s="15">
         <v>17</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D144" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E144" s="15"/>
       <c r="F144" s="21"/>
@@ -4851,16 +4859,16 @@
     </row>
     <row r="145" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B145" s="15">
         <v>17</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D145" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E145" s="15"/>
       <c r="F145" s="21"/>
@@ -4874,16 +4882,16 @@
     </row>
     <row r="146" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B146" s="15">
         <v>17</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D146" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E146" s="15"/>
       <c r="F146" s="21"/>
@@ -4897,16 +4905,16 @@
     </row>
     <row r="147" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B147" s="15">
         <v>17</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D147" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E147" s="15"/>
       <c r="F147" s="21"/>
@@ -4920,16 +4928,16 @@
     </row>
     <row r="148" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B148" s="15">
         <v>17</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D148" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E148" s="15"/>
       <c r="F148" s="21"/>
@@ -4943,16 +4951,16 @@
     </row>
     <row r="149" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B149" s="15">
         <v>17</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D149" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E149" s="15"/>
       <c r="F149" s="21"/>
@@ -4966,16 +4974,16 @@
     </row>
     <row r="150" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B150" s="15">
         <v>17</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D150" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E150" s="15"/>
       <c r="F150" s="21"/>
@@ -4989,16 +4997,16 @@
     </row>
     <row r="151" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B151" s="15">
         <v>17</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D151" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E151" s="15"/>
       <c r="F151" s="21"/>
@@ -5012,16 +5020,16 @@
     </row>
     <row r="152" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B152" s="15">
         <v>17</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D152" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E152" s="15"/>
       <c r="F152" s="21"/>
@@ -5035,16 +5043,16 @@
     </row>
     <row r="153" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B153" s="15">
         <v>17</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D153" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E153" s="15"/>
       <c r="F153" s="21"/>
@@ -5058,16 +5066,16 @@
     </row>
     <row r="154" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B154" s="15">
         <v>17</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D154" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E154" s="15"/>
       <c r="F154" s="21"/>
@@ -5081,16 +5089,16 @@
     </row>
     <row r="155" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B155" s="15">
         <v>17</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D155" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E155" s="15"/>
       <c r="F155" s="21"/>
@@ -5104,16 +5112,16 @@
     </row>
     <row r="156" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B156" s="15">
         <v>17</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D156" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E156" s="15"/>
       <c r="F156" s="21"/>
@@ -5127,16 +5135,16 @@
     </row>
     <row r="157" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B157" s="15">
         <v>17</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D157" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E157" s="15"/>
       <c r="F157" s="21"/>
@@ -5150,16 +5158,16 @@
     </row>
     <row r="158" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B158" s="15">
         <v>17</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D158" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E158" s="15"/>
       <c r="F158" s="21"/>
@@ -5173,16 +5181,16 @@
     </row>
     <row r="159" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B159" s="15">
         <v>17</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D159" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E159" s="15"/>
       <c r="F159" s="21"/>
@@ -5196,16 +5204,16 @@
     </row>
     <row r="160" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B160" s="15">
         <v>17</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D160" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E160" s="15"/>
       <c r="F160" s="21"/>
@@ -5219,16 +5227,16 @@
     </row>
     <row r="161" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B161" s="15">
         <v>17</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D161" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E161" s="15"/>
       <c r="F161" s="21"/>
@@ -5242,16 +5250,16 @@
     </row>
     <row r="162" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B162" s="15">
         <v>17</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D162" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E162" s="15"/>
       <c r="F162" s="21"/>
@@ -5265,16 +5273,16 @@
     </row>
     <row r="163" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="14" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B163" s="15">
         <v>17</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D163" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E163" s="15"/>
       <c r="F163" s="21"/>
@@ -5288,13 +5296,13 @@
     </row>
     <row r="164" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B164" s="15">
         <v>17</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D164" s="15" t="s">
         <v>44</v>
@@ -5311,13 +5319,13 @@
     </row>
     <row r="165" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B165" s="15">
         <v>17</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D165" s="15" t="s">
         <v>44</v>
@@ -5334,13 +5342,13 @@
     </row>
     <row r="166" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="14" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B166" s="15">
         <v>17</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D166" s="15" t="s">
         <v>44</v>
@@ -5357,13 +5365,13 @@
     </row>
     <row r="167" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B167" s="15">
         <v>17</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D167" s="15" t="s">
         <v>44</v>
@@ -5380,13 +5388,13 @@
     </row>
     <row r="168" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B168" s="15">
         <v>17</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D168" s="15" t="s">
         <v>44</v>
@@ -5403,13 +5411,13 @@
     </row>
     <row r="169" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B169" s="15">
         <v>17</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D169" s="15" t="s">
         <v>44</v>
@@ -5426,13 +5434,13 @@
     </row>
     <row r="170" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B170" s="15">
         <v>17</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D170" s="15" t="s">
         <v>44</v>
@@ -5449,13 +5457,13 @@
     </row>
     <row r="171" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B171" s="15">
         <v>17</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D171" s="15" t="s">
         <v>52</v>
@@ -5474,13 +5482,13 @@
     </row>
     <row r="172" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="14" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B172" s="15">
         <v>17</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D172" s="15" t="s">
         <v>52</v>
@@ -5499,13 +5507,13 @@
     </row>
     <row r="173" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="14" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B173" s="15">
         <v>17</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D173" s="15" t="s">
         <v>52</v>
@@ -5524,13 +5532,13 @@
     </row>
     <row r="174" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B174" s="15">
         <v>17</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D174" s="15" t="s">
         <v>52</v>
@@ -5549,13 +5557,13 @@
     </row>
     <row r="175" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B175" s="15">
         <v>17</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D175" s="15" t="s">
         <v>52</v>
@@ -5574,13 +5582,13 @@
     </row>
     <row r="176" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B176" s="15">
         <v>17</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D176" s="15" t="s">
         <v>52</v>
@@ -5599,13 +5607,13 @@
     </row>
     <row r="177" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B177" s="15">
         <v>17</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D177" s="15" t="s">
         <v>52</v>
@@ -5624,13 +5632,13 @@
     </row>
     <row r="178" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B178" s="15">
         <v>17</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D178" s="15" t="s">
         <v>52</v>
@@ -5649,13 +5657,13 @@
     </row>
     <row r="179" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B179" s="15">
         <v>17</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D179" s="15" t="s">
         <v>52</v>
@@ -5674,13 +5682,13 @@
     </row>
     <row r="180" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="14" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B180" s="15">
         <v>17</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D180" s="15" t="s">
         <v>52</v>
@@ -5699,13 +5707,13 @@
     </row>
     <row r="181" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="14" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B181" s="15">
         <v>17</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D181" s="15" t="s">
         <v>52</v>
@@ -5724,13 +5732,13 @@
     </row>
     <row r="182" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="14" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B182" s="15">
         <v>17</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D182" s="15" t="s">
         <v>52</v>
@@ -5749,13 +5757,13 @@
     </row>
     <row r="183" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B183" s="15">
         <v>17</v>
       </c>
       <c r="C183" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D183" s="15" t="s">
         <v>52</v>
@@ -5774,13 +5782,13 @@
     </row>
     <row r="184" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="14" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B184" s="15">
         <v>17</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D184" s="15" t="s">
         <v>52</v>
@@ -5799,13 +5807,13 @@
     </row>
     <row r="185" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="14" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B185" s="15">
         <v>17</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D185" s="15" t="s">
         <v>62</v>
@@ -5822,13 +5830,13 @@
     </row>
     <row r="186" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B186" s="15">
         <v>17</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D186" s="15" t="s">
         <v>62</v>
@@ -5845,13 +5853,13 @@
     </row>
     <row r="187" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B187" s="15">
         <v>17</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D187" s="15" t="s">
         <v>62</v>
@@ -5868,13 +5876,13 @@
     </row>
     <row r="188" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B188" s="15">
         <v>17</v>
       </c>
       <c r="C188" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D188" s="15" t="s">
         <v>31</v>
@@ -5893,13 +5901,13 @@
     </row>
     <row r="189" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B189" s="15">
         <v>17</v>
       </c>
       <c r="C189" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D189" s="15" t="s">
         <v>31</v>
@@ -5918,13 +5926,13 @@
     </row>
     <row r="190" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B190" s="15">
         <v>17</v>
       </c>
       <c r="C190" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D190" s="15" t="s">
         <v>31</v>
@@ -5943,20 +5951,20 @@
     </row>
     <row r="191" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="14" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B191" s="15">
         <v>17</v>
       </c>
       <c r="C191" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D191" s="15"/>
       <c r="E191" s="15"/>
       <c r="F191" s="15"/>
       <c r="G191" s="14"/>
       <c r="H191" s="24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I191" s="25">
         <v>1</v>
@@ -5964,20 +5972,20 @@
     </row>
     <row r="192" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="14" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B192" s="15">
         <v>17</v>
       </c>
       <c r="C192" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D192" s="15"/>
       <c r="E192" s="15"/>
       <c r="F192" s="15"/>
       <c r="G192" s="14"/>
       <c r="H192" s="24" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I192" s="25">
         <v>0.99039999999999995</v>
@@ -5985,20 +5993,20 @@
     </row>
     <row r="193" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="14" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B193" s="15">
         <v>17</v>
       </c>
       <c r="C193" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D193" s="15"/>
       <c r="E193" s="15"/>
       <c r="F193" s="15"/>
       <c r="G193" s="14"/>
       <c r="H193" s="24" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I193" s="25">
         <v>0.97119999999999995</v>
@@ -6006,20 +6014,20 @@
     </row>
     <row r="194" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="14" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B194" s="15">
         <v>17</v>
       </c>
       <c r="C194" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D194" s="15"/>
       <c r="E194" s="15"/>
       <c r="F194" s="15"/>
       <c r="G194" s="14"/>
       <c r="H194" s="24" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I194" s="25">
         <v>0.95830000000000004</v>
@@ -6027,20 +6035,20 @@
     </row>
     <row r="195" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="14" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B195" s="15">
         <v>17</v>
       </c>
       <c r="C195" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D195" s="15"/>
       <c r="E195" s="15"/>
       <c r="F195" s="15"/>
       <c r="G195" s="14"/>
       <c r="H195" s="24" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="I195" s="25">
         <v>0.88</v>
@@ -6048,20 +6056,20 @@
     </row>
     <row r="196" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="14" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B196" s="15">
         <v>17</v>
       </c>
       <c r="C196" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D196" s="15"/>
       <c r="E196" s="15"/>
       <c r="F196" s="15"/>
       <c r="G196" s="14"/>
       <c r="H196" s="24" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I196" s="25">
         <v>0.74</v>
@@ -6069,20 +6077,20 @@
     </row>
     <row r="197" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A197" s="14" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B197" s="15">
         <v>17</v>
       </c>
       <c r="C197" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D197" s="15"/>
       <c r="E197" s="15"/>
       <c r="F197" s="15"/>
       <c r="G197" s="14"/>
       <c r="H197" s="24" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I197" s="25">
         <v>0.5</v>
@@ -6090,20 +6098,20 @@
     </row>
     <row r="198" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A198" s="14" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B198" s="15">
         <v>17</v>
       </c>
       <c r="C198" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D198" s="15"/>
       <c r="E198" s="15"/>
       <c r="F198" s="15"/>
       <c r="G198" s="14"/>
       <c r="H198" s="24" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I198" s="25">
         <v>0.4</v>
@@ -6111,20 +6119,20 @@
     </row>
     <row r="199" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" s="14" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B199" s="15">
         <v>17</v>
       </c>
       <c r="C199" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D199" s="15"/>
       <c r="E199" s="15"/>
       <c r="F199" s="15"/>
       <c r="G199" s="14"/>
       <c r="H199" s="24" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I199" s="25">
         <v>0.3</v>
@@ -6132,20 +6140,20 @@
     </row>
     <row r="200" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A200" s="14" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B200" s="15">
         <v>17</v>
       </c>
       <c r="C200" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D200" s="15"/>
       <c r="E200" s="15"/>
       <c r="F200" s="15"/>
       <c r="G200" s="14"/>
       <c r="H200" s="24" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I200" s="25">
         <v>0.2</v>
@@ -6153,20 +6161,20 @@
     </row>
     <row r="201" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A201" s="14" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B201" s="15">
         <v>17</v>
       </c>
       <c r="C201" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D201" s="15"/>
       <c r="E201" s="15"/>
       <c r="F201" s="15"/>
       <c r="G201" s="14"/>
       <c r="H201" s="24" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I201" s="25">
         <v>0.18</v>
@@ -6174,20 +6182,20 @@
     </row>
     <row r="202" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A202" s="14" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B202" s="15">
         <v>17</v>
       </c>
       <c r="C202" s="15" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D202" s="15"/>
       <c r="E202" s="15"/>
       <c r="F202" s="15"/>
       <c r="G202" s="14"/>
       <c r="H202" s="24" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="I202" s="25">
         <v>0.16669999999999999</v>

</xml_diff>

<commit_message>
Uploaded 11-May-2021 12:17:27 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedDecision.xlsx
@@ -235,26 +235,10 @@
     <t>RENAL CARE (DIALYSIS)</t>
   </si>
   <si>
-    <t>getBenefit_group().getName().equals("$param")</t>
-  </si>
-  <si>
-    <t>getBenefit_group().getCoveredDays()==$param</t>
-  </si>
-  <si>
-    <t>getName().equals("$param")</t>
-  </si>
-  <si>
-    <t>getValue().equals("$param")</t>
-  </si>
-  <si>
     <t>$benefit: Benefit</t>
   </si>
   <si>
     <t>$benefit.setCalculationResult($benefit.getCalculationResult()*$param);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">getBenefit_group().getCoverageFrom().equals("$param")
-</t>
   </si>
   <si>
     <t>1st Quarter</t>
@@ -903,6 +887,22 @@
   </si>
   <si>
     <t>AssumptionUsedDecision196</t>
+  </si>
+  <si>
+    <t>getBenefit_group().getName()</t>
+  </si>
+  <si>
+    <t>getBenefit_group().getCoveredDays()</t>
+  </si>
+  <si>
+    <t>getName()</t>
+  </si>
+  <si>
+    <t>getValue()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getBenefit_group().getCoverageFrom()
+</t>
   </si>
 </sst>
 </file>
@@ -1514,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A204" sqref="A204"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1591,7 +1591,7 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
@@ -1604,22 +1604,22 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>73</v>
+        <v>287</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -1642,7 +1642,7 @@
         <v>7</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>8</v>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B7" s="15">
         <v>17</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B8" s="15">
         <v>17</v>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B9" s="15">
         <v>17</v>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B10" s="15">
         <v>17</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B11" s="15">
         <v>17</v>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B12" s="15">
         <v>17</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B13" s="15">
         <v>17</v>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B14" s="15">
         <v>17</v>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B15" s="15">
         <v>17</v>
@@ -1830,7 +1830,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B16" s="15">
         <v>17</v>
@@ -1850,7 +1850,7 @@
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B17" s="15">
         <v>17</v>
@@ -1870,7 +1870,7 @@
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B18" s="15">
         <v>17</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B19" s="15">
         <v>17</v>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B20" s="15">
         <v>17</v>
@@ -1930,7 +1930,7 @@
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B21" s="15">
         <v>17</v>
@@ -1950,7 +1950,7 @@
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B22" s="15">
         <v>17</v>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B23" s="15">
         <v>17</v>
@@ -1990,7 +1990,7 @@
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B24" s="15">
         <v>17</v>
@@ -2010,7 +2010,7 @@
     </row>
     <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B25" s="15">
         <v>17</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B26" s="15">
         <v>17</v>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B27" s="15">
         <v>17</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B28" s="15">
         <v>17</v>
@@ -2090,7 +2090,7 @@
     </row>
     <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B29" s="15">
         <v>17</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B30" s="15">
         <v>17</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B31" s="15">
         <v>17</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B32" s="15">
         <v>17</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B33" s="15">
         <v>17</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B34" s="15">
         <v>17</v>
@@ -2210,7 +2210,7 @@
     </row>
     <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B35" s="15">
         <v>17</v>
@@ -2230,7 +2230,7 @@
     </row>
     <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B36" s="15">
         <v>17</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B37" s="15">
         <v>17</v>
@@ -2270,7 +2270,7 @@
     </row>
     <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B38" s="15">
         <v>17</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B39" s="15">
         <v>17</v>
@@ -2310,7 +2310,7 @@
     </row>
     <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B40" s="15">
         <v>17</v>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B41" s="15">
         <v>17</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B42" s="15">
         <v>17</v>
@@ -2370,7 +2370,7 @@
     </row>
     <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B43" s="15">
         <v>17</v>
@@ -2390,7 +2390,7 @@
     </row>
     <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B44" s="15">
         <v>17</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B45" s="15">
         <v>17</v>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B46" s="15">
         <v>17</v>
@@ -2450,7 +2450,7 @@
     </row>
     <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B47" s="15">
         <v>17</v>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B48" s="15">
         <v>17</v>
@@ -2490,7 +2490,7 @@
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B49" s="15">
         <v>17</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B50" s="15">
         <v>17</v>
@@ -2530,7 +2530,7 @@
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B51" s="15">
         <v>17</v>
@@ -2550,7 +2550,7 @@
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B52" s="15">
         <v>17</v>
@@ -2570,7 +2570,7 @@
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B53" s="15">
         <v>17</v>
@@ -2590,7 +2590,7 @@
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B54" s="15">
         <v>17</v>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B55" s="15">
         <v>17</v>
@@ -2630,7 +2630,7 @@
     </row>
     <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B56" s="15">
         <v>17</v>
@@ -2650,7 +2650,7 @@
     </row>
     <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B57" s="15">
         <v>17</v>
@@ -2670,7 +2670,7 @@
     </row>
     <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B58" s="15">
         <v>17</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B59" s="15">
         <v>17</v>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B60" s="15">
         <v>17</v>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B61" s="15">
         <v>17</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B62" s="15">
         <v>17</v>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B63" s="15">
         <v>17</v>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B64" s="15">
         <v>17</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B65" s="15">
         <v>17</v>
@@ -2830,7 +2830,7 @@
     </row>
     <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B66" s="15">
         <v>17</v>
@@ -2850,7 +2850,7 @@
     </row>
     <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B67" s="15">
         <v>17</v>
@@ -2870,7 +2870,7 @@
     </row>
     <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B68" s="15">
         <v>17</v>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B69" s="15">
         <v>17</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B70" s="15">
         <v>17</v>
@@ -2930,7 +2930,7 @@
     </row>
     <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B71" s="15">
         <v>17</v>
@@ -2950,7 +2950,7 @@
     </row>
     <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B72" s="15">
         <v>17</v>
@@ -2970,7 +2970,7 @@
     </row>
     <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B73" s="15">
         <v>17</v>
@@ -2990,7 +2990,7 @@
     </row>
     <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B74" s="15">
         <v>17</v>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="75" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B75" s="15">
         <v>17</v>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="76" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B76" s="15">
         <v>17</v>
@@ -3050,7 +3050,7 @@
     </row>
     <row r="77" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B77" s="15">
         <v>17</v>
@@ -3070,7 +3070,7 @@
     </row>
     <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B78" s="15">
         <v>17</v>
@@ -3090,7 +3090,7 @@
     </row>
     <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B79" s="15">
         <v>17</v>
@@ -3110,7 +3110,7 @@
     </row>
     <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B80" s="15">
         <v>17</v>
@@ -3130,7 +3130,7 @@
     </row>
     <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B81" s="15">
         <v>17</v>
@@ -3150,7 +3150,7 @@
     </row>
     <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B82" s="15">
         <v>17</v>
@@ -3170,7 +3170,7 @@
     </row>
     <row r="83" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B83" s="15">
         <v>17</v>
@@ -3190,7 +3190,7 @@
     </row>
     <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B84" s="15">
         <v>17</v>
@@ -3210,7 +3210,7 @@
     </row>
     <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B85" s="15">
         <v>17</v>
@@ -3230,7 +3230,7 @@
     </row>
     <row r="86" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B86" s="15">
         <v>17</v>
@@ -3250,7 +3250,7 @@
     </row>
     <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B87" s="15">
         <v>17</v>
@@ -3270,7 +3270,7 @@
     </row>
     <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B88" s="15">
         <v>17</v>
@@ -3290,7 +3290,7 @@
     </row>
     <row r="89" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B89" s="15">
         <v>17</v>
@@ -3310,7 +3310,7 @@
     </row>
     <row r="90" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B90" s="15">
         <v>17</v>
@@ -3330,7 +3330,7 @@
     </row>
     <row r="91" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B91" s="15">
         <v>17</v>
@@ -3350,7 +3350,7 @@
     </row>
     <row r="92" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B92" s="15">
         <v>17</v>
@@ -3370,7 +3370,7 @@
     </row>
     <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B93" s="15">
         <v>17</v>
@@ -3390,7 +3390,7 @@
     </row>
     <row r="94" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B94" s="15">
         <v>17</v>
@@ -3410,7 +3410,7 @@
     </row>
     <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B95" s="15">
         <v>17</v>
@@ -3430,7 +3430,7 @@
     </row>
     <row r="96" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B96" s="15">
         <v>17</v>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B97" s="15">
         <v>17</v>
@@ -3470,7 +3470,7 @@
     </row>
     <row r="98" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B98" s="15">
         <v>17</v>
@@ -3490,7 +3490,7 @@
     </row>
     <row r="99" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B99" s="15">
         <v>17</v>
@@ -3510,7 +3510,7 @@
     </row>
     <row r="100" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B100" s="15">
         <v>17</v>
@@ -3530,7 +3530,7 @@
     </row>
     <row r="101" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B101" s="15">
         <v>17</v>
@@ -3550,7 +3550,7 @@
     </row>
     <row r="102" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B102" s="15">
         <v>17</v>
@@ -3570,7 +3570,7 @@
     </row>
     <row r="103" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B103" s="15">
         <v>17</v>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="104" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B104" s="15">
         <v>17</v>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="105" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B105" s="15">
         <v>17</v>
@@ -3630,7 +3630,7 @@
     </row>
     <row r="106" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B106" s="15">
         <v>17</v>
@@ -3650,7 +3650,7 @@
     </row>
     <row r="107" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B107" s="15">
         <v>17</v>
@@ -3670,7 +3670,7 @@
     </row>
     <row r="108" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B108" s="15">
         <v>17</v>
@@ -3690,7 +3690,7 @@
     </row>
     <row r="109" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B109" s="15">
         <v>17</v>
@@ -3710,7 +3710,7 @@
     </row>
     <row r="110" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B110" s="15">
         <v>17</v>
@@ -3730,7 +3730,7 @@
     </row>
     <row r="111" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B111" s="15">
         <v>17</v>
@@ -3750,7 +3750,7 @@
     </row>
     <row r="112" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B112" s="15">
         <v>17</v>
@@ -3770,7 +3770,7 @@
     </row>
     <row r="113" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B113" s="15">
         <v>17</v>
@@ -3790,7 +3790,7 @@
     </row>
     <row r="114" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B114" s="15">
         <v>17</v>
@@ -3810,7 +3810,7 @@
     </row>
     <row r="115" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B115" s="15">
         <v>17</v>
@@ -3830,7 +3830,7 @@
     </row>
     <row r="116" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B116" s="15">
         <v>17</v>
@@ -3850,7 +3850,7 @@
     </row>
     <row r="117" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B117" s="15">
         <v>17</v>
@@ -3870,7 +3870,7 @@
     </row>
     <row r="118" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B118" s="15">
         <v>17</v>
@@ -3890,7 +3890,7 @@
     </row>
     <row r="119" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B119" s="15">
         <v>17</v>
@@ -3910,7 +3910,7 @@
     </row>
     <row r="120" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B120" s="15">
         <v>17</v>
@@ -3930,7 +3930,7 @@
     </row>
     <row r="121" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B121" s="15">
         <v>17</v>
@@ -3950,7 +3950,7 @@
     </row>
     <row r="122" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B122" s="15">
         <v>17</v>
@@ -3970,7 +3970,7 @@
     </row>
     <row r="123" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B123" s="15">
         <v>17</v>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="124" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B124" s="15">
         <v>17</v>
@@ -4010,7 +4010,7 @@
     </row>
     <row r="125" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B125" s="15">
         <v>17</v>
@@ -4030,7 +4030,7 @@
     </row>
     <row r="126" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B126" s="15">
         <v>17</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="127" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B127" s="15">
         <v>17</v>
@@ -4070,7 +4070,7 @@
     </row>
     <row r="128" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B128" s="15">
         <v>17</v>
@@ -4090,7 +4090,7 @@
     </row>
     <row r="129" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B129" s="15">
         <v>17</v>
@@ -4110,7 +4110,7 @@
     </row>
     <row r="130" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B130" s="15">
         <v>17</v>
@@ -4130,7 +4130,7 @@
     </row>
     <row r="131" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B131" s="15">
         <v>17</v>
@@ -4150,7 +4150,7 @@
     </row>
     <row r="132" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B132" s="15">
         <v>17</v>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="133" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B133" s="15">
         <v>17</v>
@@ -4190,7 +4190,7 @@
     </row>
     <row r="134" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B134" s="15">
         <v>17</v>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="135" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B135" s="15">
         <v>17</v>
@@ -4230,7 +4230,7 @@
     </row>
     <row r="136" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B136" s="15">
         <v>17</v>
@@ -4250,7 +4250,7 @@
     </row>
     <row r="137" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B137" s="15">
         <v>17</v>
@@ -4270,7 +4270,7 @@
     </row>
     <row r="138" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B138" s="15">
         <v>17</v>
@@ -4290,7 +4290,7 @@
     </row>
     <row r="139" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B139" s="15">
         <v>17</v>
@@ -4310,13 +4310,13 @@
     </row>
     <row r="140" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B140" s="15">
         <v>17</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D140" s="15"/>
       <c r="E140" s="21"/>
@@ -4330,13 +4330,13 @@
     </row>
     <row r="141" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B141" s="15">
         <v>17</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D141" s="15"/>
       <c r="E141" s="21"/>
@@ -4350,13 +4350,13 @@
     </row>
     <row r="142" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B142" s="15">
         <v>17</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D142" s="15"/>
       <c r="E142" s="21"/>
@@ -4370,13 +4370,13 @@
     </row>
     <row r="143" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B143" s="15">
         <v>17</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D143" s="15"/>
       <c r="E143" s="21"/>
@@ -4390,13 +4390,13 @@
     </row>
     <row r="144" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B144" s="15">
         <v>17</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D144" s="15"/>
       <c r="E144" s="21"/>
@@ -4410,13 +4410,13 @@
     </row>
     <row r="145" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B145" s="15">
         <v>17</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D145" s="15"/>
       <c r="E145" s="21"/>
@@ -4430,13 +4430,13 @@
     </row>
     <row r="146" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B146" s="15">
         <v>17</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D146" s="15"/>
       <c r="E146" s="21"/>
@@ -4450,13 +4450,13 @@
     </row>
     <row r="147" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B147" s="15">
         <v>17</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D147" s="15"/>
       <c r="E147" s="21"/>
@@ -4470,13 +4470,13 @@
     </row>
     <row r="148" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B148" s="15">
         <v>17</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D148" s="15"/>
       <c r="E148" s="21"/>
@@ -4490,13 +4490,13 @@
     </row>
     <row r="149" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B149" s="15">
         <v>17</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D149" s="15"/>
       <c r="E149" s="21"/>
@@ -4510,13 +4510,13 @@
     </row>
     <row r="150" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B150" s="15">
         <v>17</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D150" s="15"/>
       <c r="E150" s="21"/>
@@ -4530,13 +4530,13 @@
     </row>
     <row r="151" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B151" s="15">
         <v>17</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D151" s="15"/>
       <c r="E151" s="21"/>
@@ -4550,13 +4550,13 @@
     </row>
     <row r="152" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B152" s="15">
         <v>17</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D152" s="15"/>
       <c r="E152" s="21"/>
@@ -4570,13 +4570,13 @@
     </row>
     <row r="153" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B153" s="15">
         <v>17</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D153" s="15"/>
       <c r="E153" s="21"/>
@@ -4590,13 +4590,13 @@
     </row>
     <row r="154" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B154" s="15">
         <v>17</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D154" s="15"/>
       <c r="E154" s="21"/>
@@ -4610,13 +4610,13 @@
     </row>
     <row r="155" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B155" s="15">
         <v>17</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D155" s="15"/>
       <c r="E155" s="21"/>
@@ -4630,13 +4630,13 @@
     </row>
     <row r="156" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B156" s="15">
         <v>17</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D156" s="15"/>
       <c r="E156" s="21"/>
@@ -4650,13 +4650,13 @@
     </row>
     <row r="157" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B157" s="15">
         <v>17</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D157" s="15"/>
       <c r="E157" s="21"/>
@@ -4670,13 +4670,13 @@
     </row>
     <row r="158" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B158" s="15">
         <v>17</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D158" s="15"/>
       <c r="E158" s="21"/>
@@ -4690,13 +4690,13 @@
     </row>
     <row r="159" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B159" s="15">
         <v>17</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D159" s="15"/>
       <c r="E159" s="21"/>
@@ -4710,13 +4710,13 @@
     </row>
     <row r="160" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B160" s="15">
         <v>17</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D160" s="15"/>
       <c r="E160" s="21"/>
@@ -4730,13 +4730,13 @@
     </row>
     <row r="161" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B161" s="15">
         <v>17</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D161" s="15"/>
       <c r="E161" s="21"/>
@@ -4750,13 +4750,13 @@
     </row>
     <row r="162" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B162" s="15">
         <v>17</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D162" s="15"/>
       <c r="E162" s="21"/>
@@ -4770,13 +4770,13 @@
     </row>
     <row r="163" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="14" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B163" s="15">
         <v>17</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D163" s="15"/>
       <c r="E163" s="21"/>
@@ -4790,7 +4790,7 @@
     </row>
     <row r="164" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B164" s="15">
         <v>17</v>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="165" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B165" s="15">
         <v>17</v>
@@ -4830,7 +4830,7 @@
     </row>
     <row r="166" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="14" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B166" s="15">
         <v>17</v>
@@ -4850,7 +4850,7 @@
     </row>
     <row r="167" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B167" s="15">
         <v>17</v>
@@ -4870,7 +4870,7 @@
     </row>
     <row r="168" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B168" s="15">
         <v>17</v>
@@ -4890,7 +4890,7 @@
     </row>
     <row r="169" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B169" s="15">
         <v>17</v>
@@ -4910,7 +4910,7 @@
     </row>
     <row r="170" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B170" s="15">
         <v>17</v>
@@ -4930,7 +4930,7 @@
     </row>
     <row r="171" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B171" s="15">
         <v>17</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="172" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B172" s="15">
         <v>17</v>
@@ -4974,7 +4974,7 @@
     </row>
     <row r="173" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="14" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B173" s="15">
         <v>17</v>
@@ -4996,7 +4996,7 @@
     </row>
     <row r="174" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B174" s="15">
         <v>17</v>
@@ -5018,7 +5018,7 @@
     </row>
     <row r="175" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B175" s="15">
         <v>17</v>
@@ -5040,7 +5040,7 @@
     </row>
     <row r="176" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B176" s="15">
         <v>17</v>
@@ -5062,7 +5062,7 @@
     </row>
     <row r="177" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B177" s="15">
         <v>17</v>
@@ -5084,7 +5084,7 @@
     </row>
     <row r="178" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B178" s="15">
         <v>17</v>
@@ -5106,7 +5106,7 @@
     </row>
     <row r="179" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B179" s="15">
         <v>17</v>
@@ -5128,7 +5128,7 @@
     </row>
     <row r="180" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="14" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B180" s="15">
         <v>17</v>
@@ -5150,7 +5150,7 @@
     </row>
     <row r="181" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="14" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B181" s="15">
         <v>17</v>
@@ -5172,7 +5172,7 @@
     </row>
     <row r="182" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="14" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B182" s="15">
         <v>17</v>
@@ -5194,7 +5194,7 @@
     </row>
     <row r="183" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B183" s="15">
         <v>17</v>
@@ -5216,7 +5216,7 @@
     </row>
     <row r="184" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="14" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B184" s="15">
         <v>17</v>
@@ -5238,7 +5238,7 @@
     </row>
     <row r="185" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="14" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B185" s="15">
         <v>17</v>
@@ -5258,7 +5258,7 @@
     </row>
     <row r="186" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B186" s="15">
         <v>17</v>
@@ -5278,7 +5278,7 @@
     </row>
     <row r="187" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B187" s="15">
         <v>17</v>
@@ -5298,7 +5298,7 @@
     </row>
     <row r="188" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B188" s="15">
         <v>17</v>
@@ -5320,7 +5320,7 @@
     </row>
     <row r="189" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B189" s="15">
         <v>17</v>
@@ -5342,7 +5342,7 @@
     </row>
     <row r="190" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B190" s="15">
         <v>17</v>
@@ -5364,7 +5364,7 @@
     </row>
     <row r="191" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="14" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B191" s="15">
         <v>17</v>
@@ -5374,7 +5374,7 @@
       <c r="E191" s="15"/>
       <c r="F191" s="14"/>
       <c r="G191" s="24" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H191" s="25">
         <v>1</v>
@@ -5382,7 +5382,7 @@
     </row>
     <row r="192" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="14" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B192" s="15">
         <v>17</v>
@@ -5392,7 +5392,7 @@
       <c r="E192" s="15"/>
       <c r="F192" s="14"/>
       <c r="G192" s="24" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H192" s="25">
         <v>0.99039999999999995</v>
@@ -5400,7 +5400,7 @@
     </row>
     <row r="193" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="14" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B193" s="15">
         <v>17</v>
@@ -5410,7 +5410,7 @@
       <c r="E193" s="15"/>
       <c r="F193" s="14"/>
       <c r="G193" s="24" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H193" s="25">
         <v>0.97119999999999995</v>
@@ -5418,7 +5418,7 @@
     </row>
     <row r="194" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="14" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B194" s="15">
         <v>17</v>
@@ -5428,7 +5428,7 @@
       <c r="E194" s="15"/>
       <c r="F194" s="14"/>
       <c r="G194" s="24" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H194" s="25">
         <v>0.95830000000000004</v>
@@ -5436,7 +5436,7 @@
     </row>
     <row r="195" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="14" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B195" s="15">
         <v>17</v>
@@ -5446,7 +5446,7 @@
       <c r="E195" s="15"/>
       <c r="F195" s="14"/>
       <c r="G195" s="24" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H195" s="25">
         <v>0.88</v>
@@ -5454,7 +5454,7 @@
     </row>
     <row r="196" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="14" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B196" s="15">
         <v>17</v>
@@ -5464,7 +5464,7 @@
       <c r="E196" s="15"/>
       <c r="F196" s="14"/>
       <c r="G196" s="24" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H196" s="25">
         <v>0.74</v>
@@ -5472,7 +5472,7 @@
     </row>
     <row r="197" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A197" s="14" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B197" s="15">
         <v>17</v>
@@ -5482,7 +5482,7 @@
       <c r="E197" s="15"/>
       <c r="F197" s="14"/>
       <c r="G197" s="24" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H197" s="25">
         <v>0.5</v>
@@ -5490,7 +5490,7 @@
     </row>
     <row r="198" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A198" s="14" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B198" s="15">
         <v>17</v>
@@ -5500,7 +5500,7 @@
       <c r="E198" s="15"/>
       <c r="F198" s="14"/>
       <c r="G198" s="24" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H198" s="25">
         <v>0.4</v>
@@ -5508,7 +5508,7 @@
     </row>
     <row r="199" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" s="14" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B199" s="15">
         <v>17</v>
@@ -5518,7 +5518,7 @@
       <c r="E199" s="15"/>
       <c r="F199" s="14"/>
       <c r="G199" s="24" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H199" s="25">
         <v>0.3</v>
@@ -5526,7 +5526,7 @@
     </row>
     <row r="200" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A200" s="14" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B200" s="15">
         <v>17</v>
@@ -5536,7 +5536,7 @@
       <c r="E200" s="15"/>
       <c r="F200" s="14"/>
       <c r="G200" s="24" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H200" s="25">
         <v>0.2</v>
@@ -5544,7 +5544,7 @@
     </row>
     <row r="201" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A201" s="14" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B201" s="15">
         <v>17</v>
@@ -5554,7 +5554,7 @@
       <c r="E201" s="15"/>
       <c r="F201" s="14"/>
       <c r="G201" s="24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H201" s="25">
         <v>0.18</v>
@@ -5562,7 +5562,7 @@
     </row>
     <row r="202" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A202" s="14" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B202" s="15">
         <v>17</v>
@@ -5572,7 +5572,7 @@
       <c r="E202" s="15"/>
       <c r="F202" s="14"/>
       <c r="G202" s="24" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H202" s="25">
         <v>0.16669999999999999</v>

</xml_diff>